<commit_message>
Just2Trade statement: trades import
</commit_message>
<xml_diff>
--- a/tests/test_data/j2t.xlsx
+++ b/tests/test_data/j2t.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="125">
   <si>
     <t xml:space="preserve">Отчет по счету клиента за период с 03.03.2021 по 10.03.2021</t>
   </si>
@@ -416,6 +416,9 @@
   </si>
   <si>
     <t xml:space="preserve">19715</t>
+  </si>
+  <si>
+    <t xml:space="preserve">000000</t>
   </si>
 </sst>
 </file>
@@ -740,7 +743,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="90">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -817,296 +820,284 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="3" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="11" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1136,17 +1127,17 @@
   </sheetPr>
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E175" activeCellId="0" sqref="E175"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K92" activeCellId="0" sqref="K92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.14"/>
@@ -1445,32 +1436,32 @@
       <c r="I19" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="L19" s="20" t="n">
+      <c r="L19" s="19" t="n">
         <v>50</v>
       </c>
-      <c r="M19" s="21" t="n">
+      <c r="M19" s="20" t="n">
         <v>40.68</v>
       </c>
-      <c r="N19" s="22" t="n">
+      <c r="N19" s="21" t="n">
         <v>2034</v>
       </c>
-      <c r="O19" s="22" t="n">
+      <c r="O19" s="21" t="n">
         <v>0.01</v>
       </c>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22" t="n">
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21" t="n">
         <v>2033.26</v>
       </c>
-      <c r="R19" s="21" t="n">
+      <c r="R19" s="20" t="n">
         <v>0.013558</v>
       </c>
-      <c r="S19" s="23" t="n">
+      <c r="S19" s="22" t="n">
         <v>27.57</v>
       </c>
     </row>
@@ -1499,32 +1490,32 @@
       <c r="I20" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="L20" s="20" t="n">
+      <c r="L20" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="M20" s="21" t="n">
+      <c r="M20" s="20" t="n">
         <v>364.97</v>
       </c>
-      <c r="N20" s="22" t="n">
+      <c r="N20" s="21" t="n">
         <v>364.97</v>
       </c>
-      <c r="O20" s="22" t="n">
+      <c r="O20" s="21" t="n">
         <v>1.52</v>
       </c>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22" t="n">
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21" t="n">
         <v>-366.49</v>
       </c>
-      <c r="R20" s="21" t="n">
+      <c r="R20" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="S20" s="23" t="n">
+      <c r="S20" s="22" t="n">
         <v>-366.49</v>
       </c>
     </row>
@@ -1553,60 +1544,60 @@
       <c r="I21" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="L21" s="20" t="n">
+      <c r="L21" s="19" t="n">
         <v>16</v>
       </c>
-      <c r="M21" s="21" t="n">
+      <c r="M21" s="20" t="n">
         <v>65.88</v>
       </c>
-      <c r="N21" s="22" t="n">
+      <c r="N21" s="21" t="n">
         <v>1054.08</v>
       </c>
-      <c r="O21" s="22" t="n">
+      <c r="O21" s="21" t="n">
         <v>3.8</v>
       </c>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22" t="n">
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21" t="n">
         <v>1050.91</v>
       </c>
-      <c r="R21" s="21" t="n">
+      <c r="R21" s="20" t="n">
         <v>1.20402</v>
       </c>
-      <c r="S21" s="23" t="n">
+      <c r="S21" s="22" t="n">
         <v>1265.33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="33" t="n">
+      <c r="C22" s="24"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="31" t="n">
         <v>40.48</v>
       </c>
-      <c r="P22" s="33" t="n">
+      <c r="P22" s="31" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" s="32"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="33" t="n">
+      <c r="Q22" s="30"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="31" t="n">
         <v>-659.8</v>
       </c>
     </row>
@@ -1726,22 +1717,22 @@
       <c r="V27" s="10"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="38"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="39"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="37"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="37"/>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
@@ -1914,7 +1905,7 @@
       <c r="W32" s="13" t="n">
         <v>22</v>
       </c>
-      <c r="X32" s="41" t="n">
+      <c r="X32" s="39" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1928,13 +1919,13 @@
       <c r="D33" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="42" t="s">
+      <c r="E33" s="18" t="s">
         <v>68</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="42" t="s">
+      <c r="G33" s="18" t="s">
         <v>69</v>
       </c>
       <c r="H33" s="16" t="s">
@@ -1949,33 +1940,33 @@
       <c r="K33" s="18"/>
       <c r="L33" s="18"/>
       <c r="M33" s="16"/>
-      <c r="N33" s="19" t="s">
+      <c r="N33" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O33" s="19" t="s">
+      <c r="O33" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="P33" s="22" t="n">
+      <c r="P33" s="21" t="n">
         <v>0.4</v>
       </c>
-      <c r="Q33" s="43" t="n">
+      <c r="Q33" s="40" t="n">
         <v>1714</v>
       </c>
-      <c r="R33" s="22" t="n">
+      <c r="R33" s="21" t="n">
         <v>685.6</v>
       </c>
-      <c r="S33" s="22" t="n">
+      <c r="S33" s="21" t="n">
         <v>2.4</v>
       </c>
-      <c r="T33" s="22"/>
-      <c r="U33" s="22"/>
-      <c r="V33" s="22" t="n">
+      <c r="T33" s="21"/>
+      <c r="U33" s="21"/>
+      <c r="V33" s="21" t="n">
         <v>683.2</v>
       </c>
-      <c r="W33" s="21" t="n">
+      <c r="W33" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="X33" s="23" t="n">
+      <c r="X33" s="22" t="n">
         <v>683.2</v>
       </c>
     </row>
@@ -1989,13 +1980,13 @@
       <c r="D34" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="18" t="s">
         <v>68</v>
       </c>
       <c r="F34" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="42" t="s">
+      <c r="G34" s="18" t="s">
         <v>69</v>
       </c>
       <c r="H34" s="16" t="s">
@@ -2010,53 +2001,53 @@
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
       <c r="M34" s="16"/>
-      <c r="N34" s="19" t="s">
+      <c r="N34" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="O34" s="19" t="s">
+      <c r="O34" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="P34" s="22" t="n">
+      <c r="P34" s="21" t="n">
         <v>0.01</v>
       </c>
-      <c r="Q34" s="43" t="n">
+      <c r="Q34" s="40" t="n">
         <v>54614.73</v>
       </c>
-      <c r="R34" s="22" t="n">
+      <c r="R34" s="21" t="n">
         <v>546.15</v>
       </c>
-      <c r="S34" s="22" t="n">
+      <c r="S34" s="21" t="n">
         <v>1.91</v>
       </c>
-      <c r="T34" s="22"/>
-      <c r="U34" s="22"/>
-      <c r="V34" s="22" t="n">
+      <c r="T34" s="21"/>
+      <c r="U34" s="21"/>
+      <c r="V34" s="21" t="n">
         <v>544.24</v>
       </c>
-      <c r="W34" s="21" t="n">
+      <c r="W34" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="X34" s="23" t="n">
+      <c r="X34" s="22" t="n">
         <v>544.24</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="34"/>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="34"/>
-      <c r="O35" s="39"/>
-      <c r="P35" s="34"/>
-      <c r="Q35" s="39"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="37"/>
+      <c r="P35" s="32"/>
+      <c r="Q35" s="37"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
@@ -2112,691 +2103,691 @@
       <c r="Q37" s="12"/>
     </row>
     <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="44" t="n">
+      <c r="B38" s="41" t="n">
         <v>44258</v>
       </c>
-      <c r="C38" s="45"/>
-      <c r="D38" s="46" t="s">
+      <c r="C38" s="42"/>
+      <c r="D38" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E38" s="47" t="n">
+      <c r="E38" s="44" t="n">
         <v>0.52</v>
       </c>
-      <c r="F38" s="47"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="49" t="s">
+      <c r="F38" s="44"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="50" t="s">
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="N38" s="50"/>
-      <c r="O38" s="50"/>
-      <c r="P38" s="50"/>
-      <c r="Q38" s="50"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="47"/>
+      <c r="P38" s="47"/>
+      <c r="Q38" s="47"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="44" t="n">
+      <c r="B39" s="41" t="n">
         <v>44258</v>
       </c>
-      <c r="C39" s="45"/>
-      <c r="D39" s="46" t="s">
+      <c r="C39" s="42"/>
+      <c r="D39" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E39" s="47" t="n">
+      <c r="E39" s="44" t="n">
         <v>3.44</v>
       </c>
-      <c r="F39" s="47"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="49" t="s">
+      <c r="F39" s="44"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="J39" s="49"/>
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="50" t="s">
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="N39" s="50"/>
-      <c r="O39" s="50"/>
-      <c r="P39" s="50"/>
-      <c r="Q39" s="50"/>
+      <c r="N39" s="47"/>
+      <c r="O39" s="47"/>
+      <c r="P39" s="47"/>
+      <c r="Q39" s="47"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="44" t="n">
+      <c r="B40" s="41" t="n">
         <v>44258</v>
       </c>
-      <c r="C40" s="45"/>
-      <c r="D40" s="46" t="s">
+      <c r="C40" s="42"/>
+      <c r="D40" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E40" s="47" t="n">
+      <c r="E40" s="44" t="n">
         <v>2.13</v>
       </c>
-      <c r="F40" s="47"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="49" t="s">
+      <c r="F40" s="44"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J40" s="49"/>
-      <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="50" t="s">
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N40" s="50"/>
-      <c r="O40" s="50"/>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="50"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="47"/>
+      <c r="P40" s="47"/>
+      <c r="Q40" s="47"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="44" t="n">
+      <c r="B41" s="41" t="n">
         <v>44258</v>
       </c>
-      <c r="C41" s="45"/>
-      <c r="D41" s="46" t="s">
+      <c r="C41" s="42"/>
+      <c r="D41" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E41" s="47" t="n">
+      <c r="E41" s="44" t="n">
         <v>6.37</v>
       </c>
-      <c r="F41" s="47"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="49" t="s">
+      <c r="F41" s="44"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J41" s="49"/>
-      <c r="K41" s="49"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="50" t="s">
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N41" s="50"/>
-      <c r="O41" s="50"/>
-      <c r="P41" s="50"/>
-      <c r="Q41" s="50"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="47"/>
+      <c r="P41" s="47"/>
+      <c r="Q41" s="47"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="44" t="n">
+      <c r="B42" s="41" t="n">
         <v>44259</v>
       </c>
-      <c r="C42" s="45"/>
-      <c r="D42" s="46" t="s">
+      <c r="C42" s="42"/>
+      <c r="D42" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="47" t="n">
+      <c r="E42" s="44" t="n">
         <v>81.3</v>
       </c>
-      <c r="F42" s="47"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="49" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J42" s="49"/>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="50" t="s">
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50"/>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="50"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="47"/>
+      <c r="Q42" s="47"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="44" t="n">
+      <c r="B43" s="41" t="n">
         <v>44259</v>
       </c>
-      <c r="C43" s="45"/>
-      <c r="D43" s="46" t="s">
+      <c r="C43" s="42"/>
+      <c r="D43" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="47" t="n">
+      <c r="E43" s="44" t="n">
         <v>84.24</v>
       </c>
-      <c r="F43" s="47"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="49" t="s">
+      <c r="F43" s="44"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J43" s="49"/>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="50" t="s">
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N43" s="50"/>
-      <c r="O43" s="50"/>
-      <c r="P43" s="50"/>
-      <c r="Q43" s="50"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="47"/>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="47"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="44" t="n">
+      <c r="B44" s="41" t="n">
         <v>44259</v>
       </c>
-      <c r="C44" s="45"/>
-      <c r="D44" s="46" t="s">
+      <c r="C44" s="42"/>
+      <c r="D44" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="47" t="n">
+      <c r="E44" s="44" t="n">
         <v>23.25</v>
       </c>
-      <c r="F44" s="47"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="49" t="s">
+      <c r="F44" s="44"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J44" s="49"/>
-      <c r="K44" s="49"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="50" t="s">
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N44" s="50"/>
-      <c r="O44" s="50"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="50"/>
+      <c r="N44" s="47"/>
+      <c r="O44" s="47"/>
+      <c r="P44" s="47"/>
+      <c r="Q44" s="47"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="44" t="n">
+      <c r="B45" s="41" t="n">
         <v>44260</v>
       </c>
-      <c r="C45" s="45"/>
-      <c r="D45" s="46" t="s">
+      <c r="C45" s="42"/>
+      <c r="D45" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="47" t="n">
+      <c r="E45" s="44" t="n">
         <v>18.34</v>
       </c>
-      <c r="F45" s="47"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="49" t="s">
+      <c r="F45" s="44"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J45" s="49"/>
-      <c r="K45" s="49"/>
-      <c r="L45" s="49"/>
-      <c r="M45" s="50" t="s">
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
+      <c r="M45" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N45" s="50"/>
-      <c r="O45" s="50"/>
-      <c r="P45" s="50"/>
-      <c r="Q45" s="50"/>
+      <c r="N45" s="47"/>
+      <c r="O45" s="47"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="47"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="44" t="n">
+      <c r="B46" s="41" t="n">
         <v>44260</v>
       </c>
-      <c r="C46" s="45"/>
-      <c r="D46" s="46" t="s">
+      <c r="C46" s="42"/>
+      <c r="D46" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E46" s="47" t="n">
+      <c r="E46" s="44" t="n">
         <v>59.69</v>
       </c>
-      <c r="F46" s="47"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="49" t="s">
+      <c r="F46" s="44"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J46" s="49"/>
-      <c r="K46" s="49"/>
-      <c r="L46" s="49"/>
-      <c r="M46" s="50" t="s">
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N46" s="50"/>
-      <c r="O46" s="50"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="50"/>
+      <c r="N46" s="47"/>
+      <c r="O46" s="47"/>
+      <c r="P46" s="47"/>
+      <c r="Q46" s="47"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="44" t="n">
+      <c r="B47" s="41" t="n">
         <v>44262</v>
       </c>
-      <c r="C47" s="45"/>
-      <c r="D47" s="46" t="s">
+      <c r="C47" s="42"/>
+      <c r="D47" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E47" s="47" t="n">
+      <c r="E47" s="44" t="n">
         <v>293.42</v>
       </c>
-      <c r="F47" s="47"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="49" t="s">
+      <c r="F47" s="44"/>
+      <c r="G47" s="45"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J47" s="49"/>
-      <c r="K47" s="49"/>
-      <c r="L47" s="49"/>
-      <c r="M47" s="50" t="s">
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N47" s="50"/>
-      <c r="O47" s="50"/>
-      <c r="P47" s="50"/>
-      <c r="Q47" s="50"/>
+      <c r="N47" s="47"/>
+      <c r="O47" s="47"/>
+      <c r="P47" s="47"/>
+      <c r="Q47" s="47"/>
     </row>
     <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="44" t="n">
+      <c r="B48" s="41" t="n">
         <v>44263</v>
       </c>
-      <c r="C48" s="45"/>
-      <c r="D48" s="46" t="s">
+      <c r="C48" s="42"/>
+      <c r="D48" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E48" s="47" t="n">
+      <c r="E48" s="44" t="n">
         <v>0.42</v>
       </c>
-      <c r="F48" s="47"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="49" t="s">
+      <c r="F48" s="44"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="J48" s="49"/>
-      <c r="K48" s="49"/>
-      <c r="L48" s="49"/>
-      <c r="M48" s="50" t="s">
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
+      <c r="M48" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="N48" s="50"/>
-      <c r="O48" s="50"/>
-      <c r="P48" s="50"/>
-      <c r="Q48" s="50"/>
+      <c r="N48" s="47"/>
+      <c r="O48" s="47"/>
+      <c r="P48" s="47"/>
+      <c r="Q48" s="47"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="44" t="n">
+      <c r="B49" s="41" t="n">
         <v>44263</v>
       </c>
-      <c r="C49" s="45"/>
-      <c r="D49" s="46" t="s">
+      <c r="C49" s="42"/>
+      <c r="D49" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="47" t="n">
+      <c r="E49" s="44" t="n">
         <v>2.78</v>
       </c>
-      <c r="F49" s="47"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="49" t="s">
+      <c r="F49" s="44"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="J49" s="49"/>
-      <c r="K49" s="49"/>
-      <c r="L49" s="49"/>
-      <c r="M49" s="50" t="s">
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
+      <c r="M49" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="N49" s="50"/>
-      <c r="O49" s="50"/>
-      <c r="P49" s="50"/>
-      <c r="Q49" s="50"/>
+      <c r="N49" s="47"/>
+      <c r="O49" s="47"/>
+      <c r="P49" s="47"/>
+      <c r="Q49" s="47"/>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="44" t="n">
+      <c r="B50" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C50" s="45"/>
-      <c r="D50" s="46" t="s">
+      <c r="C50" s="42"/>
+      <c r="D50" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E50" s="47" t="n">
+      <c r="E50" s="44" t="n">
         <v>1.46</v>
       </c>
-      <c r="F50" s="47"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="49" t="s">
+      <c r="F50" s="44"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="50" t="s">
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="N50" s="50"/>
-      <c r="O50" s="50"/>
-      <c r="P50" s="50"/>
-      <c r="Q50" s="50"/>
+      <c r="N50" s="47"/>
+      <c r="O50" s="47"/>
+      <c r="P50" s="47"/>
+      <c r="Q50" s="47"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="44" t="n">
+      <c r="B51" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C51" s="45"/>
-      <c r="D51" s="46" t="s">
+      <c r="C51" s="42"/>
+      <c r="D51" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E51" s="47" t="n">
+      <c r="E51" s="44" t="n">
         <v>9.75</v>
       </c>
-      <c r="F51" s="47"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="49" t="s">
+      <c r="F51" s="44"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="J51" s="49"/>
-      <c r="K51" s="49"/>
-      <c r="L51" s="49"/>
-      <c r="M51" s="50" t="s">
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
+      <c r="M51" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="N51" s="50"/>
-      <c r="O51" s="50"/>
-      <c r="P51" s="50"/>
-      <c r="Q51" s="50"/>
+      <c r="N51" s="47"/>
+      <c r="O51" s="47"/>
+      <c r="P51" s="47"/>
+      <c r="Q51" s="47"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="44" t="n">
+      <c r="B52" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C52" s="45"/>
-      <c r="D52" s="46" t="s">
+      <c r="C52" s="42"/>
+      <c r="D52" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E52" s="47" t="n">
+      <c r="E52" s="44" t="n">
         <v>185.48</v>
       </c>
-      <c r="F52" s="47"/>
-      <c r="G52" s="48"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="49" t="s">
+      <c r="F52" s="44"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J52" s="49"/>
-      <c r="K52" s="49"/>
-      <c r="L52" s="49"/>
-      <c r="M52" s="50" t="s">
+      <c r="J52" s="46"/>
+      <c r="K52" s="46"/>
+      <c r="L52" s="46"/>
+      <c r="M52" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N52" s="50"/>
-      <c r="O52" s="50"/>
-      <c r="P52" s="50"/>
-      <c r="Q52" s="50"/>
+      <c r="N52" s="47"/>
+      <c r="O52" s="47"/>
+      <c r="P52" s="47"/>
+      <c r="Q52" s="47"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="44" t="n">
+      <c r="B53" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C53" s="45"/>
-      <c r="D53" s="46" t="s">
+      <c r="C53" s="42"/>
+      <c r="D53" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E53" s="47" t="n">
+      <c r="E53" s="44" t="n">
         <v>9.22</v>
       </c>
-      <c r="F53" s="47"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="49" t="s">
+      <c r="F53" s="44"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J53" s="49"/>
-      <c r="K53" s="49"/>
-      <c r="L53" s="49"/>
-      <c r="M53" s="50" t="s">
+      <c r="J53" s="46"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="46"/>
+      <c r="M53" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N53" s="50"/>
-      <c r="O53" s="50"/>
-      <c r="P53" s="50"/>
-      <c r="Q53" s="50"/>
+      <c r="N53" s="47"/>
+      <c r="O53" s="47"/>
+      <c r="P53" s="47"/>
+      <c r="Q53" s="47"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="44" t="n">
+      <c r="B54" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C54" s="45"/>
-      <c r="D54" s="46" t="s">
+      <c r="C54" s="42"/>
+      <c r="D54" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E54" s="47" t="n">
+      <c r="E54" s="44" t="n">
         <v>1.82</v>
       </c>
-      <c r="F54" s="47"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="48"/>
-      <c r="I54" s="49" t="s">
+      <c r="F54" s="44"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J54" s="49"/>
-      <c r="K54" s="49"/>
-      <c r="L54" s="49"/>
-      <c r="M54" s="50" t="s">
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="M54" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N54" s="50"/>
-      <c r="O54" s="50"/>
-      <c r="P54" s="50"/>
-      <c r="Q54" s="50"/>
+      <c r="N54" s="47"/>
+      <c r="O54" s="47"/>
+      <c r="P54" s="47"/>
+      <c r="Q54" s="47"/>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="44" t="n">
+      <c r="B55" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C55" s="45"/>
-      <c r="D55" s="46" t="s">
+      <c r="C55" s="42"/>
+      <c r="D55" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E55" s="47" t="n">
+      <c r="E55" s="44" t="n">
         <v>0.61</v>
       </c>
-      <c r="F55" s="47"/>
-      <c r="G55" s="48"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="49" t="s">
+      <c r="F55" s="44"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="J55" s="49"/>
-      <c r="K55" s="49"/>
-      <c r="L55" s="49"/>
-      <c r="M55" s="50" t="s">
+      <c r="J55" s="46"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="46"/>
+      <c r="M55" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="N55" s="50"/>
-      <c r="O55" s="50"/>
-      <c r="P55" s="50"/>
-      <c r="Q55" s="50"/>
+      <c r="N55" s="47"/>
+      <c r="O55" s="47"/>
+      <c r="P55" s="47"/>
+      <c r="Q55" s="47"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="44" t="n">
+      <c r="B56" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C56" s="45"/>
-      <c r="D56" s="46" t="s">
+      <c r="C56" s="42"/>
+      <c r="D56" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="E56" s="47" t="n">
+      <c r="E56" s="44" t="n">
         <v>4.04</v>
       </c>
-      <c r="F56" s="47"/>
-      <c r="G56" s="48"/>
-      <c r="H56" s="48"/>
-      <c r="I56" s="49" t="s">
+      <c r="F56" s="44"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="J56" s="49"/>
-      <c r="K56" s="49"/>
-      <c r="L56" s="49"/>
-      <c r="M56" s="50" t="s">
+      <c r="J56" s="46"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="46"/>
+      <c r="M56" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="N56" s="50"/>
-      <c r="O56" s="50"/>
-      <c r="P56" s="50"/>
-      <c r="Q56" s="50"/>
+      <c r="N56" s="47"/>
+      <c r="O56" s="47"/>
+      <c r="P56" s="47"/>
+      <c r="Q56" s="47"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="44" t="n">
+      <c r="B57" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C57" s="45"/>
-      <c r="D57" s="46" t="s">
+      <c r="C57" s="42"/>
+      <c r="D57" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E57" s="47" t="n">
+      <c r="E57" s="44" t="n">
         <v>21.13</v>
       </c>
-      <c r="F57" s="47"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="49" t="s">
+      <c r="F57" s="44"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J57" s="49"/>
-      <c r="K57" s="49"/>
-      <c r="L57" s="49"/>
-      <c r="M57" s="50" t="s">
+      <c r="J57" s="46"/>
+      <c r="K57" s="46"/>
+      <c r="L57" s="46"/>
+      <c r="M57" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N57" s="50"/>
-      <c r="O57" s="50"/>
-      <c r="P57" s="50"/>
-      <c r="Q57" s="50"/>
+      <c r="N57" s="47"/>
+      <c r="O57" s="47"/>
+      <c r="P57" s="47"/>
+      <c r="Q57" s="47"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="44" t="n">
+      <c r="B58" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C58" s="45"/>
-      <c r="D58" s="46" t="s">
+      <c r="C58" s="42"/>
+      <c r="D58" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E58" s="47" t="n">
+      <c r="E58" s="44" t="n">
         <v>3.5</v>
       </c>
-      <c r="F58" s="47"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="48"/>
-      <c r="I58" s="49" t="s">
+      <c r="F58" s="44"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J58" s="49"/>
-      <c r="K58" s="49"/>
-      <c r="L58" s="49"/>
-      <c r="M58" s="50" t="s">
+      <c r="J58" s="46"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="46"/>
+      <c r="M58" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N58" s="50"/>
-      <c r="O58" s="50"/>
-      <c r="P58" s="50"/>
-      <c r="Q58" s="50"/>
+      <c r="N58" s="47"/>
+      <c r="O58" s="47"/>
+      <c r="P58" s="47"/>
+      <c r="Q58" s="47"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="44" t="n">
+      <c r="B59" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C59" s="45"/>
-      <c r="D59" s="46" t="s">
+      <c r="C59" s="42"/>
+      <c r="D59" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E59" s="47" t="n">
+      <c r="E59" s="44" t="n">
         <v>1.35</v>
       </c>
-      <c r="F59" s="47"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="49" t="s">
+      <c r="F59" s="44"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J59" s="49"/>
-      <c r="K59" s="49"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="50" t="s">
+      <c r="J59" s="46"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="46"/>
+      <c r="M59" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N59" s="50"/>
-      <c r="O59" s="50"/>
-      <c r="P59" s="50"/>
-      <c r="Q59" s="50"/>
+      <c r="N59" s="47"/>
+      <c r="O59" s="47"/>
+      <c r="P59" s="47"/>
+      <c r="Q59" s="47"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="51" t="s">
+      <c r="B60" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="52"/>
-      <c r="D60" s="53" t="s">
+      <c r="C60" s="49"/>
+      <c r="D60" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="E60" s="54" t="n">
+      <c r="E60" s="51" t="n">
         <v>678.9</v>
       </c>
-      <c r="F60" s="54"/>
-      <c r="G60" s="55"/>
-      <c r="H60" s="55"/>
-      <c r="I60" s="56"/>
-      <c r="J60" s="56"/>
-      <c r="K60" s="56"/>
-      <c r="L60" s="56"/>
-      <c r="M60" s="56"/>
-      <c r="N60" s="56"/>
-      <c r="O60" s="56"/>
-      <c r="P60" s="56"/>
-      <c r="Q60" s="57"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="52"/>
+      <c r="H60" s="52"/>
+      <c r="I60" s="53"/>
+      <c r="J60" s="53"/>
+      <c r="K60" s="53"/>
+      <c r="L60" s="53"/>
+      <c r="M60" s="53"/>
+      <c r="N60" s="53"/>
+      <c r="O60" s="53"/>
+      <c r="P60" s="53"/>
+      <c r="Q60" s="54"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="58" t="s">
+      <c r="B61" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="59"/>
-      <c r="D61" s="60" t="s">
+      <c r="C61" s="56"/>
+      <c r="D61" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="E61" s="61" t="n">
+      <c r="E61" s="58" t="n">
         <v>135.36</v>
       </c>
-      <c r="F61" s="61"/>
-      <c r="G61" s="62"/>
-      <c r="H61" s="62"/>
-      <c r="I61" s="63"/>
-      <c r="J61" s="63"/>
-      <c r="K61" s="63"/>
-      <c r="L61" s="63"/>
-      <c r="M61" s="63"/>
-      <c r="N61" s="63"/>
-      <c r="O61" s="63"/>
-      <c r="P61" s="63"/>
-      <c r="Q61" s="64"/>
+      <c r="F61" s="58"/>
+      <c r="G61" s="59"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="60"/>
+      <c r="J61" s="60"/>
+      <c r="K61" s="60"/>
+      <c r="L61" s="60"/>
+      <c r="M61" s="60"/>
+      <c r="N61" s="60"/>
+      <c r="O61" s="60"/>
+      <c r="P61" s="60"/>
+      <c r="Q61" s="61"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="65"/>
-      <c r="C62" s="66"/>
-      <c r="D62" s="66"/>
-      <c r="E62" s="66"/>
-      <c r="F62" s="67"/>
-      <c r="G62" s="67"/>
-      <c r="H62" s="67"/>
-      <c r="I62" s="67"/>
-      <c r="J62" s="67"/>
-      <c r="K62" s="68"/>
-      <c r="L62" s="69"/>
-      <c r="M62" s="69"/>
-      <c r="N62" s="70"/>
-      <c r="O62" s="67"/>
-      <c r="P62" s="67"/>
-      <c r="Q62" s="67"/>
-      <c r="R62" s="71"/>
-      <c r="S62" s="71"/>
-      <c r="T62" s="71"/>
-      <c r="U62" s="71"/>
-      <c r="V62" s="71"/>
+      <c r="B62" s="62"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="63"/>
+      <c r="F62" s="64"/>
+      <c r="G62" s="64"/>
+      <c r="H62" s="64"/>
+      <c r="I62" s="64"/>
+      <c r="J62" s="64"/>
+      <c r="K62" s="65"/>
+      <c r="L62" s="66"/>
+      <c r="M62" s="66"/>
+      <c r="N62" s="67"/>
+      <c r="O62" s="64"/>
+      <c r="P62" s="64"/>
+      <c r="Q62" s="64"/>
+      <c r="R62" s="68"/>
+      <c r="S62" s="68"/>
+      <c r="T62" s="68"/>
+      <c r="U62" s="68"/>
+      <c r="V62" s="68"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="3" t="s">
@@ -2848,242 +2839,242 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="72" t="n">
+      <c r="B65" s="69" t="n">
         <v>44258</v>
       </c>
-      <c r="C65" s="73" t="n">
+      <c r="C65" s="70" t="n">
         <v>44256.6360300926</v>
       </c>
-      <c r="D65" s="73"/>
+      <c r="D65" s="70"/>
       <c r="E65" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F65" s="74" t="s">
+      <c r="F65" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G65" s="74"/>
-      <c r="H65" s="74"/>
-      <c r="I65" s="22" t="n">
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="21" t="n">
         <v>-1</v>
       </c>
-      <c r="J65" s="22"/>
-      <c r="K65" s="22"/>
-      <c r="L65" s="22"/>
-      <c r="M65" s="75"/>
+      <c r="J65" s="21"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="21"/>
+      <c r="M65" s="72"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="72" t="n">
+      <c r="B66" s="69" t="n">
         <v>44258</v>
       </c>
-      <c r="C66" s="73" t="n">
+      <c r="C66" s="70" t="n">
         <v>44256.6360300926</v>
       </c>
-      <c r="D66" s="73"/>
+      <c r="D66" s="70"/>
       <c r="E66" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F66" s="74"/>
-      <c r="G66" s="74"/>
-      <c r="H66" s="74"/>
-      <c r="I66" s="22"/>
-      <c r="J66" s="22"/>
-      <c r="K66" s="22" t="n">
+      <c r="F66" s="71"/>
+      <c r="G66" s="71"/>
+      <c r="H66" s="71"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21" t="n">
         <v>390.39</v>
       </c>
-      <c r="L66" s="22"/>
-      <c r="M66" s="75" t="s">
+      <c r="L66" s="21"/>
+      <c r="M66" s="72" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="72" t="n">
+      <c r="B67" s="69" t="n">
         <v>44258</v>
       </c>
-      <c r="C67" s="73" t="n">
+      <c r="C67" s="70" t="n">
         <v>44256.7498148148</v>
       </c>
-      <c r="D67" s="73"/>
+      <c r="D67" s="70"/>
       <c r="E67" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F67" s="74" t="s">
+      <c r="F67" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G67" s="74"/>
-      <c r="H67" s="74"/>
-      <c r="I67" s="22" t="n">
+      <c r="G67" s="71"/>
+      <c r="H67" s="71"/>
+      <c r="I67" s="21" t="n">
         <v>-1</v>
       </c>
-      <c r="J67" s="22"/>
-      <c r="K67" s="22"/>
-      <c r="L67" s="22"/>
-      <c r="M67" s="75"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="72"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="72" t="n">
+      <c r="B68" s="69" t="n">
         <v>44258</v>
       </c>
-      <c r="C68" s="73" t="n">
+      <c r="C68" s="70" t="n">
         <v>44256.7498148148</v>
       </c>
-      <c r="D68" s="73"/>
+      <c r="D68" s="70"/>
       <c r="E68" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F68" s="74"/>
-      <c r="G68" s="74"/>
-      <c r="H68" s="74"/>
-      <c r="I68" s="22"/>
-      <c r="J68" s="22"/>
-      <c r="K68" s="22" t="n">
+      <c r="F68" s="71"/>
+      <c r="G68" s="71"/>
+      <c r="H68" s="71"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="21" t="n">
         <v>403.39</v>
       </c>
-      <c r="L68" s="22"/>
-      <c r="M68" s="75" t="s">
+      <c r="L68" s="21"/>
+      <c r="M68" s="72" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="72" t="n">
+      <c r="B69" s="69" t="n">
         <v>44259</v>
       </c>
-      <c r="C69" s="73" t="n">
+      <c r="C69" s="70" t="n">
         <v>44257.8319444444</v>
       </c>
-      <c r="D69" s="73"/>
+      <c r="D69" s="70"/>
       <c r="E69" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F69" s="74" t="s">
+      <c r="F69" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G69" s="74"/>
-      <c r="H69" s="74"/>
-      <c r="I69" s="22" t="n">
+      <c r="G69" s="71"/>
+      <c r="H69" s="71"/>
+      <c r="I69" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="J69" s="22"/>
-      <c r="K69" s="22"/>
-      <c r="L69" s="22"/>
-      <c r="M69" s="75"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="72"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="72" t="n">
+      <c r="B70" s="69" t="n">
         <v>44259</v>
       </c>
-      <c r="C70" s="73" t="n">
+      <c r="C70" s="70" t="n">
         <v>44257.8319444444</v>
       </c>
-      <c r="D70" s="73"/>
+      <c r="D70" s="70"/>
       <c r="E70" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
-      <c r="I70" s="22"/>
-      <c r="J70" s="22"/>
-      <c r="K70" s="22" t="n">
+      <c r="F70" s="71"/>
+      <c r="G70" s="71"/>
+      <c r="H70" s="71"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="21" t="n">
         <v>-382.44</v>
       </c>
-      <c r="L70" s="22"/>
-      <c r="M70" s="75" t="s">
+      <c r="L70" s="21"/>
+      <c r="M70" s="72" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="72" t="n">
+      <c r="B71" s="69" t="n">
         <v>44259</v>
       </c>
-      <c r="C71" s="73" t="n">
+      <c r="C71" s="70" t="n">
         <v>44257.3449884259</v>
       </c>
-      <c r="D71" s="73"/>
+      <c r="D71" s="70"/>
       <c r="E71" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F71" s="74"/>
-      <c r="G71" s="74"/>
-      <c r="H71" s="74"/>
-      <c r="I71" s="22"/>
-      <c r="J71" s="22"/>
-      <c r="K71" s="22" t="n">
+      <c r="F71" s="71"/>
+      <c r="G71" s="71"/>
+      <c r="H71" s="71"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="21" t="n">
         <v>-13257</v>
       </c>
-      <c r="L71" s="22"/>
-      <c r="M71" s="75" t="s">
+      <c r="L71" s="21"/>
+      <c r="M71" s="72" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="72" t="n">
+      <c r="B72" s="69" t="n">
         <v>44260</v>
       </c>
-      <c r="C72" s="73" t="n">
+      <c r="C72" s="70" t="n">
         <v>44258.4781365741</v>
       </c>
-      <c r="D72" s="73"/>
+      <c r="D72" s="70"/>
       <c r="E72" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="F72" s="74"/>
-      <c r="G72" s="74"/>
-      <c r="H72" s="74"/>
-      <c r="I72" s="22"/>
-      <c r="J72" s="22"/>
-      <c r="K72" s="22" t="n">
+      <c r="F72" s="71"/>
+      <c r="G72" s="71"/>
+      <c r="H72" s="71"/>
+      <c r="I72" s="21"/>
+      <c r="J72" s="21"/>
+      <c r="K72" s="21" t="n">
         <v>14149</v>
       </c>
-      <c r="L72" s="22"/>
-      <c r="M72" s="75" t="s">
+      <c r="L72" s="21"/>
+      <c r="M72" s="72" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="72" t="n">
+      <c r="B73" s="69" t="n">
         <v>44260</v>
       </c>
-      <c r="C73" s="73" t="n">
+      <c r="C73" s="70" t="n">
         <v>44258.4974421296</v>
       </c>
-      <c r="D73" s="73"/>
+      <c r="D73" s="70"/>
       <c r="E73" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F73" s="74" t="s">
+      <c r="F73" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="G73" s="74"/>
-      <c r="H73" s="74"/>
-      <c r="I73" s="22" t="n">
+      <c r="G73" s="71"/>
+      <c r="H73" s="71"/>
+      <c r="I73" s="21" t="n">
         <v>-50</v>
       </c>
-      <c r="J73" s="22"/>
-      <c r="K73" s="22"/>
-      <c r="L73" s="22"/>
-      <c r="M73" s="75"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
+      <c r="M73" s="72"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="72" t="n">
+      <c r="B74" s="69" t="n">
         <v>44260</v>
       </c>
-      <c r="C74" s="73" t="n">
+      <c r="C74" s="70" t="n">
         <v>44258.4974421296</v>
       </c>
-      <c r="D74" s="73"/>
+      <c r="D74" s="70"/>
       <c r="E74" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F74" s="74"/>
-      <c r="G74" s="74"/>
-      <c r="H74" s="74"/>
-      <c r="I74" s="22"/>
-      <c r="J74" s="22"/>
-      <c r="K74" s="22" t="n">
+      <c r="F74" s="71"/>
+      <c r="G74" s="71"/>
+      <c r="H74" s="71"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21" t="n">
         <v>2034</v>
       </c>
-      <c r="L74" s="22"/>
-      <c r="M74" s="75" t="s">
+      <c r="L74" s="21"/>
+      <c r="M74" s="72" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3112,14 +3103,14 @@
       <c r="R76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="76" t="s">
+      <c r="B77" s="73" t="s">
         <v>75</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D77" s="12"/>
-      <c r="E77" s="77" t="s">
+      <c r="E77" s="74" t="s">
         <v>10</v>
       </c>
       <c r="F77" s="12" t="s">
@@ -3136,100 +3127,100 @@
       <c r="O77" s="12"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="72" t="n">
+      <c r="B78" s="69" t="n">
         <v>44257.9967824074</v>
       </c>
-      <c r="C78" s="22" t="n">
+      <c r="C78" s="21" t="n">
         <v>0.26</v>
       </c>
-      <c r="D78" s="22"/>
-      <c r="E78" s="78" t="s">
+      <c r="D78" s="21"/>
+      <c r="E78" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="F78" s="50" t="s">
+      <c r="F78" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="G78" s="50"/>
-      <c r="H78" s="50"/>
-      <c r="I78" s="50"/>
-      <c r="J78" s="50"/>
-      <c r="K78" s="50"/>
-      <c r="L78" s="50"/>
-      <c r="M78" s="50"/>
-      <c r="N78" s="50"/>
-      <c r="O78" s="50"/>
+      <c r="G78" s="47"/>
+      <c r="H78" s="47"/>
+      <c r="I78" s="47"/>
+      <c r="J78" s="47"/>
+      <c r="K78" s="47"/>
+      <c r="L78" s="47"/>
+      <c r="M78" s="47"/>
+      <c r="N78" s="47"/>
+      <c r="O78" s="47"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="72" t="n">
+      <c r="B79" s="69" t="n">
         <v>44257.9999884259</v>
       </c>
-      <c r="C79" s="22" t="n">
+      <c r="C79" s="21" t="n">
         <v>0.5</v>
       </c>
-      <c r="D79" s="22"/>
-      <c r="E79" s="78" t="s">
+      <c r="D79" s="21"/>
+      <c r="E79" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="F79" s="50" t="s">
+      <c r="F79" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="G79" s="50"/>
-      <c r="H79" s="50"/>
-      <c r="I79" s="50"/>
-      <c r="J79" s="50"/>
-      <c r="K79" s="50"/>
-      <c r="L79" s="50"/>
-      <c r="M79" s="50"/>
-      <c r="N79" s="50"/>
-      <c r="O79" s="50"/>
+      <c r="G79" s="47"/>
+      <c r="H79" s="47"/>
+      <c r="I79" s="47"/>
+      <c r="J79" s="47"/>
+      <c r="K79" s="47"/>
+      <c r="L79" s="47"/>
+      <c r="M79" s="47"/>
+      <c r="N79" s="47"/>
+      <c r="O79" s="47"/>
     </row>
     <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="72" t="n">
+      <c r="B80" s="69" t="n">
         <v>44258</v>
       </c>
-      <c r="C80" s="22" t="n">
+      <c r="C80" s="21" t="n">
         <v>2.92</v>
       </c>
-      <c r="D80" s="22"/>
-      <c r="E80" s="78" t="s">
+      <c r="D80" s="21"/>
+      <c r="E80" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="F80" s="50" t="s">
+      <c r="F80" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="G80" s="50"/>
-      <c r="H80" s="50"/>
-      <c r="I80" s="50"/>
-      <c r="J80" s="50"/>
-      <c r="K80" s="50"/>
-      <c r="L80" s="50"/>
-      <c r="M80" s="50"/>
-      <c r="N80" s="50"/>
-      <c r="O80" s="50"/>
+      <c r="G80" s="47"/>
+      <c r="H80" s="47"/>
+      <c r="I80" s="47"/>
+      <c r="J80" s="47"/>
+      <c r="K80" s="47"/>
+      <c r="L80" s="47"/>
+      <c r="M80" s="47"/>
+      <c r="N80" s="47"/>
+      <c r="O80" s="47"/>
     </row>
     <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="79" t="s">
+      <c r="B81" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="33" t="n">
+      <c r="C81" s="31" t="n">
         <v>69.62</v>
       </c>
-      <c r="D81" s="33"/>
-      <c r="E81" s="80"/>
-      <c r="F81" s="81"/>
-      <c r="G81" s="81"/>
-      <c r="H81" s="81"/>
-      <c r="I81" s="81"/>
-      <c r="J81" s="81"/>
-      <c r="K81" s="81"/>
-      <c r="L81" s="81"/>
-      <c r="M81" s="81"/>
-      <c r="N81" s="81"/>
-      <c r="O81" s="82"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="77"/>
+      <c r="F81" s="78"/>
+      <c r="G81" s="78"/>
+      <c r="H81" s="78"/>
+      <c r="I81" s="78"/>
+      <c r="J81" s="78"/>
+      <c r="K81" s="78"/>
+      <c r="L81" s="78"/>
+      <c r="M81" s="78"/>
+      <c r="N81" s="78"/>
+      <c r="O81" s="79"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="2"/>
-      <c r="H82" s="83"/>
+      <c r="H82" s="80"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="3" t="s">
@@ -3264,13 +3255,13 @@
         <v>29</v>
       </c>
       <c r="H84" s="12"/>
-      <c r="I84" s="84" t="s">
+      <c r="I84" s="81" t="s">
         <v>30</v>
       </c>
       <c r="J84" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K84" s="85" t="s">
+      <c r="K84" s="82" t="s">
         <v>32</v>
       </c>
       <c r="L84" s="12" t="s">
@@ -3283,134 +3274,149 @@
       <c r="O84" s="12"/>
     </row>
     <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="86" t="s">
+      <c r="B85" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="86"/>
-      <c r="D85" s="86"/>
-      <c r="E85" s="86"/>
-      <c r="F85" s="86"/>
-      <c r="G85" s="87" t="s">
+      <c r="C85" s="83"/>
+      <c r="D85" s="83"/>
+      <c r="E85" s="83"/>
+      <c r="F85" s="83"/>
+      <c r="G85" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="H85" s="87"/>
-      <c r="I85" s="88" t="s">
+      <c r="H85" s="18"/>
+      <c r="I85" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="J85" s="19" t="s">
+      <c r="J85" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="K85" s="19" t="s">
+      <c r="K85" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L85" s="89" t="s">
+      <c r="L85" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="M85" s="89"/>
-      <c r="N85" s="90" t="n">
+      <c r="M85" s="15"/>
+      <c r="N85" s="85" t="n">
         <v>6</v>
       </c>
-      <c r="O85" s="90"/>
+      <c r="O85" s="85"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="86" t="s">
+      <c r="B86" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="C86" s="86"/>
-      <c r="D86" s="86"/>
-      <c r="E86" s="86"/>
-      <c r="F86" s="86"/>
-      <c r="G86" s="87" t="s">
+      <c r="C86" s="83"/>
+      <c r="D86" s="83"/>
+      <c r="E86" s="83"/>
+      <c r="F86" s="83"/>
+      <c r="G86" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="H86" s="87"/>
-      <c r="I86" s="88"/>
-      <c r="J86" s="19" t="s">
+      <c r="H86" s="18"/>
+      <c r="I86" s="84"/>
+      <c r="J86" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="K86" s="19" t="s">
+      <c r="K86" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="L86" s="89" t="s">
+      <c r="L86" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="M86" s="89"/>
-      <c r="N86" s="90" t="n">
+      <c r="M86" s="15"/>
+      <c r="N86" s="85" t="n">
         <v>400</v>
       </c>
-      <c r="O86" s="90"/>
+      <c r="O86" s="85"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="86" t="s">
+      <c r="B87" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C87" s="86"/>
-      <c r="D87" s="86"/>
-      <c r="E87" s="86"/>
-      <c r="F87" s="86"/>
-      <c r="G87" s="87" t="s">
+      <c r="C87" s="83"/>
+      <c r="D87" s="83"/>
+      <c r="E87" s="83"/>
+      <c r="F87" s="83"/>
+      <c r="G87" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H87" s="87"/>
-      <c r="I87" s="88"/>
-      <c r="J87" s="19" t="s">
+      <c r="H87" s="18"/>
+      <c r="I87" s="84"/>
+      <c r="J87" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K87" s="19" t="s">
+      <c r="K87" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="L87" s="89" t="s">
+      <c r="L87" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="M87" s="89"/>
-      <c r="N87" s="90" t="n">
+      <c r="M87" s="15"/>
+      <c r="N87" s="85" t="n">
         <v>200</v>
       </c>
-      <c r="O87" s="90"/>
+      <c r="O87" s="85"/>
     </row>
     <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="86" t="s">
+      <c r="B88" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="C88" s="86"/>
-      <c r="D88" s="86"/>
-      <c r="E88" s="86"/>
-      <c r="F88" s="86"/>
-      <c r="G88" s="87" t="s">
+      <c r="C88" s="83"/>
+      <c r="D88" s="83"/>
+      <c r="E88" s="83"/>
+      <c r="F88" s="83"/>
+      <c r="G88" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="H88" s="87"/>
-      <c r="I88" s="88" t="s">
+      <c r="H88" s="18"/>
+      <c r="I88" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="J88" s="19" t="s">
+      <c r="J88" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="K88" s="19" t="s">
+      <c r="K88" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L88" s="89" t="s">
+      <c r="L88" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="M88" s="89"/>
-      <c r="N88" s="90" t="n">
+      <c r="M88" s="15"/>
+      <c r="N88" s="85" t="n">
         <v>9</v>
       </c>
-      <c r="O88" s="90"/>
-    </row>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="67"/>
-      <c r="C89" s="67"/>
-      <c r="D89" s="69"/>
-      <c r="E89" s="69"/>
-      <c r="F89" s="91"/>
-      <c r="G89" s="91"/>
-      <c r="H89" s="91"/>
-      <c r="I89" s="70"/>
-      <c r="J89" s="70"/>
+      <c r="O88" s="85"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B89" s="86" t="s">
+        <v>73</v>
+      </c>
+      <c r="C89" s="86"/>
+      <c r="D89" s="86"/>
+      <c r="E89" s="86"/>
+      <c r="F89" s="86"/>
+      <c r="G89" s="87"/>
+      <c r="H89" s="87"/>
+      <c r="I89" s="84"/>
+      <c r="J89" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="K89" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L89" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="M89" s="88"/>
+      <c r="N89" s="85" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="O89" s="85"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="92"/>
+      <c r="B90" s="89"/>
     </row>
     <row r="1048262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3728,7 +3734,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="212">
+  <mergeCells count="216">
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
@@ -3941,6 +3947,10 @@
     <mergeCell ref="G88:H88"/>
     <mergeCell ref="L88:M88"/>
     <mergeCell ref="N88:O88"/>
+    <mergeCell ref="B89:F89"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="L89:M89"/>
+    <mergeCell ref="N89:O89"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3963,7 +3973,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3986,7 +3996,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Just2Trade statement: Price calculation was corrected for trades import
</commit_message>
<xml_diff>
--- a/tests/test_data/j2t.xlsx
+++ b/tests/test_data/j2t.xlsx
@@ -14,12 +14,12 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="__DB10__" vbProcedure="false">page1!#ref!</definedName>
-    <definedName function="false" hidden="false" name="__DB11__" vbProcedure="false">Page1!$B$65:$M$65</definedName>
-    <definedName function="false" hidden="false" name="__DB12__" vbProcedure="false">Page1!$B$78:$E$78</definedName>
+    <definedName function="false" hidden="false" name="__DB11__" vbProcedure="false">Page1!$B$66:$M$66</definedName>
+    <definedName function="false" hidden="false" name="__DB12__" vbProcedure="false">Page1!$B$79:$E$79</definedName>
     <definedName function="false" hidden="false" name="__DB13__" vbProcedure="false">page1!#ref!</definedName>
-    <definedName function="false" hidden="false" name="__DB14__" vbProcedure="false">Page1!$B$85:$O$85</definedName>
+    <definedName function="false" hidden="false" name="__DB14__" vbProcedure="false">Page1!$B$86:$O$86</definedName>
     <definedName function="false" hidden="false" name="__DB15__" vbProcedure="false">page1!#ref!</definedName>
-    <definedName function="false" hidden="false" name="__DB17__" vbProcedure="false">Page1!$B$33:$X$33</definedName>
+    <definedName function="false" hidden="false" name="__DB17__" vbProcedure="false">Page1!$B$34:$X$34</definedName>
     <definedName function="false" hidden="false" name="__DB18__" vbProcedure="false">page1!#ref!</definedName>
     <definedName function="false" hidden="false" name="__DB19__" vbProcedure="false">page1!#ref!</definedName>
     <definedName function="false" hidden="false" name="__DB1__" vbProcedure="false">Page1!$F$3:$G$4</definedName>
@@ -31,7 +31,7 @@
     <definedName function="false" hidden="false" name="__DB6__" vbProcedure="false">page1!#ref!</definedName>
     <definedName function="false" hidden="false" name="__DB7__" vbProcedure="false">page1!#ref!</definedName>
     <definedName function="false" hidden="false" name="__DB8__" vbProcedure="false">page1!#ref!</definedName>
-    <definedName function="false" hidden="false" name="__DB9__" vbProcedure="false">Page1!$B$38:$H$38</definedName>
+    <definedName function="false" hidden="false" name="__DB9__" vbProcedure="false">Page1!$B$39:$H$39</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="127">
   <si>
     <t xml:space="preserve">Отчет по счету клиента за период с 03.03.2021 по 10.03.2021</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t xml:space="preserve">Купля</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.03.2021 14:36:26, GMT+01:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR265763834</t>
   </si>
   <si>
     <t xml:space="preserve">04.03.2021 10:30:41, GMT+01:00</t>
@@ -743,7 +749,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="88">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -836,6 +842,10 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1086,18 +1096,6 @@
     </xf>
     <xf numFmtId="174" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1127,17 +1125,17 @@
   </sheetPr>
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K92" activeCellId="0" sqref="K92"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T21" activeCellId="0" sqref="T21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.14"/>
@@ -1519,112 +1517,143 @@
         <v>-366.49</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="23" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E21" s="17" t="n">
-        <v>44263</v>
+        <v>44267</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="K21" s="15" t="s">
         <v>40</v>
       </c>
       <c r="L21" s="19" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="M21" s="20" t="n">
-        <v>65.88</v>
+        <v>348.89</v>
       </c>
       <c r="N21" s="21" t="n">
-        <v>1054.08</v>
+        <v>348.89</v>
       </c>
       <c r="O21" s="21" t="n">
-        <v>3.8</v>
+        <v>1.52</v>
       </c>
       <c r="P21" s="21"/>
       <c r="Q21" s="21" t="n">
+        <v>347.37</v>
+      </c>
+      <c r="R21" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="S21" s="22" t="n">
+        <v>347.37</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="17" t="n">
+        <v>44263</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="L22" s="19" t="n">
+        <v>16</v>
+      </c>
+      <c r="M22" s="20" t="n">
+        <v>65.88</v>
+      </c>
+      <c r="N22" s="21" t="n">
+        <v>1054.08</v>
+      </c>
+      <c r="O22" s="21" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21" t="n">
         <v>1050.91</v>
       </c>
-      <c r="R21" s="20" t="n">
+      <c r="R22" s="20" t="n">
         <v>1.20402</v>
       </c>
-      <c r="S21" s="22" t="n">
+      <c r="S22" s="22" t="n">
         <v>1265.33</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="31" t="n">
+    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="32" t="n">
         <v>40.48</v>
       </c>
-      <c r="P22" s="31" t="n">
+      <c r="P23" s="32" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="31" t="n">
+      <c r="Q23" s="31"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="32" t="n">
         <v>-659.8</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-    </row>
-    <row r="24" customFormat="false" ht="0.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="24.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -1647,7 +1676,7 @@
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="0.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -1670,7 +1699,7 @@
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
     </row>
-    <row r="26" customFormat="false" ht="13.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -1693,7 +1722,7 @@
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1716,287 +1745,249 @@
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="32"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="37"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="32"/>
-      <c r="O28" s="37"/>
-      <c r="P28" s="32"/>
-      <c r="Q28" s="37"/>
-    </row>
-    <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10"/>
-      <c r="B29" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="11" t="s">
+    <row r="28" customFormat="false" ht="12.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="38"/>
+    </row>
+    <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10"/>
+      <c r="B30" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="11" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G30" s="11" t="s">
+      <c r="E31" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="F31" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I30" s="11" t="s">
+      <c r="G31" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="J31" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="11" t="s">
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="P30" s="11" t="s">
+      <c r="P31" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="Q30" s="11" t="s">
+      <c r="Q31" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="R30" s="11" t="s">
+      <c r="R31" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="S30" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="T30" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="U30" s="11" t="s">
+      <c r="S31" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="T31" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="U31" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="V30" s="11" t="s">
+      <c r="V31" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="W30" s="11" t="s">
+      <c r="W31" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="X30" s="11" t="s">
+      <c r="X31" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="K31" s="11" t="s">
+    <row r="32" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K32" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L31" s="11" t="s">
+      <c r="L32" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M31" s="11" t="s">
+      <c r="M32" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N31" s="11" t="s">
+      <c r="N32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="13" t="n">
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="C32" s="13" t="n">
+      <c r="C33" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="D32" s="13" t="n">
+      <c r="D33" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="E32" s="13" t="n">
+      <c r="E33" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="F32" s="13" t="n">
+      <c r="F33" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="G32" s="13" t="n">
+      <c r="G33" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="H32" s="13" t="n">
+      <c r="H33" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="I32" s="13" t="n">
+      <c r="I33" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="J32" s="13" t="n">
+      <c r="J33" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="K32" s="13" t="n">
+      <c r="K33" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="L32" s="13" t="n">
+      <c r="L33" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="M32" s="13" t="n">
+      <c r="M33" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="N32" s="13" t="n">
+      <c r="N33" s="13" t="n">
         <v>13</v>
       </c>
-      <c r="O32" s="13" t="n">
+      <c r="O33" s="13" t="n">
         <v>14</v>
       </c>
-      <c r="P32" s="13" t="n">
+      <c r="P33" s="13" t="n">
         <v>15</v>
       </c>
-      <c r="Q32" s="13" t="n">
+      <c r="Q33" s="13" t="n">
         <v>16</v>
       </c>
-      <c r="R32" s="13" t="n">
+      <c r="R33" s="13" t="n">
         <v>17</v>
       </c>
-      <c r="S32" s="13" t="n">
+      <c r="S33" s="13" t="n">
         <v>18</v>
       </c>
-      <c r="T32" s="13" t="n">
+      <c r="T33" s="13" t="n">
         <v>19</v>
       </c>
-      <c r="U32" s="13" t="n">
+      <c r="U33" s="13" t="n">
         <v>20</v>
       </c>
-      <c r="V32" s="13" t="n">
+      <c r="V33" s="13" t="n">
         <v>21</v>
       </c>
-      <c r="W32" s="13" t="n">
+      <c r="W33" s="13" t="n">
         <v>22</v>
       </c>
-      <c r="X32" s="39" t="n">
+      <c r="X33" s="40" t="n">
         <v>23</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="14" t="n">
-        <v>44262.9788773148</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="H33" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="I33" s="17" t="n">
-        <v>44263</v>
-      </c>
-      <c r="J33" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="O33" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="P33" s="21" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="Q33" s="40" t="n">
-        <v>1714</v>
-      </c>
-      <c r="R33" s="21" t="n">
-        <v>685.6</v>
-      </c>
-      <c r="S33" s="21" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="T33" s="21"/>
-      <c r="U33" s="21"/>
-      <c r="V33" s="21" t="n">
-        <v>683.2</v>
-      </c>
-      <c r="W33" s="20" t="n">
-        <v>1</v>
-      </c>
-      <c r="X33" s="22" t="n">
-        <v>683.2</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="14" t="n">
-        <v>44264.574212963</v>
+        <v>44262.9788773148</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F34" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H34" s="16" t="s">
         <v>35</v>
       </c>
       <c r="I34" s="17" t="n">
-        <v>44264</v>
+        <v>44263</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K34" s="18"/>
       <c r="L34" s="18"/>
@@ -2005,1420 +1996,1480 @@
         <v>11</v>
       </c>
       <c r="O34" s="15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="P34" s="21" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="Q34" s="40" t="n">
-        <v>54614.73</v>
+        <v>0.4</v>
+      </c>
+      <c r="Q34" s="41" t="n">
+        <v>1714</v>
       </c>
       <c r="R34" s="21" t="n">
-        <v>546.15</v>
+        <v>685.6</v>
       </c>
       <c r="S34" s="21" t="n">
-        <v>1.91</v>
+        <v>2.4</v>
       </c>
       <c r="T34" s="21"/>
       <c r="U34" s="21"/>
       <c r="V34" s="21" t="n">
-        <v>544.24</v>
+        <v>683.2</v>
       </c>
       <c r="W34" s="20" t="n">
         <v>1</v>
       </c>
       <c r="X34" s="22" t="n">
+        <v>683.2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="14" t="n">
+        <v>44264.574212963</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" s="17" t="n">
+        <v>44264</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O35" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="P35" s="21" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Q35" s="41" t="n">
+        <v>54614.73</v>
+      </c>
+      <c r="R35" s="21" t="n">
+        <v>546.15</v>
+      </c>
+      <c r="S35" s="21" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="T35" s="21"/>
+      <c r="U35" s="21"/>
+      <c r="V35" s="21" t="n">
         <v>544.24</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="32"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="37"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="37"/>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="37"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
-      <c r="R36" s="4"/>
-    </row>
-    <row r="37" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="12" t="s">
+      <c r="W35" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="X35" s="22" t="n">
+        <v>544.24</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="33"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="38"/>
+      <c r="P36" s="33"/>
+      <c r="Q36" s="38"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+    </row>
+    <row r="38" customFormat="false" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="C38" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12" t="s">
+      <c r="F38" s="12"/>
+      <c r="G38" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-    </row>
-    <row r="38" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="41" t="n">
+      <c r="H38" s="12"/>
+      <c r="I38" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+    </row>
+    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="42" t="n">
         <v>44258</v>
       </c>
-      <c r="C38" s="42"/>
-      <c r="D38" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="44" t="n">
+      <c r="C39" s="43"/>
+      <c r="D39" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="45" t="n">
         <v>0.52</v>
       </c>
-      <c r="F38" s="44"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="J38" s="46"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="47" t="s">
+      <c r="F39" s="45"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="47"/>
+      <c r="M39" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="N39" s="48"/>
+      <c r="O39" s="48"/>
+      <c r="P39" s="48"/>
+      <c r="Q39" s="48"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="42" t="n">
+        <v>44258</v>
+      </c>
+      <c r="C40" s="43"/>
+      <c r="D40" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="45" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="F40" s="45"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="J40" s="47"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="47"/>
+      <c r="M40" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="N40" s="48"/>
+      <c r="O40" s="48"/>
+      <c r="P40" s="48"/>
+      <c r="Q40" s="48"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B41" s="42" t="n">
+        <v>44258</v>
+      </c>
+      <c r="C41" s="43"/>
+      <c r="D41" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E41" s="45" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="F41" s="45"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J41" s="47"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N41" s="48"/>
+      <c r="O41" s="48"/>
+      <c r="P41" s="48"/>
+      <c r="Q41" s="48"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="42" t="n">
+        <v>44258</v>
+      </c>
+      <c r="C42" s="43"/>
+      <c r="D42" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E42" s="45" t="n">
+        <v>6.37</v>
+      </c>
+      <c r="F42" s="45"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N42" s="48"/>
+      <c r="O42" s="48"/>
+      <c r="P42" s="48"/>
+      <c r="Q42" s="48"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="42" t="n">
+        <v>44259</v>
+      </c>
+      <c r="C43" s="43"/>
+      <c r="D43" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="N38" s="47"/>
-      <c r="O38" s="47"/>
-      <c r="P38" s="47"/>
-      <c r="Q38" s="47"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="41" t="n">
+      <c r="E43" s="45" t="n">
+        <v>81.3</v>
+      </c>
+      <c r="F43" s="45"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="N43" s="48"/>
+      <c r="O43" s="48"/>
+      <c r="P43" s="48"/>
+      <c r="Q43" s="48"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="42" t="n">
+        <v>44259</v>
+      </c>
+      <c r="C44" s="43"/>
+      <c r="D44" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="45" t="n">
+        <v>84.24</v>
+      </c>
+      <c r="F44" s="45"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J44" s="47"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="47"/>
+      <c r="M44" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N44" s="48"/>
+      <c r="O44" s="48"/>
+      <c r="P44" s="48"/>
+      <c r="Q44" s="48"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="42" t="n">
+        <v>44259</v>
+      </c>
+      <c r="C45" s="43"/>
+      <c r="D45" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="45" t="n">
+        <v>23.25</v>
+      </c>
+      <c r="F45" s="45"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N45" s="48"/>
+      <c r="O45" s="48"/>
+      <c r="P45" s="48"/>
+      <c r="Q45" s="48"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="42" t="n">
+        <v>44260</v>
+      </c>
+      <c r="C46" s="43"/>
+      <c r="D46" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" s="45" t="n">
+        <v>18.34</v>
+      </c>
+      <c r="F46" s="45"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J46" s="47"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="47"/>
+      <c r="M46" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N46" s="48"/>
+      <c r="O46" s="48"/>
+      <c r="P46" s="48"/>
+      <c r="Q46" s="48"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="42" t="n">
+        <v>44260</v>
+      </c>
+      <c r="C47" s="43"/>
+      <c r="D47" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" s="45" t="n">
+        <v>59.69</v>
+      </c>
+      <c r="F47" s="45"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+      <c r="M47" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N47" s="48"/>
+      <c r="O47" s="48"/>
+      <c r="P47" s="48"/>
+      <c r="Q47" s="48"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="42" t="n">
+        <v>44262</v>
+      </c>
+      <c r="C48" s="43"/>
+      <c r="D48" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" s="45" t="n">
+        <v>293.42</v>
+      </c>
+      <c r="F48" s="45"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J48" s="47"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="N48" s="48"/>
+      <c r="O48" s="48"/>
+      <c r="P48" s="48"/>
+      <c r="Q48" s="48"/>
+    </row>
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B49" s="42" t="n">
+        <v>44263</v>
+      </c>
+      <c r="C49" s="43"/>
+      <c r="D49" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" s="45" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="F49" s="45"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="J49" s="47"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="N49" s="48"/>
+      <c r="O49" s="48"/>
+      <c r="P49" s="48"/>
+      <c r="Q49" s="48"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B50" s="42" t="n">
+        <v>44263</v>
+      </c>
+      <c r="C50" s="43"/>
+      <c r="D50" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" s="45" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="F50" s="45"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="J50" s="47"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="N50" s="48"/>
+      <c r="O50" s="48"/>
+      <c r="P50" s="48"/>
+      <c r="Q50" s="48"/>
+    </row>
+    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B51" s="42" t="n">
+        <v>44264</v>
+      </c>
+      <c r="C51" s="43"/>
+      <c r="D51" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E51" s="45" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="F51" s="45"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="J51" s="47"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="47"/>
+      <c r="M51" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="N51" s="48"/>
+      <c r="O51" s="48"/>
+      <c r="P51" s="48"/>
+      <c r="Q51" s="48"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B52" s="42" t="n">
+        <v>44264</v>
+      </c>
+      <c r="C52" s="43"/>
+      <c r="D52" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="45" t="n">
+        <v>9.75</v>
+      </c>
+      <c r="F52" s="45"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="J52" s="47"/>
+      <c r="K52" s="47"/>
+      <c r="L52" s="47"/>
+      <c r="M52" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="N52" s="48"/>
+      <c r="O52" s="48"/>
+      <c r="P52" s="48"/>
+      <c r="Q52" s="48"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="42" t="n">
+        <v>44264</v>
+      </c>
+      <c r="C53" s="43"/>
+      <c r="D53" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" s="45" t="n">
+        <v>185.48</v>
+      </c>
+      <c r="F53" s="45"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J53" s="47"/>
+      <c r="K53" s="47"/>
+      <c r="L53" s="47"/>
+      <c r="M53" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N53" s="48"/>
+      <c r="O53" s="48"/>
+      <c r="P53" s="48"/>
+      <c r="Q53" s="48"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B54" s="42" t="n">
+        <v>44264</v>
+      </c>
+      <c r="C54" s="43"/>
+      <c r="D54" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E54" s="45" t="n">
+        <v>9.22</v>
+      </c>
+      <c r="F54" s="45"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J54" s="47"/>
+      <c r="K54" s="47"/>
+      <c r="L54" s="47"/>
+      <c r="M54" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N54" s="48"/>
+      <c r="O54" s="48"/>
+      <c r="P54" s="48"/>
+      <c r="Q54" s="48"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B55" s="42" t="n">
+        <v>44264</v>
+      </c>
+      <c r="C55" s="43"/>
+      <c r="D55" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" s="45" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="F55" s="45"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J55" s="47"/>
+      <c r="K55" s="47"/>
+      <c r="L55" s="47"/>
+      <c r="M55" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N55" s="48"/>
+      <c r="O55" s="48"/>
+      <c r="P55" s="48"/>
+      <c r="Q55" s="48"/>
+    </row>
+    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B56" s="42" t="n">
+        <v>44265</v>
+      </c>
+      <c r="C56" s="43"/>
+      <c r="D56" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" s="45" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="F56" s="45"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="J56" s="47"/>
+      <c r="K56" s="47"/>
+      <c r="L56" s="47"/>
+      <c r="M56" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="N56" s="48"/>
+      <c r="O56" s="48"/>
+      <c r="P56" s="48"/>
+      <c r="Q56" s="48"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B57" s="42" t="n">
+        <v>44265</v>
+      </c>
+      <c r="C57" s="43"/>
+      <c r="D57" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" s="45" t="n">
+        <v>4.04</v>
+      </c>
+      <c r="F57" s="45"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="J57" s="47"/>
+      <c r="K57" s="47"/>
+      <c r="L57" s="47"/>
+      <c r="M57" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="N57" s="48"/>
+      <c r="O57" s="48"/>
+      <c r="P57" s="48"/>
+      <c r="Q57" s="48"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B58" s="42" t="n">
+        <v>44265</v>
+      </c>
+      <c r="C58" s="43"/>
+      <c r="D58" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E58" s="45" t="n">
+        <v>21.13</v>
+      </c>
+      <c r="F58" s="45"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J58" s="47"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="47"/>
+      <c r="M58" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N58" s="48"/>
+      <c r="O58" s="48"/>
+      <c r="P58" s="48"/>
+      <c r="Q58" s="48"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B59" s="42" t="n">
+        <v>44265</v>
+      </c>
+      <c r="C59" s="43"/>
+      <c r="D59" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" s="45" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F59" s="45"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J59" s="47"/>
+      <c r="K59" s="47"/>
+      <c r="L59" s="47"/>
+      <c r="M59" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N59" s="48"/>
+      <c r="O59" s="48"/>
+      <c r="P59" s="48"/>
+      <c r="Q59" s="48"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B60" s="42" t="n">
+        <v>44265</v>
+      </c>
+      <c r="C60" s="43"/>
+      <c r="D60" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E60" s="45" t="n">
+        <v>1.35</v>
+      </c>
+      <c r="F60" s="45"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="J60" s="47"/>
+      <c r="K60" s="47"/>
+      <c r="L60" s="47"/>
+      <c r="M60" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="N60" s="48"/>
+      <c r="O60" s="48"/>
+      <c r="P60" s="48"/>
+      <c r="Q60" s="48"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" s="50"/>
+      <c r="D61" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E61" s="52" t="n">
+        <v>678.9</v>
+      </c>
+      <c r="F61" s="52"/>
+      <c r="G61" s="53"/>
+      <c r="H61" s="53"/>
+      <c r="I61" s="54"/>
+      <c r="J61" s="54"/>
+      <c r="K61" s="54"/>
+      <c r="L61" s="54"/>
+      <c r="M61" s="54"/>
+      <c r="N61" s="54"/>
+      <c r="O61" s="54"/>
+      <c r="P61" s="54"/>
+      <c r="Q61" s="55"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="57"/>
+      <c r="D62" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="E62" s="59" t="n">
+        <v>135.36</v>
+      </c>
+      <c r="F62" s="59"/>
+      <c r="G62" s="60"/>
+      <c r="H62" s="60"/>
+      <c r="I62" s="61"/>
+      <c r="J62" s="61"/>
+      <c r="K62" s="61"/>
+      <c r="L62" s="61"/>
+      <c r="M62" s="61"/>
+      <c r="N62" s="61"/>
+      <c r="O62" s="61"/>
+      <c r="P62" s="61"/>
+      <c r="Q62" s="62"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="63"/>
+      <c r="C63" s="64"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="65"/>
+      <c r="G63" s="65"/>
+      <c r="H63" s="65"/>
+      <c r="I63" s="65"/>
+      <c r="J63" s="65"/>
+      <c r="K63" s="66"/>
+      <c r="L63" s="67"/>
+      <c r="M63" s="67"/>
+      <c r="N63" s="68"/>
+      <c r="O63" s="65"/>
+      <c r="P63" s="65"/>
+      <c r="Q63" s="65"/>
+      <c r="R63" s="69"/>
+      <c r="S63" s="69"/>
+      <c r="T63" s="69"/>
+      <c r="U63" s="69"/>
+      <c r="V63" s="69"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+    </row>
+    <row r="65" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B65" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="L65" s="12"/>
+      <c r="M65" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B66" s="70" t="n">
         <v>44258</v>
       </c>
-      <c r="C39" s="42"/>
-      <c r="D39" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="44" t="n">
-        <v>3.44</v>
-      </c>
-      <c r="F39" s="44"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="J39" s="46"/>
-      <c r="K39" s="46"/>
-      <c r="L39" s="46"/>
-      <c r="M39" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="N39" s="47"/>
-      <c r="O39" s="47"/>
-      <c r="P39" s="47"/>
-      <c r="Q39" s="47"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="41" t="n">
+      <c r="C66" s="71" t="n">
+        <v>44256.6360300926</v>
+      </c>
+      <c r="D66" s="71"/>
+      <c r="E66" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F66" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="G66" s="72"/>
+      <c r="H66" s="72"/>
+      <c r="I66" s="21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J66" s="21"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="73"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="70" t="n">
         <v>44258</v>
       </c>
-      <c r="C40" s="42"/>
-      <c r="D40" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" s="44" t="n">
-        <v>2.13</v>
-      </c>
-      <c r="F40" s="44"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J40" s="46"/>
-      <c r="K40" s="46"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N40" s="47"/>
-      <c r="O40" s="47"/>
-      <c r="P40" s="47"/>
-      <c r="Q40" s="47"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="41" t="n">
+      <c r="C67" s="71" t="n">
+        <v>44256.6360300926</v>
+      </c>
+      <c r="D67" s="71"/>
+      <c r="E67" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F67" s="72"/>
+      <c r="G67" s="72"/>
+      <c r="H67" s="72"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21" t="n">
+        <v>390.39</v>
+      </c>
+      <c r="L67" s="21"/>
+      <c r="M67" s="73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B68" s="70" t="n">
         <v>44258</v>
       </c>
-      <c r="C41" s="42"/>
-      <c r="D41" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="44" t="n">
-        <v>6.37</v>
-      </c>
-      <c r="F41" s="44"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J41" s="46"/>
-      <c r="K41" s="46"/>
-      <c r="L41" s="46"/>
-      <c r="M41" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N41" s="47"/>
-      <c r="O41" s="47"/>
-      <c r="P41" s="47"/>
-      <c r="Q41" s="47"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="41" t="n">
+      <c r="C68" s="71" t="n">
+        <v>44256.7498148148</v>
+      </c>
+      <c r="D68" s="71"/>
+      <c r="E68" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F68" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="G68" s="72"/>
+      <c r="H68" s="72"/>
+      <c r="I68" s="21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J68" s="21"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="21"/>
+      <c r="M68" s="73"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="70" t="n">
+        <v>44258</v>
+      </c>
+      <c r="C69" s="71" t="n">
+        <v>44256.7498148148</v>
+      </c>
+      <c r="D69" s="71"/>
+      <c r="E69" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F69" s="72"/>
+      <c r="G69" s="72"/>
+      <c r="H69" s="72"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21" t="n">
+        <v>403.39</v>
+      </c>
+      <c r="L69" s="21"/>
+      <c r="M69" s="73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B70" s="70" t="n">
         <v>44259</v>
       </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E42" s="44" t="n">
-        <v>81.3</v>
-      </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J42" s="46"/>
-      <c r="K42" s="46"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="N42" s="47"/>
-      <c r="O42" s="47"/>
-      <c r="P42" s="47"/>
-      <c r="Q42" s="47"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="41" t="n">
+      <c r="C70" s="71" t="n">
+        <v>44257.8319444444</v>
+      </c>
+      <c r="D70" s="71"/>
+      <c r="E70" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F70" s="72" t="s">
+        <v>43</v>
+      </c>
+      <c r="G70" s="72"/>
+      <c r="H70" s="72"/>
+      <c r="I70" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J70" s="21"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="73"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="70" t="n">
         <v>44259</v>
       </c>
-      <c r="C43" s="42"/>
-      <c r="D43" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E43" s="44" t="n">
-        <v>84.24</v>
-      </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J43" s="46"/>
-      <c r="K43" s="46"/>
-      <c r="L43" s="46"/>
-      <c r="M43" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N43" s="47"/>
-      <c r="O43" s="47"/>
-      <c r="P43" s="47"/>
-      <c r="Q43" s="47"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="41" t="n">
-        <v>44259</v>
-      </c>
-      <c r="C44" s="42"/>
-      <c r="D44" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E44" s="44" t="n">
-        <v>23.25</v>
-      </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J44" s="46"/>
-      <c r="K44" s="46"/>
-      <c r="L44" s="46"/>
-      <c r="M44" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N44" s="47"/>
-      <c r="O44" s="47"/>
-      <c r="P44" s="47"/>
-      <c r="Q44" s="47"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="41" t="n">
-        <v>44260</v>
-      </c>
-      <c r="C45" s="42"/>
-      <c r="D45" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E45" s="44" t="n">
-        <v>18.34</v>
-      </c>
-      <c r="F45" s="44"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J45" s="46"/>
-      <c r="K45" s="46"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N45" s="47"/>
-      <c r="O45" s="47"/>
-      <c r="P45" s="47"/>
-      <c r="Q45" s="47"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="41" t="n">
-        <v>44260</v>
-      </c>
-      <c r="C46" s="42"/>
-      <c r="D46" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E46" s="44" t="n">
-        <v>59.69</v>
-      </c>
-      <c r="F46" s="44"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J46" s="46"/>
-      <c r="K46" s="46"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N46" s="47"/>
-      <c r="O46" s="47"/>
-      <c r="P46" s="47"/>
-      <c r="Q46" s="47"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="41" t="n">
-        <v>44262</v>
-      </c>
-      <c r="C47" s="42"/>
-      <c r="D47" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E47" s="44" t="n">
-        <v>293.42</v>
-      </c>
-      <c r="F47" s="44"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J47" s="46"/>
-      <c r="K47" s="46"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="N47" s="47"/>
-      <c r="O47" s="47"/>
-      <c r="P47" s="47"/>
-      <c r="Q47" s="47"/>
-    </row>
-    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="41" t="n">
-        <v>44263</v>
-      </c>
-      <c r="C48" s="42"/>
-      <c r="D48" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" s="44" t="n">
-        <v>0.42</v>
-      </c>
-      <c r="F48" s="44"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="J48" s="46"/>
-      <c r="K48" s="46"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="47" t="s">
-        <v>91</v>
-      </c>
-      <c r="N48" s="47"/>
-      <c r="O48" s="47"/>
-      <c r="P48" s="47"/>
-      <c r="Q48" s="47"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="41" t="n">
-        <v>44263</v>
-      </c>
-      <c r="C49" s="42"/>
-      <c r="D49" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E49" s="44" t="n">
-        <v>2.78</v>
-      </c>
-      <c r="F49" s="44"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="J49" s="46"/>
-      <c r="K49" s="46"/>
-      <c r="L49" s="46"/>
-      <c r="M49" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="N49" s="47"/>
-      <c r="O49" s="47"/>
-      <c r="P49" s="47"/>
-      <c r="Q49" s="47"/>
-    </row>
-    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="41" t="n">
-        <v>44264</v>
-      </c>
-      <c r="C50" s="42"/>
-      <c r="D50" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50" s="44" t="n">
-        <v>1.46</v>
-      </c>
-      <c r="F50" s="44"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="J50" s="46"/>
-      <c r="K50" s="46"/>
-      <c r="L50" s="46"/>
-      <c r="M50" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="N50" s="47"/>
-      <c r="O50" s="47"/>
-      <c r="P50" s="47"/>
-      <c r="Q50" s="47"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="41" t="n">
-        <v>44264</v>
-      </c>
-      <c r="C51" s="42"/>
-      <c r="D51" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E51" s="44" t="n">
-        <v>9.75</v>
-      </c>
-      <c r="F51" s="44"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="45"/>
-      <c r="I51" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="J51" s="46"/>
-      <c r="K51" s="46"/>
-      <c r="L51" s="46"/>
-      <c r="M51" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="N51" s="47"/>
-      <c r="O51" s="47"/>
-      <c r="P51" s="47"/>
-      <c r="Q51" s="47"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="41" t="n">
-        <v>44264</v>
-      </c>
-      <c r="C52" s="42"/>
-      <c r="D52" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E52" s="44" t="n">
-        <v>185.48</v>
-      </c>
-      <c r="F52" s="44"/>
-      <c r="G52" s="45"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J52" s="46"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="46"/>
-      <c r="M52" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N52" s="47"/>
-      <c r="O52" s="47"/>
-      <c r="P52" s="47"/>
-      <c r="Q52" s="47"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="41" t="n">
-        <v>44264</v>
-      </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="44" t="n">
-        <v>9.22</v>
-      </c>
-      <c r="F53" s="44"/>
-      <c r="G53" s="45"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J53" s="46"/>
-      <c r="K53" s="46"/>
-      <c r="L53" s="46"/>
-      <c r="M53" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N53" s="47"/>
-      <c r="O53" s="47"/>
-      <c r="P53" s="47"/>
-      <c r="Q53" s="47"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="41" t="n">
-        <v>44264</v>
-      </c>
-      <c r="C54" s="42"/>
-      <c r="D54" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E54" s="44" t="n">
-        <v>1.82</v>
-      </c>
-      <c r="F54" s="44"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J54" s="46"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="46"/>
-      <c r="M54" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N54" s="47"/>
-      <c r="O54" s="47"/>
-      <c r="P54" s="47"/>
-      <c r="Q54" s="47"/>
-    </row>
-    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C55" s="42"/>
-      <c r="D55" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E55" s="44" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="F55" s="44"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="46" t="s">
-        <v>82</v>
-      </c>
-      <c r="J55" s="46"/>
-      <c r="K55" s="46"/>
-      <c r="L55" s="46"/>
-      <c r="M55" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="N55" s="47"/>
-      <c r="O55" s="47"/>
-      <c r="P55" s="47"/>
-      <c r="Q55" s="47"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C56" s="42"/>
-      <c r="D56" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="E56" s="44" t="n">
-        <v>4.04</v>
-      </c>
-      <c r="F56" s="44"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="J56" s="46"/>
-      <c r="K56" s="46"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="N56" s="47"/>
-      <c r="O56" s="47"/>
-      <c r="P56" s="47"/>
-      <c r="Q56" s="47"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C57" s="42"/>
-      <c r="D57" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E57" s="44" t="n">
-        <v>21.13</v>
-      </c>
-      <c r="F57" s="44"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J57" s="46"/>
-      <c r="K57" s="46"/>
-      <c r="L57" s="46"/>
-      <c r="M57" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N57" s="47"/>
-      <c r="O57" s="47"/>
-      <c r="P57" s="47"/>
-      <c r="Q57" s="47"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C58" s="42"/>
-      <c r="D58" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E58" s="44" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="F58" s="44"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J58" s="46"/>
-      <c r="K58" s="46"/>
-      <c r="L58" s="46"/>
-      <c r="M58" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N58" s="47"/>
-      <c r="O58" s="47"/>
-      <c r="P58" s="47"/>
-      <c r="Q58" s="47"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C59" s="42"/>
-      <c r="D59" s="43" t="s">
-        <v>81</v>
-      </c>
-      <c r="E59" s="44" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="F59" s="44"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J59" s="46"/>
-      <c r="K59" s="46"/>
-      <c r="L59" s="46"/>
-      <c r="M59" s="47" t="s">
-        <v>88</v>
-      </c>
-      <c r="N59" s="47"/>
-      <c r="O59" s="47"/>
-      <c r="P59" s="47"/>
-      <c r="Q59" s="47"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="49"/>
-      <c r="D60" s="50" t="s">
-        <v>84</v>
-      </c>
-      <c r="E60" s="51" t="n">
-        <v>678.9</v>
-      </c>
-      <c r="F60" s="51"/>
-      <c r="G60" s="52"/>
-      <c r="H60" s="52"/>
-      <c r="I60" s="53"/>
-      <c r="J60" s="53"/>
-      <c r="K60" s="53"/>
-      <c r="L60" s="53"/>
-      <c r="M60" s="53"/>
-      <c r="N60" s="53"/>
-      <c r="O60" s="53"/>
-      <c r="P60" s="53"/>
-      <c r="Q60" s="54"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="C61" s="56"/>
-      <c r="D61" s="57" t="s">
-        <v>81</v>
-      </c>
-      <c r="E61" s="58" t="n">
-        <v>135.36</v>
-      </c>
-      <c r="F61" s="58"/>
-      <c r="G61" s="59"/>
-      <c r="H61" s="59"/>
-      <c r="I61" s="60"/>
-      <c r="J61" s="60"/>
-      <c r="K61" s="60"/>
-      <c r="L61" s="60"/>
-      <c r="M61" s="60"/>
-      <c r="N61" s="60"/>
-      <c r="O61" s="60"/>
-      <c r="P61" s="60"/>
-      <c r="Q61" s="61"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="62"/>
-      <c r="C62" s="63"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="63"/>
-      <c r="F62" s="64"/>
-      <c r="G62" s="64"/>
-      <c r="H62" s="64"/>
-      <c r="I62" s="64"/>
-      <c r="J62" s="64"/>
-      <c r="K62" s="65"/>
-      <c r="L62" s="66"/>
-      <c r="M62" s="66"/>
-      <c r="N62" s="67"/>
-      <c r="O62" s="64"/>
-      <c r="P62" s="64"/>
-      <c r="Q62" s="64"/>
-      <c r="R62" s="68"/>
-      <c r="S62" s="68"/>
-      <c r="T62" s="68"/>
-      <c r="U62" s="68"/>
-      <c r="V62" s="68"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
-      <c r="P63" s="4"/>
-      <c r="Q63" s="4"/>
-      <c r="R63" s="4"/>
-    </row>
-    <row r="64" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C64" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F64" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="J64" s="12"/>
-      <c r="K64" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="L64" s="12"/>
-      <c r="M64" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="69" t="n">
-        <v>44258</v>
-      </c>
-      <c r="C65" s="70" t="n">
-        <v>44256.6360300926</v>
-      </c>
-      <c r="D65" s="70"/>
-      <c r="E65" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="F65" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="G65" s="71"/>
-      <c r="H65" s="71"/>
-      <c r="I65" s="21" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J65" s="21"/>
-      <c r="K65" s="21"/>
-      <c r="L65" s="21"/>
-      <c r="M65" s="72"/>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="69" t="n">
-        <v>44258</v>
-      </c>
-      <c r="C66" s="70" t="n">
-        <v>44256.6360300926</v>
-      </c>
-      <c r="D66" s="70"/>
-      <c r="E66" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="F66" s="71"/>
-      <c r="G66" s="71"/>
-      <c r="H66" s="71"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21" t="n">
-        <v>390.39</v>
-      </c>
-      <c r="L66" s="21"/>
-      <c r="M66" s="72" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="69" t="n">
-        <v>44258</v>
-      </c>
-      <c r="C67" s="70" t="n">
-        <v>44256.7498148148</v>
-      </c>
-      <c r="D67" s="70"/>
-      <c r="E67" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="F67" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="G67" s="71"/>
-      <c r="H67" s="71"/>
-      <c r="I67" s="21" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21"/>
-      <c r="L67" s="21"/>
-      <c r="M67" s="72"/>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="69" t="n">
-        <v>44258</v>
-      </c>
-      <c r="C68" s="70" t="n">
-        <v>44256.7498148148</v>
-      </c>
-      <c r="D68" s="70"/>
-      <c r="E68" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="F68" s="71"/>
-      <c r="G68" s="71"/>
-      <c r="H68" s="71"/>
-      <c r="I68" s="21"/>
-      <c r="J68" s="21"/>
-      <c r="K68" s="21" t="n">
-        <v>403.39</v>
-      </c>
-      <c r="L68" s="21"/>
-      <c r="M68" s="72" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="69" t="n">
-        <v>44259</v>
-      </c>
-      <c r="C69" s="70" t="n">
+      <c r="C71" s="71" t="n">
         <v>44257.8319444444</v>
       </c>
-      <c r="D69" s="70"/>
-      <c r="E69" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F69" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="G69" s="71"/>
-      <c r="H69" s="71"/>
-      <c r="I69" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21"/>
-      <c r="L69" s="21"/>
-      <c r="M69" s="72"/>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="69" t="n">
-        <v>44259</v>
-      </c>
-      <c r="C70" s="70" t="n">
-        <v>44257.8319444444</v>
-      </c>
-      <c r="D70" s="70"/>
-      <c r="E70" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F70" s="71"/>
-      <c r="G70" s="71"/>
-      <c r="H70" s="71"/>
-      <c r="I70" s="21"/>
-      <c r="J70" s="21"/>
-      <c r="K70" s="21" t="n">
-        <v>-382.44</v>
-      </c>
-      <c r="L70" s="21"/>
-      <c r="M70" s="72" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="69" t="n">
-        <v>44259</v>
-      </c>
-      <c r="C71" s="70" t="n">
-        <v>44257.3449884259</v>
-      </c>
-      <c r="D71" s="70"/>
+      <c r="D71" s="71"/>
       <c r="E71" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="F71" s="71"/>
-      <c r="G71" s="71"/>
-      <c r="H71" s="71"/>
+        <v>107</v>
+      </c>
+      <c r="F71" s="72"/>
+      <c r="G71" s="72"/>
+      <c r="H71" s="72"/>
       <c r="I71" s="21"/>
       <c r="J71" s="21"/>
       <c r="K71" s="21" t="n">
-        <v>-13257</v>
+        <v>-382.44</v>
       </c>
       <c r="L71" s="21"/>
-      <c r="M71" s="72" t="s">
-        <v>39</v>
+      <c r="M71" s="73" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="69" t="n">
-        <v>44260</v>
-      </c>
-      <c r="C72" s="70" t="n">
-        <v>44258.4781365741</v>
-      </c>
-      <c r="D72" s="70"/>
+      <c r="B72" s="70" t="n">
+        <v>44259</v>
+      </c>
+      <c r="C72" s="71" t="n">
+        <v>44257.3449884259</v>
+      </c>
+      <c r="D72" s="71"/>
       <c r="E72" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="F72" s="71"/>
-      <c r="G72" s="71"/>
-      <c r="H72" s="71"/>
+        <v>108</v>
+      </c>
+      <c r="F72" s="72"/>
+      <c r="G72" s="72"/>
+      <c r="H72" s="72"/>
       <c r="I72" s="21"/>
       <c r="J72" s="21"/>
       <c r="K72" s="21" t="n">
+        <v>-13257</v>
+      </c>
+      <c r="L72" s="21"/>
+      <c r="M72" s="73" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="70" t="n">
+        <v>44260</v>
+      </c>
+      <c r="C73" s="71" t="n">
+        <v>44258.4781365741</v>
+      </c>
+      <c r="D73" s="71"/>
+      <c r="E73" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F73" s="72"/>
+      <c r="G73" s="72"/>
+      <c r="H73" s="72"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21" t="n">
         <v>14149</v>
       </c>
-      <c r="L72" s="21"/>
-      <c r="M72" s="72" t="s">
+      <c r="L73" s="21"/>
+      <c r="M73" s="73" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B73" s="69" t="n">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B74" s="70" t="n">
         <v>44260</v>
       </c>
-      <c r="C73" s="70" t="n">
+      <c r="C74" s="71" t="n">
         <v>44258.4974421296</v>
       </c>
-      <c r="D73" s="70"/>
-      <c r="E73" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F73" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="G73" s="71"/>
-      <c r="H73" s="71"/>
-      <c r="I73" s="21" t="n">
-        <v>-50</v>
-      </c>
-      <c r="J73" s="21"/>
-      <c r="K73" s="21"/>
-      <c r="L73" s="21"/>
-      <c r="M73" s="72"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="69" t="n">
-        <v>44260</v>
-      </c>
-      <c r="C74" s="70" t="n">
-        <v>44258.4974421296</v>
-      </c>
-      <c r="D74" s="70"/>
+      <c r="D74" s="71"/>
       <c r="E74" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F74" s="71"/>
-      <c r="G74" s="71"/>
-      <c r="H74" s="71"/>
-      <c r="I74" s="21"/>
+      <c r="F74" s="72" t="s">
+        <v>36</v>
+      </c>
+      <c r="G74" s="72"/>
+      <c r="H74" s="72"/>
+      <c r="I74" s="21" t="n">
+        <v>-50</v>
+      </c>
       <c r="J74" s="21"/>
-      <c r="K74" s="21" t="n">
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
+      <c r="M74" s="73"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="70" t="n">
+        <v>44260</v>
+      </c>
+      <c r="C75" s="71" t="n">
+        <v>44258.4974421296</v>
+      </c>
+      <c r="D75" s="71"/>
+      <c r="E75" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F75" s="72"/>
+      <c r="G75" s="72"/>
+      <c r="H75" s="72"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="21" t="n">
         <v>2034</v>
       </c>
-      <c r="L74" s="21"/>
-      <c r="M74" s="72" t="s">
+      <c r="L75" s="21"/>
+      <c r="M75" s="73" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="9"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
-      <c r="J76" s="4"/>
-      <c r="K76" s="4"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
-      <c r="Q76" s="4"/>
-      <c r="R76" s="4"/>
-    </row>
-    <row r="77" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B77" s="73" t="s">
-        <v>75</v>
-      </c>
-      <c r="C77" s="12" t="s">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="9"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
+    </row>
+    <row r="78" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B78" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="12"/>
-      <c r="E77" s="74" t="s">
+      <c r="D78" s="12"/>
+      <c r="E78" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F77" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="12"/>
-      <c r="K77" s="12"/>
-      <c r="L77" s="12"/>
-      <c r="M77" s="12"/>
-      <c r="N77" s="12"/>
-      <c r="O77" s="12"/>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="69" t="n">
+      <c r="F78" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="12"/>
+      <c r="K78" s="12"/>
+      <c r="L78" s="12"/>
+      <c r="M78" s="12"/>
+      <c r="N78" s="12"/>
+      <c r="O78" s="12"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B79" s="70" t="n">
         <v>44257.9967824074</v>
       </c>
-      <c r="C78" s="21" t="n">
+      <c r="C79" s="21" t="n">
         <v>0.26</v>
       </c>
-      <c r="D78" s="21"/>
-      <c r="E78" s="75" t="s">
+      <c r="D79" s="21"/>
+      <c r="E79" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F78" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="G78" s="47"/>
-      <c r="H78" s="47"/>
-      <c r="I78" s="47"/>
-      <c r="J78" s="47"/>
-      <c r="K78" s="47"/>
-      <c r="L78" s="47"/>
-      <c r="M78" s="47"/>
-      <c r="N78" s="47"/>
-      <c r="O78" s="47"/>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="69" t="n">
+      <c r="F79" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="G79" s="48"/>
+      <c r="H79" s="48"/>
+      <c r="I79" s="48"/>
+      <c r="J79" s="48"/>
+      <c r="K79" s="48"/>
+      <c r="L79" s="48"/>
+      <c r="M79" s="48"/>
+      <c r="N79" s="48"/>
+      <c r="O79" s="48"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B80" s="70" t="n">
         <v>44257.9999884259</v>
       </c>
-      <c r="C79" s="21" t="n">
+      <c r="C80" s="21" t="n">
         <v>0.5</v>
       </c>
-      <c r="D79" s="21"/>
-      <c r="E79" s="75" t="s">
+      <c r="D80" s="21"/>
+      <c r="E80" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F79" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="G79" s="47"/>
-      <c r="H79" s="47"/>
-      <c r="I79" s="47"/>
-      <c r="J79" s="47"/>
-      <c r="K79" s="47"/>
-      <c r="L79" s="47"/>
-      <c r="M79" s="47"/>
-      <c r="N79" s="47"/>
-      <c r="O79" s="47"/>
-    </row>
-    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="69" t="n">
+      <c r="F80" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="G80" s="48"/>
+      <c r="H80" s="48"/>
+      <c r="I80" s="48"/>
+      <c r="J80" s="48"/>
+      <c r="K80" s="48"/>
+      <c r="L80" s="48"/>
+      <c r="M80" s="48"/>
+      <c r="N80" s="48"/>
+      <c r="O80" s="48"/>
+    </row>
+    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B81" s="70" t="n">
         <v>44258</v>
       </c>
-      <c r="C80" s="21" t="n">
+      <c r="C81" s="21" t="n">
         <v>2.92</v>
       </c>
-      <c r="D80" s="21"/>
-      <c r="E80" s="75" t="s">
+      <c r="D81" s="21"/>
+      <c r="E81" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="F80" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="G80" s="47"/>
-      <c r="H80" s="47"/>
-      <c r="I80" s="47"/>
-      <c r="J80" s="47"/>
-      <c r="K80" s="47"/>
-      <c r="L80" s="47"/>
-      <c r="M80" s="47"/>
-      <c r="N80" s="47"/>
-      <c r="O80" s="47"/>
-    </row>
-    <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="76" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="31" t="n">
+      <c r="F81" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="G81" s="48"/>
+      <c r="H81" s="48"/>
+      <c r="I81" s="48"/>
+      <c r="J81" s="48"/>
+      <c r="K81" s="48"/>
+      <c r="L81" s="48"/>
+      <c r="M81" s="48"/>
+      <c r="N81" s="48"/>
+      <c r="O81" s="48"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B82" s="77" t="s">
+        <v>99</v>
+      </c>
+      <c r="C82" s="32" t="n">
         <v>69.62</v>
       </c>
-      <c r="D81" s="31"/>
-      <c r="E81" s="77"/>
-      <c r="F81" s="78"/>
-      <c r="G81" s="78"/>
-      <c r="H81" s="78"/>
-      <c r="I81" s="78"/>
-      <c r="J81" s="78"/>
-      <c r="K81" s="78"/>
-      <c r="L81" s="78"/>
-      <c r="M81" s="78"/>
-      <c r="N81" s="78"/>
-      <c r="O81" s="79"/>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="2"/>
-      <c r="H82" s="80"/>
+      <c r="D82" s="32"/>
+      <c r="E82" s="78"/>
+      <c r="F82" s="79"/>
+      <c r="G82" s="79"/>
+      <c r="H82" s="79"/>
+      <c r="I82" s="79"/>
+      <c r="J82" s="79"/>
+      <c r="K82" s="79"/>
+      <c r="L82" s="79"/>
+      <c r="M82" s="79"/>
+      <c r="N82" s="79"/>
+      <c r="O82" s="80"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
-      <c r="K83" s="4"/>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4"/>
-      <c r="N83" s="4"/>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
-      <c r="Q83" s="4"/>
-      <c r="R83" s="4"/>
-    </row>
-    <row r="84" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B84" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12" t="s">
+      <c r="B83" s="2"/>
+      <c r="H83" s="81"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C84" s="4"/>
+      <c r="D84" s="4"/>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="4"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="4"/>
+      <c r="R84" s="4"/>
+    </row>
+    <row r="85" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B85" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H84" s="12"/>
-      <c r="I84" s="81" t="s">
+      <c r="H85" s="12"/>
+      <c r="I85" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="J84" s="12" t="s">
+      <c r="J85" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K84" s="82" t="s">
+      <c r="K85" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="L84" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="M84" s="12"/>
-      <c r="N84" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="O84" s="12"/>
-    </row>
-    <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="83" t="s">
+      <c r="L85" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C85" s="83"/>
-      <c r="D85" s="83"/>
-      <c r="E85" s="83"/>
-      <c r="F85" s="83"/>
-      <c r="G85" s="18" t="s">
+      <c r="M85" s="12"/>
+      <c r="N85" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="H85" s="18"/>
-      <c r="I85" s="84" t="s">
+      <c r="O85" s="12"/>
+    </row>
+    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B86" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="J85" s="15" t="s">
+      <c r="C86" s="84"/>
+      <c r="D86" s="84"/>
+      <c r="E86" s="84"/>
+      <c r="F86" s="84"/>
+      <c r="G86" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="K85" s="15" t="s">
+      <c r="H86" s="18"/>
+      <c r="I86" s="85" t="s">
+        <v>120</v>
+      </c>
+      <c r="J86" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="K86" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L85" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="M85" s="15"/>
-      <c r="N85" s="85" t="n">
+      <c r="L86" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="M86" s="15"/>
+      <c r="N86" s="86" t="n">
         <v>6</v>
       </c>
-      <c r="O85" s="85"/>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="83" t="s">
-        <v>121</v>
-      </c>
-      <c r="C86" s="83"/>
-      <c r="D86" s="83"/>
-      <c r="E86" s="83"/>
-      <c r="F86" s="83"/>
-      <c r="G86" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="H86" s="18"/>
-      <c r="I86" s="84"/>
-      <c r="J86" s="15" t="s">
+      <c r="O86" s="86"/>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B87" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="K86" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L86" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="M86" s="15"/>
-      <c r="N86" s="85" t="n">
-        <v>400</v>
-      </c>
-      <c r="O86" s="85"/>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="C87" s="83"/>
-      <c r="D87" s="83"/>
-      <c r="E87" s="83"/>
-      <c r="F87" s="83"/>
+      <c r="C87" s="84"/>
+      <c r="D87" s="84"/>
+      <c r="E87" s="84"/>
+      <c r="F87" s="84"/>
       <c r="G87" s="18" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="H87" s="18"/>
-      <c r="I87" s="84"/>
+      <c r="I87" s="85"/>
       <c r="J87" s="15" t="s">
-        <v>38</v>
+        <v>125</v>
       </c>
       <c r="K87" s="15" t="s">
         <v>39</v>
       </c>
       <c r="L87" s="15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="M87" s="15"/>
-      <c r="N87" s="85" t="n">
+      <c r="N87" s="86" t="n">
+        <v>400</v>
+      </c>
+      <c r="O87" s="86"/>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B88" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C88" s="84"/>
+      <c r="D88" s="84"/>
+      <c r="E88" s="84"/>
+      <c r="F88" s="84"/>
+      <c r="G88" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H88" s="18"/>
+      <c r="I88" s="85"/>
+      <c r="J88" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K88" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L88" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="M88" s="15"/>
+      <c r="N88" s="86" t="n">
         <v>200</v>
       </c>
-      <c r="O87" s="85"/>
-    </row>
-    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="83" t="s">
+      <c r="O88" s="86"/>
+    </row>
+    <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B89" s="84" t="s">
         <v>43</v>
       </c>
-      <c r="C88" s="83"/>
-      <c r="D88" s="83"/>
-      <c r="E88" s="83"/>
-      <c r="F88" s="83"/>
-      <c r="G88" s="18" t="s">
+      <c r="C89" s="84"/>
+      <c r="D89" s="84"/>
+      <c r="E89" s="84"/>
+      <c r="F89" s="84"/>
+      <c r="G89" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="H88" s="18"/>
-      <c r="I88" s="84" t="s">
+      <c r="H89" s="18"/>
+      <c r="I89" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="J88" s="15" t="s">
+      <c r="J89" s="15" t="s">
         <v>46</v>
-      </c>
-      <c r="K88" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L88" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="M88" s="15"/>
-      <c r="N88" s="85" t="n">
-        <v>9</v>
-      </c>
-      <c r="O88" s="85"/>
-    </row>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="86" t="s">
-        <v>73</v>
-      </c>
-      <c r="C89" s="86"/>
-      <c r="D89" s="86"/>
-      <c r="E89" s="86"/>
-      <c r="F89" s="86"/>
-      <c r="G89" s="87"/>
-      <c r="H89" s="87"/>
-      <c r="I89" s="84"/>
-      <c r="J89" s="15" t="s">
-        <v>124</v>
       </c>
       <c r="K89" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L89" s="88" t="s">
-        <v>120</v>
-      </c>
-      <c r="M89" s="88"/>
-      <c r="N89" s="85" t="n">
+      <c r="L89" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="M89" s="15"/>
+      <c r="N89" s="86" t="n">
+        <v>9</v>
+      </c>
+      <c r="O89" s="86"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B90" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="C90" s="84"/>
+      <c r="D90" s="84"/>
+      <c r="E90" s="84"/>
+      <c r="F90" s="84"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="85"/>
+      <c r="J90" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K90" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L90" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="M90" s="15"/>
+      <c r="N90" s="86" t="n">
         <v>0.06</v>
       </c>
-      <c r="O89" s="85"/>
-    </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="89"/>
-    </row>
-    <row r="1048262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="O90" s="86"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="87"/>
+    </row>
     <row r="1048263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3761,29 +3812,25 @@
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="R16:R17"/>
     <mergeCell ref="S16:S17"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="Q30:Q31"/>
-    <mergeCell ref="R30:R31"/>
-    <mergeCell ref="S30:S31"/>
-    <mergeCell ref="T30:T31"/>
-    <mergeCell ref="U30:U31"/>
-    <mergeCell ref="V30:V31"/>
-    <mergeCell ref="W30:W31"/>
-    <mergeCell ref="X30:X31"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:L37"/>
-    <mergeCell ref="M37:Q37"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="O31:O32"/>
+    <mergeCell ref="P31:P32"/>
+    <mergeCell ref="Q31:Q32"/>
+    <mergeCell ref="R31:R32"/>
+    <mergeCell ref="S31:S32"/>
+    <mergeCell ref="T31:T32"/>
+    <mergeCell ref="U31:U32"/>
+    <mergeCell ref="V31:V32"/>
+    <mergeCell ref="W31:W32"/>
+    <mergeCell ref="X31:X32"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="I38:L38"/>
@@ -3873,11 +3920,11 @@
     <mergeCell ref="I59:L59"/>
     <mergeCell ref="M59:Q59"/>
     <mergeCell ref="E60:F60"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="I60:L60"/>
+    <mergeCell ref="M60:Q60"/>
     <mergeCell ref="E61:F61"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="E62:F62"/>
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="F65:H65"/>
     <mergeCell ref="I65:J65"/>
@@ -3918,8 +3965,10 @@
     <mergeCell ref="F74:H74"/>
     <mergeCell ref="I74:J74"/>
     <mergeCell ref="K74:L74"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="F77:O77"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="K75:L75"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="F78:O78"/>
     <mergeCell ref="C79:D79"/>
@@ -3927,10 +3976,8 @@
     <mergeCell ref="C80:D80"/>
     <mergeCell ref="F80:O80"/>
     <mergeCell ref="C81:D81"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="L84:M84"/>
-    <mergeCell ref="N84:O84"/>
+    <mergeCell ref="F81:O81"/>
+    <mergeCell ref="C82:D82"/>
     <mergeCell ref="B85:F85"/>
     <mergeCell ref="G85:H85"/>
     <mergeCell ref="L85:M85"/>
@@ -3951,6 +3998,10 @@
     <mergeCell ref="G89:H89"/>
     <mergeCell ref="L89:M89"/>
     <mergeCell ref="N89:O89"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="L90:M90"/>
+    <mergeCell ref="N90:O90"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3973,7 +4024,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3996,7 +4047,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Just2Trade statement: crypto-currencies assets import
</commit_message>
<xml_diff>
--- a/tests/test_data/j2t.xlsx
+++ b/tests/test_data/j2t.xlsx
@@ -255,7 +255,7 @@
     <t xml:space="preserve">TR265176832</t>
   </si>
   <si>
-    <t xml:space="preserve">JT289500</t>
+    <t xml:space="preserve">JT222222</t>
   </si>
   <si>
     <t xml:space="preserve">MT5 Global (USD)</t>
@@ -749,7 +749,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -840,10 +840,6 @@
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1125,11 +1121,11 @@
   </sheetPr>
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T21" activeCellId="0" sqref="T21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.15"/>
@@ -1521,7 +1517,7 @@
       <c r="B21" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="15" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="16" t="s">
@@ -1626,30 +1622,30 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="32" t="n">
+      <c r="C23" s="24"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="31" t="n">
         <v>40.48</v>
       </c>
-      <c r="P23" s="32" t="n">
+      <c r="P23" s="31" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" s="31"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="32" t="n">
+      <c r="Q23" s="30"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="31" t="n">
         <v>-659.8</v>
       </c>
     </row>
@@ -1769,22 +1765,22 @@
       <c r="V28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="33"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="36"/>
-      <c r="K29" s="37"/>
-      <c r="L29" s="38"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="33"/>
-      <c r="O29" s="38"/>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="37"/>
     </row>
     <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
@@ -1957,7 +1953,7 @@
       <c r="W33" s="13" t="n">
         <v>22</v>
       </c>
-      <c r="X33" s="40" t="n">
+      <c r="X33" s="39" t="n">
         <v>23</v>
       </c>
     </row>
@@ -2001,7 +1997,7 @@
       <c r="P34" s="21" t="n">
         <v>0.4</v>
       </c>
-      <c r="Q34" s="41" t="n">
+      <c r="Q34" s="40" t="n">
         <v>1714</v>
       </c>
       <c r="R34" s="21" t="n">
@@ -2062,7 +2058,7 @@
       <c r="P35" s="21" t="n">
         <v>0.01</v>
       </c>
-      <c r="Q35" s="41" t="n">
+      <c r="Q35" s="40" t="n">
         <v>54614.73</v>
       </c>
       <c r="R35" s="21" t="n">
@@ -2084,22 +2080,22 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="33"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="37"/>
-      <c r="L36" s="38"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="33"/>
-      <c r="O36" s="38"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="38"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="37"/>
+      <c r="P36" s="32"/>
+      <c r="Q36" s="37"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="3" t="s">
@@ -2155,691 +2151,691 @@
       <c r="Q38" s="12"/>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="42" t="n">
+      <c r="B39" s="41" t="n">
         <v>44258</v>
       </c>
-      <c r="C39" s="43"/>
-      <c r="D39" s="44" t="s">
+      <c r="C39" s="42"/>
+      <c r="D39" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="45" t="n">
+      <c r="E39" s="44" t="n">
         <v>0.52</v>
       </c>
-      <c r="F39" s="45"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="47" t="s">
+      <c r="F39" s="44"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="J39" s="47"/>
-      <c r="K39" s="47"/>
-      <c r="L39" s="47"/>
-      <c r="M39" s="48" t="s">
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="N39" s="48"/>
-      <c r="O39" s="48"/>
-      <c r="P39" s="48"/>
-      <c r="Q39" s="48"/>
+      <c r="N39" s="47"/>
+      <c r="O39" s="47"/>
+      <c r="P39" s="47"/>
+      <c r="Q39" s="47"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="42" t="n">
+      <c r="B40" s="41" t="n">
         <v>44258</v>
       </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="44" t="s">
+      <c r="C40" s="42"/>
+      <c r="D40" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E40" s="45" t="n">
+      <c r="E40" s="44" t="n">
         <v>3.44</v>
       </c>
-      <c r="F40" s="45"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="47" t="s">
+      <c r="F40" s="44"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J40" s="47"/>
-      <c r="K40" s="47"/>
-      <c r="L40" s="47"/>
-      <c r="M40" s="48" t="s">
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="N40" s="48"/>
-      <c r="O40" s="48"/>
-      <c r="P40" s="48"/>
-      <c r="Q40" s="48"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="47"/>
+      <c r="P40" s="47"/>
+      <c r="Q40" s="47"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="42" t="n">
+      <c r="B41" s="41" t="n">
         <v>44258</v>
       </c>
-      <c r="C41" s="43"/>
-      <c r="D41" s="44" t="s">
+      <c r="C41" s="42"/>
+      <c r="D41" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E41" s="45" t="n">
+      <c r="E41" s="44" t="n">
         <v>2.13</v>
       </c>
-      <c r="F41" s="45"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="47" t="s">
+      <c r="F41" s="44"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="47"/>
-      <c r="M41" s="48" t="s">
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N41" s="48"/>
-      <c r="O41" s="48"/>
-      <c r="P41" s="48"/>
-      <c r="Q41" s="48"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="47"/>
+      <c r="P41" s="47"/>
+      <c r="Q41" s="47"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="42" t="n">
+      <c r="B42" s="41" t="n">
         <v>44258</v>
       </c>
-      <c r="C42" s="43"/>
-      <c r="D42" s="44" t="s">
+      <c r="C42" s="42"/>
+      <c r="D42" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E42" s="45" t="n">
+      <c r="E42" s="44" t="n">
         <v>6.37</v>
       </c>
-      <c r="F42" s="45"/>
-      <c r="G42" s="46"/>
-      <c r="H42" s="46"/>
-      <c r="I42" s="47" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J42" s="47"/>
-      <c r="K42" s="47"/>
-      <c r="L42" s="47"/>
-      <c r="M42" s="48" t="s">
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N42" s="48"/>
-      <c r="O42" s="48"/>
-      <c r="P42" s="48"/>
-      <c r="Q42" s="48"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="47"/>
+      <c r="Q42" s="47"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="42" t="n">
+      <c r="B43" s="41" t="n">
         <v>44259</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="44" t="s">
+      <c r="C43" s="42"/>
+      <c r="D43" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E43" s="45" t="n">
+      <c r="E43" s="44" t="n">
         <v>81.3</v>
       </c>
-      <c r="F43" s="45"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="46"/>
-      <c r="I43" s="47" t="s">
+      <c r="F43" s="44"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
-      <c r="L43" s="47"/>
-      <c r="M43" s="48" t="s">
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="47"/>
+      <c r="P43" s="47"/>
+      <c r="Q43" s="47"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="42" t="n">
+      <c r="B44" s="41" t="n">
         <v>44259</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="44" t="s">
+      <c r="C44" s="42"/>
+      <c r="D44" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="45" t="n">
+      <c r="E44" s="44" t="n">
         <v>84.24</v>
       </c>
-      <c r="F44" s="45"/>
-      <c r="G44" s="46"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="47" t="s">
+      <c r="F44" s="44"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J44" s="47"/>
-      <c r="K44" s="47"/>
-      <c r="L44" s="47"/>
-      <c r="M44" s="48" t="s">
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N44" s="48"/>
-      <c r="O44" s="48"/>
-      <c r="P44" s="48"/>
-      <c r="Q44" s="48"/>
+      <c r="N44" s="47"/>
+      <c r="O44" s="47"/>
+      <c r="P44" s="47"/>
+      <c r="Q44" s="47"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="42" t="n">
+      <c r="B45" s="41" t="n">
         <v>44259</v>
       </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="44" t="s">
+      <c r="C45" s="42"/>
+      <c r="D45" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E45" s="45" t="n">
+      <c r="E45" s="44" t="n">
         <v>23.25</v>
       </c>
-      <c r="F45" s="45"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="47" t="s">
+      <c r="F45" s="44"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J45" s="47"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="47"/>
-      <c r="M45" s="48" t="s">
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
+      <c r="M45" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N45" s="48"/>
-      <c r="O45" s="48"/>
-      <c r="P45" s="48"/>
-      <c r="Q45" s="48"/>
+      <c r="N45" s="47"/>
+      <c r="O45" s="47"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="47"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="42" t="n">
+      <c r="B46" s="41" t="n">
         <v>44260</v>
       </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="44" t="s">
+      <c r="C46" s="42"/>
+      <c r="D46" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E46" s="45" t="n">
+      <c r="E46" s="44" t="n">
         <v>18.34</v>
       </c>
-      <c r="F46" s="45"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
-      <c r="I46" s="47" t="s">
+      <c r="F46" s="44"/>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45"/>
+      <c r="I46" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J46" s="47"/>
-      <c r="K46" s="47"/>
-      <c r="L46" s="47"/>
-      <c r="M46" s="48" t="s">
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N46" s="48"/>
-      <c r="O46" s="48"/>
-      <c r="P46" s="48"/>
-      <c r="Q46" s="48"/>
+      <c r="N46" s="47"/>
+      <c r="O46" s="47"/>
+      <c r="P46" s="47"/>
+      <c r="Q46" s="47"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="42" t="n">
+      <c r="B47" s="41" t="n">
         <v>44260</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="44" t="s">
+      <c r="C47" s="42"/>
+      <c r="D47" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="45" t="n">
+      <c r="E47" s="44" t="n">
         <v>59.69</v>
       </c>
-      <c r="F47" s="45"/>
-      <c r="G47" s="46"/>
-      <c r="H47" s="46"/>
-      <c r="I47" s="47" t="s">
+      <c r="F47" s="44"/>
+      <c r="G47" s="45"/>
+      <c r="H47" s="45"/>
+      <c r="I47" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J47" s="47"/>
-      <c r="K47" s="47"/>
-      <c r="L47" s="47"/>
-      <c r="M47" s="48" t="s">
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N47" s="48"/>
-      <c r="O47" s="48"/>
-      <c r="P47" s="48"/>
-      <c r="Q47" s="48"/>
+      <c r="N47" s="47"/>
+      <c r="O47" s="47"/>
+      <c r="P47" s="47"/>
+      <c r="Q47" s="47"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="42" t="n">
+      <c r="B48" s="41" t="n">
         <v>44262</v>
       </c>
-      <c r="C48" s="43"/>
-      <c r="D48" s="44" t="s">
+      <c r="C48" s="42"/>
+      <c r="D48" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="45" t="n">
+      <c r="E48" s="44" t="n">
         <v>293.42</v>
       </c>
-      <c r="F48" s="45"/>
-      <c r="G48" s="46"/>
-      <c r="H48" s="46"/>
-      <c r="I48" s="47" t="s">
+      <c r="F48" s="44"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J48" s="47"/>
-      <c r="K48" s="47"/>
-      <c r="L48" s="47"/>
-      <c r="M48" s="48" t="s">
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
+      <c r="M48" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="N48" s="48"/>
-      <c r="O48" s="48"/>
-      <c r="P48" s="48"/>
-      <c r="Q48" s="48"/>
+      <c r="N48" s="47"/>
+      <c r="O48" s="47"/>
+      <c r="P48" s="47"/>
+      <c r="Q48" s="47"/>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="42" t="n">
+      <c r="B49" s="41" t="n">
         <v>44263</v>
       </c>
-      <c r="C49" s="43"/>
-      <c r="D49" s="44" t="s">
+      <c r="C49" s="42"/>
+      <c r="D49" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="45" t="n">
+      <c r="E49" s="44" t="n">
         <v>0.42</v>
       </c>
-      <c r="F49" s="45"/>
-      <c r="G49" s="46"/>
-      <c r="H49" s="46"/>
-      <c r="I49" s="47" t="s">
+      <c r="F49" s="44"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="J49" s="47"/>
-      <c r="K49" s="47"/>
-      <c r="L49" s="47"/>
-      <c r="M49" s="48" t="s">
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
+      <c r="M49" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="N49" s="48"/>
-      <c r="O49" s="48"/>
-      <c r="P49" s="48"/>
-      <c r="Q49" s="48"/>
+      <c r="N49" s="47"/>
+      <c r="O49" s="47"/>
+      <c r="P49" s="47"/>
+      <c r="Q49" s="47"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="42" t="n">
+      <c r="B50" s="41" t="n">
         <v>44263</v>
       </c>
-      <c r="C50" s="43"/>
-      <c r="D50" s="44" t="s">
+      <c r="C50" s="42"/>
+      <c r="D50" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E50" s="45" t="n">
+      <c r="E50" s="44" t="n">
         <v>2.78</v>
       </c>
-      <c r="F50" s="45"/>
-      <c r="G50" s="46"/>
-      <c r="H50" s="46"/>
-      <c r="I50" s="47" t="s">
+      <c r="F50" s="44"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J50" s="47"/>
-      <c r="K50" s="47"/>
-      <c r="L50" s="47"/>
-      <c r="M50" s="48" t="s">
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="N50" s="48"/>
-      <c r="O50" s="48"/>
-      <c r="P50" s="48"/>
-      <c r="Q50" s="48"/>
+      <c r="N50" s="47"/>
+      <c r="O50" s="47"/>
+      <c r="P50" s="47"/>
+      <c r="Q50" s="47"/>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="42" t="n">
+      <c r="B51" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C51" s="43"/>
-      <c r="D51" s="44" t="s">
+      <c r="C51" s="42"/>
+      <c r="D51" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E51" s="45" t="n">
+      <c r="E51" s="44" t="n">
         <v>1.46</v>
       </c>
-      <c r="F51" s="45"/>
-      <c r="G51" s="46"/>
-      <c r="H51" s="46"/>
-      <c r="I51" s="47" t="s">
+      <c r="F51" s="44"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="J51" s="47"/>
-      <c r="K51" s="47"/>
-      <c r="L51" s="47"/>
-      <c r="M51" s="48" t="s">
+      <c r="J51" s="46"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="46"/>
+      <c r="M51" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="N51" s="48"/>
-      <c r="O51" s="48"/>
-      <c r="P51" s="48"/>
-      <c r="Q51" s="48"/>
+      <c r="N51" s="47"/>
+      <c r="O51" s="47"/>
+      <c r="P51" s="47"/>
+      <c r="Q51" s="47"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="42" t="n">
+      <c r="B52" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C52" s="43"/>
-      <c r="D52" s="44" t="s">
+      <c r="C52" s="42"/>
+      <c r="D52" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E52" s="45" t="n">
+      <c r="E52" s="44" t="n">
         <v>9.75</v>
       </c>
-      <c r="F52" s="45"/>
-      <c r="G52" s="46"/>
-      <c r="H52" s="46"/>
-      <c r="I52" s="47" t="s">
+      <c r="F52" s="44"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="45"/>
+      <c r="I52" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J52" s="47"/>
-      <c r="K52" s="47"/>
-      <c r="L52" s="47"/>
-      <c r="M52" s="48" t="s">
+      <c r="J52" s="46"/>
+      <c r="K52" s="46"/>
+      <c r="L52" s="46"/>
+      <c r="M52" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="N52" s="48"/>
-      <c r="O52" s="48"/>
-      <c r="P52" s="48"/>
-      <c r="Q52" s="48"/>
+      <c r="N52" s="47"/>
+      <c r="O52" s="47"/>
+      <c r="P52" s="47"/>
+      <c r="Q52" s="47"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="42" t="n">
+      <c r="B53" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C53" s="43"/>
-      <c r="D53" s="44" t="s">
+      <c r="C53" s="42"/>
+      <c r="D53" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E53" s="45" t="n">
+      <c r="E53" s="44" t="n">
         <v>185.48</v>
       </c>
-      <c r="F53" s="45"/>
-      <c r="G53" s="46"/>
-      <c r="H53" s="46"/>
-      <c r="I53" s="47" t="s">
+      <c r="F53" s="44"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="45"/>
+      <c r="I53" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J53" s="47"/>
-      <c r="K53" s="47"/>
-      <c r="L53" s="47"/>
-      <c r="M53" s="48" t="s">
+      <c r="J53" s="46"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="46"/>
+      <c r="M53" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N53" s="48"/>
-      <c r="O53" s="48"/>
-      <c r="P53" s="48"/>
-      <c r="Q53" s="48"/>
+      <c r="N53" s="47"/>
+      <c r="O53" s="47"/>
+      <c r="P53" s="47"/>
+      <c r="Q53" s="47"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="42" t="n">
+      <c r="B54" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C54" s="43"/>
-      <c r="D54" s="44" t="s">
+      <c r="C54" s="42"/>
+      <c r="D54" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E54" s="45" t="n">
+      <c r="E54" s="44" t="n">
         <v>9.22</v>
       </c>
-      <c r="F54" s="45"/>
-      <c r="G54" s="46"/>
-      <c r="H54" s="46"/>
-      <c r="I54" s="47" t="s">
+      <c r="F54" s="44"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J54" s="47"/>
-      <c r="K54" s="47"/>
-      <c r="L54" s="47"/>
-      <c r="M54" s="48" t="s">
+      <c r="J54" s="46"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="46"/>
+      <c r="M54" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N54" s="48"/>
-      <c r="O54" s="48"/>
-      <c r="P54" s="48"/>
-      <c r="Q54" s="48"/>
+      <c r="N54" s="47"/>
+      <c r="O54" s="47"/>
+      <c r="P54" s="47"/>
+      <c r="Q54" s="47"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="42" t="n">
+      <c r="B55" s="41" t="n">
         <v>44264</v>
       </c>
-      <c r="C55" s="43"/>
-      <c r="D55" s="44" t="s">
+      <c r="C55" s="42"/>
+      <c r="D55" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E55" s="45" t="n">
+      <c r="E55" s="44" t="n">
         <v>1.82</v>
       </c>
-      <c r="F55" s="45"/>
-      <c r="G55" s="46"/>
-      <c r="H55" s="46"/>
-      <c r="I55" s="47" t="s">
+      <c r="F55" s="44"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J55" s="47"/>
-      <c r="K55" s="47"/>
-      <c r="L55" s="47"/>
-      <c r="M55" s="48" t="s">
+      <c r="J55" s="46"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="46"/>
+      <c r="M55" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N55" s="48"/>
-      <c r="O55" s="48"/>
-      <c r="P55" s="48"/>
-      <c r="Q55" s="48"/>
+      <c r="N55" s="47"/>
+      <c r="O55" s="47"/>
+      <c r="P55" s="47"/>
+      <c r="Q55" s="47"/>
     </row>
     <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="42" t="n">
+      <c r="B56" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C56" s="43"/>
-      <c r="D56" s="44" t="s">
+      <c r="C56" s="42"/>
+      <c r="D56" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E56" s="45" t="n">
+      <c r="E56" s="44" t="n">
         <v>0.61</v>
       </c>
-      <c r="F56" s="45"/>
-      <c r="G56" s="46"/>
-      <c r="H56" s="46"/>
-      <c r="I56" s="47" t="s">
+      <c r="F56" s="44"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="J56" s="47"/>
-      <c r="K56" s="47"/>
-      <c r="L56" s="47"/>
-      <c r="M56" s="48" t="s">
+      <c r="J56" s="46"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="46"/>
+      <c r="M56" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="N56" s="48"/>
-      <c r="O56" s="48"/>
-      <c r="P56" s="48"/>
-      <c r="Q56" s="48"/>
+      <c r="N56" s="47"/>
+      <c r="O56" s="47"/>
+      <c r="P56" s="47"/>
+      <c r="Q56" s="47"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="42" t="n">
+      <c r="B57" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C57" s="43"/>
-      <c r="D57" s="44" t="s">
+      <c r="C57" s="42"/>
+      <c r="D57" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E57" s="45" t="n">
+      <c r="E57" s="44" t="n">
         <v>4.04</v>
       </c>
-      <c r="F57" s="45"/>
-      <c r="G57" s="46"/>
-      <c r="H57" s="46"/>
-      <c r="I57" s="47" t="s">
+      <c r="F57" s="44"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="J57" s="47"/>
-      <c r="K57" s="47"/>
-      <c r="L57" s="47"/>
-      <c r="M57" s="48" t="s">
+      <c r="J57" s="46"/>
+      <c r="K57" s="46"/>
+      <c r="L57" s="46"/>
+      <c r="M57" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="N57" s="48"/>
-      <c r="O57" s="48"/>
-      <c r="P57" s="48"/>
-      <c r="Q57" s="48"/>
+      <c r="N57" s="47"/>
+      <c r="O57" s="47"/>
+      <c r="P57" s="47"/>
+      <c r="Q57" s="47"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="42" t="n">
+      <c r="B58" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C58" s="43"/>
-      <c r="D58" s="44" t="s">
+      <c r="C58" s="42"/>
+      <c r="D58" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E58" s="45" t="n">
+      <c r="E58" s="44" t="n">
         <v>21.13</v>
       </c>
-      <c r="F58" s="45"/>
-      <c r="G58" s="46"/>
-      <c r="H58" s="46"/>
-      <c r="I58" s="47" t="s">
+      <c r="F58" s="44"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J58" s="47"/>
-      <c r="K58" s="47"/>
-      <c r="L58" s="47"/>
-      <c r="M58" s="48" t="s">
+      <c r="J58" s="46"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="46"/>
+      <c r="M58" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N58" s="48"/>
-      <c r="O58" s="48"/>
-      <c r="P58" s="48"/>
-      <c r="Q58" s="48"/>
+      <c r="N58" s="47"/>
+      <c r="O58" s="47"/>
+      <c r="P58" s="47"/>
+      <c r="Q58" s="47"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="42" t="n">
+      <c r="B59" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C59" s="43"/>
-      <c r="D59" s="44" t="s">
+      <c r="C59" s="42"/>
+      <c r="D59" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E59" s="45" t="n">
+      <c r="E59" s="44" t="n">
         <v>3.5</v>
       </c>
-      <c r="F59" s="45"/>
-      <c r="G59" s="46"/>
-      <c r="H59" s="46"/>
-      <c r="I59" s="47" t="s">
+      <c r="F59" s="44"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J59" s="47"/>
-      <c r="K59" s="47"/>
-      <c r="L59" s="47"/>
-      <c r="M59" s="48" t="s">
+      <c r="J59" s="46"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="46"/>
+      <c r="M59" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N59" s="48"/>
-      <c r="O59" s="48"/>
-      <c r="P59" s="48"/>
-      <c r="Q59" s="48"/>
+      <c r="N59" s="47"/>
+      <c r="O59" s="47"/>
+      <c r="P59" s="47"/>
+      <c r="Q59" s="47"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="42" t="n">
+      <c r="B60" s="41" t="n">
         <v>44265</v>
       </c>
-      <c r="C60" s="43"/>
-      <c r="D60" s="44" t="s">
+      <c r="C60" s="42"/>
+      <c r="D60" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="E60" s="45" t="n">
+      <c r="E60" s="44" t="n">
         <v>1.35</v>
       </c>
-      <c r="F60" s="45"/>
-      <c r="G60" s="46"/>
-      <c r="H60" s="46"/>
-      <c r="I60" s="47" t="s">
+      <c r="F60" s="44"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="45"/>
+      <c r="I60" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="J60" s="47"/>
-      <c r="K60" s="47"/>
-      <c r="L60" s="47"/>
-      <c r="M60" s="48" t="s">
+      <c r="J60" s="46"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="46"/>
+      <c r="M60" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N60" s="48"/>
-      <c r="O60" s="48"/>
-      <c r="P60" s="48"/>
-      <c r="Q60" s="48"/>
+      <c r="N60" s="47"/>
+      <c r="O60" s="47"/>
+      <c r="P60" s="47"/>
+      <c r="Q60" s="47"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="49" t="s">
+      <c r="B61" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="C61" s="50"/>
-      <c r="D61" s="51" t="s">
+      <c r="C61" s="49"/>
+      <c r="D61" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="E61" s="52" t="n">
+      <c r="E61" s="51" t="n">
         <v>678.9</v>
       </c>
-      <c r="F61" s="52"/>
-      <c r="G61" s="53"/>
-      <c r="H61" s="53"/>
-      <c r="I61" s="54"/>
-      <c r="J61" s="54"/>
-      <c r="K61" s="54"/>
-      <c r="L61" s="54"/>
-      <c r="M61" s="54"/>
-      <c r="N61" s="54"/>
-      <c r="O61" s="54"/>
-      <c r="P61" s="54"/>
-      <c r="Q61" s="55"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="52"/>
+      <c r="H61" s="52"/>
+      <c r="I61" s="53"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="53"/>
+      <c r="L61" s="53"/>
+      <c r="M61" s="53"/>
+      <c r="N61" s="53"/>
+      <c r="O61" s="53"/>
+      <c r="P61" s="53"/>
+      <c r="Q61" s="54"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="56" t="s">
+      <c r="B62" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="57"/>
-      <c r="D62" s="58" t="s">
+      <c r="C62" s="56"/>
+      <c r="D62" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="E62" s="59" t="n">
+      <c r="E62" s="58" t="n">
         <v>135.36</v>
       </c>
-      <c r="F62" s="59"/>
-      <c r="G62" s="60"/>
-      <c r="H62" s="60"/>
-      <c r="I62" s="61"/>
-      <c r="J62" s="61"/>
-      <c r="K62" s="61"/>
-      <c r="L62" s="61"/>
-      <c r="M62" s="61"/>
-      <c r="N62" s="61"/>
-      <c r="O62" s="61"/>
-      <c r="P62" s="61"/>
-      <c r="Q62" s="62"/>
+      <c r="F62" s="58"/>
+      <c r="G62" s="59"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="60"/>
+      <c r="J62" s="60"/>
+      <c r="K62" s="60"/>
+      <c r="L62" s="60"/>
+      <c r="M62" s="60"/>
+      <c r="N62" s="60"/>
+      <c r="O62" s="60"/>
+      <c r="P62" s="60"/>
+      <c r="Q62" s="61"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="63"/>
-      <c r="C63" s="64"/>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="65"/>
-      <c r="G63" s="65"/>
-      <c r="H63" s="65"/>
-      <c r="I63" s="65"/>
-      <c r="J63" s="65"/>
-      <c r="K63" s="66"/>
-      <c r="L63" s="67"/>
-      <c r="M63" s="67"/>
-      <c r="N63" s="68"/>
-      <c r="O63" s="65"/>
-      <c r="P63" s="65"/>
-      <c r="Q63" s="65"/>
-      <c r="R63" s="69"/>
-      <c r="S63" s="69"/>
-      <c r="T63" s="69"/>
-      <c r="U63" s="69"/>
-      <c r="V63" s="69"/>
+      <c r="B63" s="62"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="63"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="64"/>
+      <c r="I63" s="64"/>
+      <c r="J63" s="64"/>
+      <c r="K63" s="65"/>
+      <c r="L63" s="66"/>
+      <c r="M63" s="66"/>
+      <c r="N63" s="67"/>
+      <c r="O63" s="64"/>
+      <c r="P63" s="64"/>
+      <c r="Q63" s="64"/>
+      <c r="R63" s="68"/>
+      <c r="S63" s="68"/>
+      <c r="T63" s="68"/>
+      <c r="U63" s="68"/>
+      <c r="V63" s="68"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="3" t="s">
@@ -2891,242 +2887,242 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="70" t="n">
+      <c r="B66" s="69" t="n">
         <v>44258</v>
       </c>
-      <c r="C66" s="71" t="n">
+      <c r="C66" s="70" t="n">
         <v>44256.6360300926</v>
       </c>
-      <c r="D66" s="71"/>
+      <c r="D66" s="70"/>
       <c r="E66" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F66" s="72" t="s">
+      <c r="F66" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G66" s="72"/>
-      <c r="H66" s="72"/>
+      <c r="G66" s="71"/>
+      <c r="H66" s="71"/>
       <c r="I66" s="21" t="n">
         <v>-1</v>
       </c>
       <c r="J66" s="21"/>
       <c r="K66" s="21"/>
       <c r="L66" s="21"/>
-      <c r="M66" s="73"/>
+      <c r="M66" s="72"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="70" t="n">
+      <c r="B67" s="69" t="n">
         <v>44258</v>
       </c>
-      <c r="C67" s="71" t="n">
+      <c r="C67" s="70" t="n">
         <v>44256.6360300926</v>
       </c>
-      <c r="D67" s="71"/>
+      <c r="D67" s="70"/>
       <c r="E67" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F67" s="72"/>
-      <c r="G67" s="72"/>
-      <c r="H67" s="72"/>
+      <c r="F67" s="71"/>
+      <c r="G67" s="71"/>
+      <c r="H67" s="71"/>
       <c r="I67" s="21"/>
       <c r="J67" s="21"/>
       <c r="K67" s="21" t="n">
         <v>390.39</v>
       </c>
       <c r="L67" s="21"/>
-      <c r="M67" s="73" t="s">
+      <c r="M67" s="72" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="70" t="n">
+      <c r="B68" s="69" t="n">
         <v>44258</v>
       </c>
-      <c r="C68" s="71" t="n">
+      <c r="C68" s="70" t="n">
         <v>44256.7498148148</v>
       </c>
-      <c r="D68" s="71"/>
+      <c r="D68" s="70"/>
       <c r="E68" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F68" s="72" t="s">
+      <c r="F68" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G68" s="72"/>
-      <c r="H68" s="72"/>
+      <c r="G68" s="71"/>
+      <c r="H68" s="71"/>
       <c r="I68" s="21" t="n">
         <v>-1</v>
       </c>
       <c r="J68" s="21"/>
       <c r="K68" s="21"/>
       <c r="L68" s="21"/>
-      <c r="M68" s="73"/>
+      <c r="M68" s="72"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="70" t="n">
+      <c r="B69" s="69" t="n">
         <v>44258</v>
       </c>
-      <c r="C69" s="71" t="n">
+      <c r="C69" s="70" t="n">
         <v>44256.7498148148</v>
       </c>
-      <c r="D69" s="71"/>
+      <c r="D69" s="70"/>
       <c r="E69" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F69" s="72"/>
-      <c r="G69" s="72"/>
-      <c r="H69" s="72"/>
+      <c r="F69" s="71"/>
+      <c r="G69" s="71"/>
+      <c r="H69" s="71"/>
       <c r="I69" s="21"/>
       <c r="J69" s="21"/>
       <c r="K69" s="21" t="n">
         <v>403.39</v>
       </c>
       <c r="L69" s="21"/>
-      <c r="M69" s="73" t="s">
+      <c r="M69" s="72" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B70" s="70" t="n">
+      <c r="B70" s="69" t="n">
         <v>44259</v>
       </c>
-      <c r="C70" s="71" t="n">
+      <c r="C70" s="70" t="n">
         <v>44257.8319444444</v>
       </c>
-      <c r="D70" s="71"/>
+      <c r="D70" s="70"/>
       <c r="E70" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="F70" s="72" t="s">
+      <c r="F70" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G70" s="72"/>
-      <c r="H70" s="72"/>
+      <c r="G70" s="71"/>
+      <c r="H70" s="71"/>
       <c r="I70" s="21" t="n">
         <v>1</v>
       </c>
       <c r="J70" s="21"/>
       <c r="K70" s="21"/>
       <c r="L70" s="21"/>
-      <c r="M70" s="73"/>
+      <c r="M70" s="72"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="70" t="n">
+      <c r="B71" s="69" t="n">
         <v>44259</v>
       </c>
-      <c r="C71" s="71" t="n">
+      <c r="C71" s="70" t="n">
         <v>44257.8319444444</v>
       </c>
-      <c r="D71" s="71"/>
+      <c r="D71" s="70"/>
       <c r="E71" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="F71" s="72"/>
-      <c r="G71" s="72"/>
-      <c r="H71" s="72"/>
+      <c r="F71" s="71"/>
+      <c r="G71" s="71"/>
+      <c r="H71" s="71"/>
       <c r="I71" s="21"/>
       <c r="J71" s="21"/>
       <c r="K71" s="21" t="n">
         <v>-382.44</v>
       </c>
       <c r="L71" s="21"/>
-      <c r="M71" s="73" t="s">
+      <c r="M71" s="72" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="70" t="n">
+      <c r="B72" s="69" t="n">
         <v>44259</v>
       </c>
-      <c r="C72" s="71" t="n">
+      <c r="C72" s="70" t="n">
         <v>44257.3449884259</v>
       </c>
-      <c r="D72" s="71"/>
+      <c r="D72" s="70"/>
       <c r="E72" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="F72" s="72"/>
-      <c r="G72" s="72"/>
-      <c r="H72" s="72"/>
+      <c r="F72" s="71"/>
+      <c r="G72" s="71"/>
+      <c r="H72" s="71"/>
       <c r="I72" s="21"/>
       <c r="J72" s="21"/>
       <c r="K72" s="21" t="n">
         <v>-13257</v>
       </c>
       <c r="L72" s="21"/>
-      <c r="M72" s="73" t="s">
+      <c r="M72" s="72" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="70" t="n">
+      <c r="B73" s="69" t="n">
         <v>44260</v>
       </c>
-      <c r="C73" s="71" t="n">
+      <c r="C73" s="70" t="n">
         <v>44258.4781365741</v>
       </c>
-      <c r="D73" s="71"/>
+      <c r="D73" s="70"/>
       <c r="E73" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="F73" s="72"/>
-      <c r="G73" s="72"/>
-      <c r="H73" s="72"/>
+      <c r="F73" s="71"/>
+      <c r="G73" s="71"/>
+      <c r="H73" s="71"/>
       <c r="I73" s="21"/>
       <c r="J73" s="21"/>
       <c r="K73" s="21" t="n">
         <v>14149</v>
       </c>
       <c r="L73" s="21"/>
-      <c r="M73" s="73" t="s">
+      <c r="M73" s="72" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="70" t="n">
+      <c r="B74" s="69" t="n">
         <v>44260</v>
       </c>
-      <c r="C74" s="71" t="n">
+      <c r="C74" s="70" t="n">
         <v>44258.4974421296</v>
       </c>
-      <c r="D74" s="71"/>
+      <c r="D74" s="70"/>
       <c r="E74" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F74" s="72" t="s">
+      <c r="F74" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="G74" s="72"/>
-      <c r="H74" s="72"/>
+      <c r="G74" s="71"/>
+      <c r="H74" s="71"/>
       <c r="I74" s="21" t="n">
         <v>-50</v>
       </c>
       <c r="J74" s="21"/>
       <c r="K74" s="21"/>
       <c r="L74" s="21"/>
-      <c r="M74" s="73"/>
+      <c r="M74" s="72"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="70" t="n">
+      <c r="B75" s="69" t="n">
         <v>44260</v>
       </c>
-      <c r="C75" s="71" t="n">
+      <c r="C75" s="70" t="n">
         <v>44258.4974421296</v>
       </c>
-      <c r="D75" s="71"/>
+      <c r="D75" s="70"/>
       <c r="E75" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F75" s="72"/>
-      <c r="G75" s="72"/>
-      <c r="H75" s="72"/>
+      <c r="F75" s="71"/>
+      <c r="G75" s="71"/>
+      <c r="H75" s="71"/>
       <c r="I75" s="21"/>
       <c r="J75" s="21"/>
       <c r="K75" s="21" t="n">
         <v>2034</v>
       </c>
       <c r="L75" s="21"/>
-      <c r="M75" s="73" t="s">
+      <c r="M75" s="72" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3155,14 +3151,14 @@
       <c r="R77" s="4"/>
     </row>
     <row r="78" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="74" t="s">
+      <c r="B78" s="73" t="s">
         <v>77</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D78" s="12"/>
-      <c r="E78" s="75" t="s">
+      <c r="E78" s="74" t="s">
         <v>10</v>
       </c>
       <c r="F78" s="12" t="s">
@@ -3179,100 +3175,100 @@
       <c r="O78" s="12"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="70" t="n">
+      <c r="B79" s="69" t="n">
         <v>44257.9967824074</v>
       </c>
       <c r="C79" s="21" t="n">
         <v>0.26</v>
       </c>
       <c r="D79" s="21"/>
-      <c r="E79" s="76" t="s">
+      <c r="E79" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="F79" s="48" t="s">
+      <c r="F79" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="G79" s="48"/>
-      <c r="H79" s="48"/>
-      <c r="I79" s="48"/>
-      <c r="J79" s="48"/>
-      <c r="K79" s="48"/>
-      <c r="L79" s="48"/>
-      <c r="M79" s="48"/>
-      <c r="N79" s="48"/>
-      <c r="O79" s="48"/>
+      <c r="G79" s="47"/>
+      <c r="H79" s="47"/>
+      <c r="I79" s="47"/>
+      <c r="J79" s="47"/>
+      <c r="K79" s="47"/>
+      <c r="L79" s="47"/>
+      <c r="M79" s="47"/>
+      <c r="N79" s="47"/>
+      <c r="O79" s="47"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="70" t="n">
+      <c r="B80" s="69" t="n">
         <v>44257.9999884259</v>
       </c>
       <c r="C80" s="21" t="n">
         <v>0.5</v>
       </c>
       <c r="D80" s="21"/>
-      <c r="E80" s="76" t="s">
+      <c r="E80" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="F80" s="48" t="s">
+      <c r="F80" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="G80" s="48"/>
-      <c r="H80" s="48"/>
-      <c r="I80" s="48"/>
-      <c r="J80" s="48"/>
-      <c r="K80" s="48"/>
-      <c r="L80" s="48"/>
-      <c r="M80" s="48"/>
-      <c r="N80" s="48"/>
-      <c r="O80" s="48"/>
+      <c r="G80" s="47"/>
+      <c r="H80" s="47"/>
+      <c r="I80" s="47"/>
+      <c r="J80" s="47"/>
+      <c r="K80" s="47"/>
+      <c r="L80" s="47"/>
+      <c r="M80" s="47"/>
+      <c r="N80" s="47"/>
+      <c r="O80" s="47"/>
     </row>
     <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="70" t="n">
+      <c r="B81" s="69" t="n">
         <v>44258</v>
       </c>
       <c r="C81" s="21" t="n">
         <v>2.92</v>
       </c>
       <c r="D81" s="21"/>
-      <c r="E81" s="76" t="s">
+      <c r="E81" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="F81" s="48" t="s">
+      <c r="F81" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="G81" s="48"/>
-      <c r="H81" s="48"/>
-      <c r="I81" s="48"/>
-      <c r="J81" s="48"/>
-      <c r="K81" s="48"/>
-      <c r="L81" s="48"/>
-      <c r="M81" s="48"/>
-      <c r="N81" s="48"/>
-      <c r="O81" s="48"/>
+      <c r="G81" s="47"/>
+      <c r="H81" s="47"/>
+      <c r="I81" s="47"/>
+      <c r="J81" s="47"/>
+      <c r="K81" s="47"/>
+      <c r="L81" s="47"/>
+      <c r="M81" s="47"/>
+      <c r="N81" s="47"/>
+      <c r="O81" s="47"/>
     </row>
     <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="77" t="s">
+      <c r="B82" s="76" t="s">
         <v>99</v>
       </c>
-      <c r="C82" s="32" t="n">
+      <c r="C82" s="31" t="n">
         <v>69.62</v>
       </c>
-      <c r="D82" s="32"/>
-      <c r="E82" s="78"/>
-      <c r="F82" s="79"/>
-      <c r="G82" s="79"/>
-      <c r="H82" s="79"/>
-      <c r="I82" s="79"/>
-      <c r="J82" s="79"/>
-      <c r="K82" s="79"/>
-      <c r="L82" s="79"/>
-      <c r="M82" s="79"/>
-      <c r="N82" s="79"/>
-      <c r="O82" s="80"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="77"/>
+      <c r="F82" s="78"/>
+      <c r="G82" s="78"/>
+      <c r="H82" s="78"/>
+      <c r="I82" s="78"/>
+      <c r="J82" s="78"/>
+      <c r="K82" s="78"/>
+      <c r="L82" s="78"/>
+      <c r="M82" s="78"/>
+      <c r="N82" s="78"/>
+      <c r="O82" s="79"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="2"/>
-      <c r="H83" s="81"/>
+      <c r="H83" s="80"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="3" t="s">
@@ -3307,13 +3303,13 @@
         <v>29</v>
       </c>
       <c r="H85" s="12"/>
-      <c r="I85" s="82" t="s">
+      <c r="I85" s="81" t="s">
         <v>30</v>
       </c>
       <c r="J85" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="K85" s="83" t="s">
+      <c r="K85" s="82" t="s">
         <v>32</v>
       </c>
       <c r="L85" s="12" t="s">
@@ -3326,18 +3322,18 @@
       <c r="O85" s="12"/>
     </row>
     <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="84" t="s">
+      <c r="B86" s="83" t="s">
         <v>118</v>
       </c>
-      <c r="C86" s="84"/>
-      <c r="D86" s="84"/>
-      <c r="E86" s="84"/>
-      <c r="F86" s="84"/>
+      <c r="C86" s="83"/>
+      <c r="D86" s="83"/>
+      <c r="E86" s="83"/>
+      <c r="F86" s="83"/>
       <c r="G86" s="18" t="s">
         <v>119</v>
       </c>
       <c r="H86" s="18"/>
-      <c r="I86" s="85" t="s">
+      <c r="I86" s="84" t="s">
         <v>120</v>
       </c>
       <c r="J86" s="15" t="s">
@@ -3350,24 +3346,24 @@
         <v>122</v>
       </c>
       <c r="M86" s="15"/>
-      <c r="N86" s="86" t="n">
+      <c r="N86" s="85" t="n">
         <v>6</v>
       </c>
-      <c r="O86" s="86"/>
+      <c r="O86" s="85"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="84" t="s">
+      <c r="B87" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="C87" s="84"/>
-      <c r="D87" s="84"/>
-      <c r="E87" s="84"/>
-      <c r="F87" s="84"/>
+      <c r="C87" s="83"/>
+      <c r="D87" s="83"/>
+      <c r="E87" s="83"/>
+      <c r="F87" s="83"/>
       <c r="G87" s="18" t="s">
         <v>124</v>
       </c>
       <c r="H87" s="18"/>
-      <c r="I87" s="85"/>
+      <c r="I87" s="84"/>
       <c r="J87" s="15" t="s">
         <v>125</v>
       </c>
@@ -3378,24 +3374,24 @@
         <v>122</v>
       </c>
       <c r="M87" s="15"/>
-      <c r="N87" s="86" t="n">
+      <c r="N87" s="85" t="n">
         <v>400</v>
       </c>
-      <c r="O87" s="86"/>
+      <c r="O87" s="85"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="84" t="s">
+      <c r="B88" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C88" s="84"/>
-      <c r="D88" s="84"/>
-      <c r="E88" s="84"/>
-      <c r="F88" s="84"/>
+      <c r="C88" s="83"/>
+      <c r="D88" s="83"/>
+      <c r="E88" s="83"/>
+      <c r="F88" s="83"/>
       <c r="G88" s="18" t="s">
         <v>37</v>
       </c>
       <c r="H88" s="18"/>
-      <c r="I88" s="85"/>
+      <c r="I88" s="84"/>
       <c r="J88" s="15" t="s">
         <v>38</v>
       </c>
@@ -3406,24 +3402,24 @@
         <v>122</v>
       </c>
       <c r="M88" s="15"/>
-      <c r="N88" s="86" t="n">
+      <c r="N88" s="85" t="n">
         <v>200</v>
       </c>
-      <c r="O88" s="86"/>
+      <c r="O88" s="85"/>
     </row>
     <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="84" t="s">
+      <c r="B89" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="C89" s="84"/>
-      <c r="D89" s="84"/>
-      <c r="E89" s="84"/>
-      <c r="F89" s="84"/>
+      <c r="C89" s="83"/>
+      <c r="D89" s="83"/>
+      <c r="E89" s="83"/>
+      <c r="F89" s="83"/>
       <c r="G89" s="18" t="s">
         <v>44</v>
       </c>
       <c r="H89" s="18"/>
-      <c r="I89" s="85" t="s">
+      <c r="I89" s="84" t="s">
         <v>45</v>
       </c>
       <c r="J89" s="15" t="s">
@@ -3436,22 +3432,22 @@
         <v>122</v>
       </c>
       <c r="M89" s="15"/>
-      <c r="N89" s="86" t="n">
+      <c r="N89" s="85" t="n">
         <v>9</v>
       </c>
-      <c r="O89" s="86"/>
+      <c r="O89" s="85"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="84" t="s">
+      <c r="B90" s="83" t="s">
         <v>75</v>
       </c>
-      <c r="C90" s="84"/>
-      <c r="D90" s="84"/>
-      <c r="E90" s="84"/>
-      <c r="F90" s="84"/>
+      <c r="C90" s="83"/>
+      <c r="D90" s="83"/>
+      <c r="E90" s="83"/>
+      <c r="F90" s="83"/>
       <c r="G90" s="18"/>
       <c r="H90" s="18"/>
-      <c r="I90" s="85"/>
+      <c r="I90" s="84"/>
       <c r="J90" s="15" t="s">
         <v>126</v>
       </c>
@@ -3462,13 +3458,13 @@
         <v>122</v>
       </c>
       <c r="M90" s="15"/>
-      <c r="N90" s="86" t="n">
+      <c r="N90" s="85" t="n">
         <v>0.06</v>
       </c>
-      <c r="O90" s="86"/>
+      <c r="O90" s="85"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="87"/>
+      <c r="B91" s="86"/>
     </row>
     <row r="1048263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4024,7 +4020,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4047,7 +4043,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Just2Trade statement: import dividends and corresponding taxes
</commit_message>
<xml_diff>
--- a/tests/test_data/j2t.xlsx
+++ b/tests/test_data/j2t.xlsx
@@ -14,10 +14,10 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="__DB10__" vbProcedure="false">page1!#ref!</definedName>
-    <definedName function="false" hidden="false" name="__DB11__" vbProcedure="false">Page1!$B$66:$M$66</definedName>
-    <definedName function="false" hidden="false" name="__DB12__" vbProcedure="false">Page1!$B$79:$E$79</definedName>
+    <definedName function="false" hidden="false" name="__DB11__" vbProcedure="false">Page1!$B$57:$M$57</definedName>
+    <definedName function="false" hidden="false" name="__DB12__" vbProcedure="false">Page1!$B$70:$E$70</definedName>
     <definedName function="false" hidden="false" name="__DB13__" vbProcedure="false">page1!#ref!</definedName>
-    <definedName function="false" hidden="false" name="__DB14__" vbProcedure="false">Page1!$B$86:$O$86</definedName>
+    <definedName function="false" hidden="false" name="__DB14__" vbProcedure="false">Page1!$B$77:$O$77</definedName>
     <definedName function="false" hidden="false" name="__DB15__" vbProcedure="false">page1!#ref!</definedName>
     <definedName function="false" hidden="false" name="__DB17__" vbProcedure="false">Page1!$B$34:$X$34</definedName>
     <definedName function="false" hidden="false" name="__DB18__" vbProcedure="false">page1!#ref!</definedName>
@@ -31,7 +31,7 @@
     <definedName function="false" hidden="false" name="__DB6__" vbProcedure="false">page1!#ref!</definedName>
     <definedName function="false" hidden="false" name="__DB7__" vbProcedure="false">page1!#ref!</definedName>
     <definedName function="false" hidden="false" name="__DB8__" vbProcedure="false">page1!#ref!</definedName>
-    <definedName function="false" hidden="false" name="__DB9__" vbProcedure="false">Page1!$B$39:$H$39</definedName>
+    <definedName function="false" hidden="false" name="__DB9__" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="126">
   <si>
     <t xml:space="preserve">Отчет по счету клиента за период с 03.03.2021 по 10.03.2021</t>
   </si>
@@ -295,45 +295,30 @@
     <t xml:space="preserve">Комментарий</t>
   </si>
   <si>
+    <t xml:space="preserve">IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Переоценка</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t xml:space="preserve">OUT</t>
   </si>
   <si>
+    <t xml:space="preserve">(2.8)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Внешние затраты::Комиссия внешнего брокера::Удержанный налог</t>
   </si>
   <si>
-    <t xml:space="preserve">Налог на дивиденды; Инструмент ConocoPhillips; Дата отсечки 12/02/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN</t>
+    <t xml:space="preserve">Налог на дивиденды; Инструмент PFIZER Inc; Дата отсечки 29/01/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Корпоративные действия::Дивиденды</t>
   </si>
   <si>
-    <t xml:space="preserve">Дивиденды; Инструмент ConocoPhillips; Дата отсечки 12/02/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Переоценка</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[sl 65.90]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2.8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Налог на дивиденды; Инструмент INTEL CORP; Дата отсечки 07/02/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дивиденды; Инструмент INTEL CORP; Дата отсечки 07/02/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Налог на дивиденды; Инструмент PFIZER Inc; Дата отсечки 29/01/2021</t>
-  </si>
-  <si>
     <t xml:space="preserve">Дивиденды; Инструмент PFIZER Inc; Дата отсечки 29/01/2021</t>
   </si>
   <si>
@@ -425,6 +410,18 @@
   </si>
   <si>
     <t xml:space="preserve">000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFIZER Inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US7170811035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFE  ;PFE.DE    ;PFE;5471</t>
   </si>
 </sst>
 </file>
@@ -444,7 +441,7 @@
     <numFmt numFmtId="173" formatCode="@"/>
     <numFmt numFmtId="174" formatCode="#,##0.000000"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
@@ -537,12 +534,6 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial Cyr"/>
-      <family val="0"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -749,7 +740,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1094,8 +1085,16 @@
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1121,11 +1120,11 @@
   </sheetPr>
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.15"/>
@@ -1513,7 +1512,7 @@
         <v>-366.49</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="32.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="14" t="s">
         <v>48</v>
       </c>
@@ -2150,7 +2149,7 @@
       <c r="P38" s="12"/>
       <c r="Q38" s="12"/>
     </row>
-    <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="41" t="n">
         <v>44258</v>
       </c>
@@ -2159,7 +2158,7 @@
         <v>83</v>
       </c>
       <c r="E39" s="44" t="n">
-        <v>0.52</v>
+        <v>2.13</v>
       </c>
       <c r="F39" s="44"/>
       <c r="G39" s="45"/>
@@ -2180,26 +2179,26 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="41" t="n">
-        <v>44258</v>
+        <v>44259</v>
       </c>
       <c r="C40" s="42"/>
       <c r="D40" s="43" t="s">
         <v>86</v>
       </c>
       <c r="E40" s="44" t="n">
-        <v>3.44</v>
+        <v>23.25</v>
       </c>
       <c r="F40" s="44"/>
       <c r="G40" s="45"/>
       <c r="H40" s="45"/>
       <c r="I40" s="46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J40" s="46"/>
       <c r="K40" s="46"/>
       <c r="L40" s="46"/>
       <c r="M40" s="47" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N40" s="47"/>
       <c r="O40" s="47"/>
@@ -2208,54 +2207,54 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="41" t="n">
-        <v>44258</v>
+        <v>44262</v>
       </c>
       <c r="C41" s="42"/>
       <c r="D41" s="43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E41" s="44" t="n">
-        <v>2.13</v>
+        <v>293.42</v>
       </c>
       <c r="F41" s="44"/>
       <c r="G41" s="45"/>
       <c r="H41" s="45"/>
       <c r="I41" s="46" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J41" s="46"/>
       <c r="K41" s="46"/>
       <c r="L41" s="46"/>
       <c r="M41" s="47" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N41" s="47"/>
       <c r="O41" s="47"/>
       <c r="P41" s="47"/>
       <c r="Q41" s="47"/>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="41" t="n">
-        <v>44258</v>
+        <v>44264</v>
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="43" t="s">
         <v>86</v>
       </c>
       <c r="E42" s="44" t="n">
-        <v>6.37</v>
+        <v>1.46</v>
       </c>
       <c r="F42" s="44"/>
       <c r="G42" s="45"/>
       <c r="H42" s="45"/>
       <c r="I42" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J42" s="46"/>
       <c r="K42" s="46"/>
       <c r="L42" s="46"/>
       <c r="M42" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N42" s="47"/>
       <c r="O42" s="47"/>
@@ -2264,20 +2263,20 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="41" t="n">
-        <v>44259</v>
+        <v>44264</v>
       </c>
       <c r="C43" s="42"/>
       <c r="D43" s="43" t="s">
         <v>83</v>
       </c>
       <c r="E43" s="44" t="n">
-        <v>81.3</v>
+        <v>9.75</v>
       </c>
       <c r="F43" s="44"/>
       <c r="G43" s="45"/>
       <c r="H43" s="45"/>
       <c r="I43" s="46" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J43" s="46"/>
       <c r="K43" s="46"/>
@@ -2292,26 +2291,26 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="41" t="n">
-        <v>44259</v>
+        <v>44264</v>
       </c>
       <c r="C44" s="42"/>
       <c r="D44" s="43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E44" s="44" t="n">
-        <v>84.24</v>
+        <v>185.48</v>
       </c>
       <c r="F44" s="44"/>
       <c r="G44" s="45"/>
       <c r="H44" s="45"/>
       <c r="I44" s="46" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J44" s="46"/>
       <c r="K44" s="46"/>
       <c r="L44" s="46"/>
       <c r="M44" s="47" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="N44" s="47"/>
       <c r="O44" s="47"/>
@@ -2320,26 +2319,26 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="41" t="n">
-        <v>44259</v>
+        <v>44264</v>
       </c>
       <c r="C45" s="42"/>
       <c r="D45" s="43" t="s">
         <v>83</v>
       </c>
       <c r="E45" s="44" t="n">
-        <v>23.25</v>
+        <v>9.22</v>
       </c>
       <c r="F45" s="44"/>
       <c r="G45" s="45"/>
       <c r="H45" s="45"/>
       <c r="I45" s="46" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J45" s="46"/>
       <c r="K45" s="46"/>
       <c r="L45" s="46"/>
       <c r="M45" s="47" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="N45" s="47"/>
       <c r="O45" s="47"/>
@@ -2348,54 +2347,54 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="41" t="n">
-        <v>44260</v>
+        <v>44264</v>
       </c>
       <c r="C46" s="42"/>
       <c r="D46" s="43" t="s">
         <v>86</v>
       </c>
       <c r="E46" s="44" t="n">
-        <v>18.34</v>
+        <v>1.82</v>
       </c>
       <c r="F46" s="44"/>
       <c r="G46" s="45"/>
       <c r="H46" s="45"/>
       <c r="I46" s="46" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="J46" s="46"/>
       <c r="K46" s="46"/>
       <c r="L46" s="46"/>
       <c r="M46" s="47" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="N46" s="47"/>
       <c r="O46" s="47"/>
       <c r="P46" s="47"/>
       <c r="Q46" s="47"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="41" t="n">
-        <v>44260</v>
+        <v>44265</v>
       </c>
       <c r="C47" s="42"/>
       <c r="D47" s="43" t="s">
         <v>86</v>
       </c>
       <c r="E47" s="44" t="n">
-        <v>59.69</v>
+        <v>0.61</v>
       </c>
       <c r="F47" s="44"/>
       <c r="G47" s="45"/>
       <c r="H47" s="45"/>
       <c r="I47" s="46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J47" s="46"/>
       <c r="K47" s="46"/>
       <c r="L47" s="46"/>
       <c r="M47" s="47" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="N47" s="47"/>
       <c r="O47" s="47"/>
@@ -2404,42 +2403,42 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="41" t="n">
-        <v>44262</v>
+        <v>44265</v>
       </c>
       <c r="C48" s="42"/>
       <c r="D48" s="43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E48" s="44" t="n">
-        <v>293.42</v>
+        <v>4.04</v>
       </c>
       <c r="F48" s="44"/>
       <c r="G48" s="45"/>
       <c r="H48" s="45"/>
       <c r="I48" s="46" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J48" s="46"/>
       <c r="K48" s="46"/>
       <c r="L48" s="46"/>
       <c r="M48" s="47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N48" s="47"/>
       <c r="O48" s="47"/>
       <c r="P48" s="47"/>
       <c r="Q48" s="47"/>
     </row>
-    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="41" t="n">
-        <v>44263</v>
+        <v>44265</v>
       </c>
       <c r="C49" s="42"/>
       <c r="D49" s="43" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E49" s="44" t="n">
-        <v>0.42</v>
+        <v>21.13</v>
       </c>
       <c r="F49" s="44"/>
       <c r="G49" s="45"/>
@@ -2451,7 +2450,7 @@
       <c r="K49" s="46"/>
       <c r="L49" s="46"/>
       <c r="M49" s="47" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="N49" s="47"/>
       <c r="O49" s="47"/>
@@ -2460,42 +2459,42 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="41" t="n">
-        <v>44263</v>
+        <v>44265</v>
       </c>
       <c r="C50" s="42"/>
       <c r="D50" s="43" t="s">
         <v>86</v>
       </c>
       <c r="E50" s="44" t="n">
-        <v>2.78</v>
+        <v>3.5</v>
       </c>
       <c r="F50" s="44"/>
       <c r="G50" s="45"/>
       <c r="H50" s="45"/>
       <c r="I50" s="46" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J50" s="46"/>
       <c r="K50" s="46"/>
       <c r="L50" s="46"/>
       <c r="M50" s="47" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="N50" s="47"/>
       <c r="O50" s="47"/>
       <c r="P50" s="47"/>
       <c r="Q50" s="47"/>
     </row>
-    <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="41" t="n">
-        <v>44264</v>
+        <v>44265</v>
       </c>
       <c r="C51" s="42"/>
       <c r="D51" s="43" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E51" s="44" t="n">
-        <v>1.46</v>
+        <v>1.35</v>
       </c>
       <c r="F51" s="44"/>
       <c r="G51" s="45"/>
@@ -2507,965 +2506,749 @@
       <c r="K51" s="46"/>
       <c r="L51" s="46"/>
       <c r="M51" s="47" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="N51" s="47"/>
       <c r="O51" s="47"/>
       <c r="P51" s="47"/>
       <c r="Q51" s="47"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="41" t="n">
-        <v>44264</v>
-      </c>
-      <c r="C52" s="42"/>
-      <c r="D52" s="43" t="s">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="49"/>
+      <c r="D52" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" s="51" t="n">
+        <v>678.9</v>
+      </c>
+      <c r="F52" s="51"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="53"/>
+      <c r="L52" s="53"/>
+      <c r="M52" s="53"/>
+      <c r="N52" s="53"/>
+      <c r="O52" s="53"/>
+      <c r="P52" s="53"/>
+      <c r="Q52" s="54"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="56"/>
+      <c r="D53" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="E52" s="44" t="n">
-        <v>9.75</v>
-      </c>
-      <c r="F52" s="44"/>
-      <c r="G52" s="45"/>
-      <c r="H52" s="45"/>
-      <c r="I52" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J52" s="46"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="46"/>
-      <c r="M52" s="47" t="s">
+      <c r="E53" s="58" t="n">
+        <v>135.36</v>
+      </c>
+      <c r="F53" s="58"/>
+      <c r="G53" s="59"/>
+      <c r="H53" s="59"/>
+      <c r="I53" s="60"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="60"/>
+      <c r="L53" s="60"/>
+      <c r="M53" s="60"/>
+      <c r="N53" s="60"/>
+      <c r="O53" s="60"/>
+      <c r="P53" s="60"/>
+      <c r="Q53" s="61"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="62"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="64"/>
+      <c r="G54" s="64"/>
+      <c r="H54" s="64"/>
+      <c r="I54" s="64"/>
+      <c r="J54" s="64"/>
+      <c r="K54" s="65"/>
+      <c r="L54" s="66"/>
+      <c r="M54" s="66"/>
+      <c r="N54" s="67"/>
+      <c r="O54" s="64"/>
+      <c r="P54" s="64"/>
+      <c r="Q54" s="64"/>
+      <c r="R54" s="68"/>
+      <c r="S54" s="68"/>
+      <c r="T54" s="68"/>
+      <c r="U54" s="68"/>
+      <c r="V54" s="68"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+    </row>
+    <row r="56" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B56" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F56" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="N52" s="47"/>
-      <c r="O52" s="47"/>
-      <c r="P52" s="47"/>
-      <c r="Q52" s="47"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="41" t="n">
-        <v>44264</v>
-      </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" s="44" t="n">
-        <v>185.48</v>
-      </c>
-      <c r="F53" s="44"/>
-      <c r="G53" s="45"/>
-      <c r="H53" s="45"/>
-      <c r="I53" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="J53" s="46"/>
-      <c r="K53" s="46"/>
-      <c r="L53" s="46"/>
-      <c r="M53" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="N53" s="47"/>
-      <c r="O53" s="47"/>
-      <c r="P53" s="47"/>
-      <c r="Q53" s="47"/>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B54" s="41" t="n">
-        <v>44264</v>
-      </c>
-      <c r="C54" s="42"/>
-      <c r="D54" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" s="44" t="n">
-        <v>9.22</v>
-      </c>
-      <c r="F54" s="44"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="45"/>
-      <c r="I54" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="J54" s="46"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="46"/>
-      <c r="M54" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="N54" s="47"/>
-      <c r="O54" s="47"/>
-      <c r="P54" s="47"/>
-      <c r="Q54" s="47"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B55" s="41" t="n">
-        <v>44264</v>
-      </c>
-      <c r="C55" s="42"/>
-      <c r="D55" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="E55" s="44" t="n">
-        <v>1.82</v>
-      </c>
-      <c r="F55" s="44"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="J55" s="46"/>
-      <c r="K55" s="46"/>
-      <c r="L55" s="46"/>
-      <c r="M55" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="N55" s="47"/>
-      <c r="O55" s="47"/>
-      <c r="P55" s="47"/>
-      <c r="Q55" s="47"/>
-    </row>
-    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C56" s="42"/>
-      <c r="D56" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="E56" s="44" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="F56" s="44"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="J56" s="46"/>
-      <c r="K56" s="46"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="47" t="s">
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="N56" s="47"/>
-      <c r="O56" s="47"/>
-      <c r="P56" s="47"/>
-      <c r="Q56" s="47"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L56" s="12"/>
+      <c r="M56" s="12" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C57" s="42"/>
-      <c r="D57" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="E57" s="44" t="n">
-        <v>4.04</v>
-      </c>
-      <c r="F57" s="44"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="46" t="s">
-        <v>87</v>
-      </c>
-      <c r="J57" s="46"/>
-      <c r="K57" s="46"/>
-      <c r="L57" s="46"/>
-      <c r="M57" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="N57" s="47"/>
-      <c r="O57" s="47"/>
-      <c r="P57" s="47"/>
-      <c r="Q57" s="47"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B58" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C58" s="42"/>
-      <c r="D58" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="E58" s="44" t="n">
-        <v>21.13</v>
-      </c>
-      <c r="F58" s="44"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="J58" s="46"/>
-      <c r="K58" s="46"/>
-      <c r="L58" s="46"/>
-      <c r="M58" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="N58" s="47"/>
-      <c r="O58" s="47"/>
-      <c r="P58" s="47"/>
-      <c r="Q58" s="47"/>
+      <c r="B57" s="69" t="n">
+        <v>44258</v>
+      </c>
+      <c r="C57" s="70" t="n">
+        <v>44256.6360300926</v>
+      </c>
+      <c r="D57" s="70"/>
+      <c r="E57" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="G57" s="71"/>
+      <c r="H57" s="71"/>
+      <c r="I57" s="21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J57" s="21"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="72"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="69" t="n">
+        <v>44258</v>
+      </c>
+      <c r="C58" s="70" t="n">
+        <v>44256.6360300926</v>
+      </c>
+      <c r="D58" s="70"/>
+      <c r="E58" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F58" s="71"/>
+      <c r="G58" s="71"/>
+      <c r="H58" s="71"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21" t="n">
+        <v>390.39</v>
+      </c>
+      <c r="L58" s="21"/>
+      <c r="M58" s="72" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C59" s="42"/>
-      <c r="D59" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="E59" s="44" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="F59" s="44"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="J59" s="46"/>
-      <c r="K59" s="46"/>
-      <c r="L59" s="46"/>
-      <c r="M59" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="N59" s="47"/>
-      <c r="O59" s="47"/>
-      <c r="P59" s="47"/>
-      <c r="Q59" s="47"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="41" t="n">
-        <v>44265</v>
-      </c>
-      <c r="C60" s="42"/>
-      <c r="D60" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="E60" s="44" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="F60" s="44"/>
-      <c r="G60" s="45"/>
-      <c r="H60" s="45"/>
-      <c r="I60" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="J60" s="46"/>
-      <c r="K60" s="46"/>
-      <c r="L60" s="46"/>
-      <c r="M60" s="47" t="s">
-        <v>90</v>
-      </c>
-      <c r="N60" s="47"/>
-      <c r="O60" s="47"/>
-      <c r="P60" s="47"/>
-      <c r="Q60" s="47"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" s="49"/>
-      <c r="D61" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="E61" s="51" t="n">
-        <v>678.9</v>
-      </c>
-      <c r="F61" s="51"/>
-      <c r="G61" s="52"/>
-      <c r="H61" s="52"/>
-      <c r="I61" s="53"/>
-      <c r="J61" s="53"/>
-      <c r="K61" s="53"/>
-      <c r="L61" s="53"/>
-      <c r="M61" s="53"/>
-      <c r="N61" s="53"/>
-      <c r="O61" s="53"/>
-      <c r="P61" s="53"/>
-      <c r="Q61" s="54"/>
+      <c r="B59" s="69" t="n">
+        <v>44258</v>
+      </c>
+      <c r="C59" s="70" t="n">
+        <v>44256.7498148148</v>
+      </c>
+      <c r="D59" s="70"/>
+      <c r="E59" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F59" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="G59" s="71"/>
+      <c r="H59" s="71"/>
+      <c r="I59" s="21" t="n">
+        <v>-1</v>
+      </c>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
+      <c r="M59" s="72"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="69" t="n">
+        <v>44258</v>
+      </c>
+      <c r="C60" s="70" t="n">
+        <v>44256.7498148148</v>
+      </c>
+      <c r="D60" s="70"/>
+      <c r="E60" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" s="71"/>
+      <c r="G60" s="71"/>
+      <c r="H60" s="71"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21" t="n">
+        <v>403.39</v>
+      </c>
+      <c r="L60" s="21"/>
+      <c r="M60" s="72" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B61" s="69" t="n">
+        <v>44259</v>
+      </c>
+      <c r="C61" s="70" t="n">
+        <v>44257.8319444444</v>
+      </c>
+      <c r="D61" s="70"/>
+      <c r="E61" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F61" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="G61" s="71"/>
+      <c r="H61" s="71"/>
+      <c r="I61" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
+      <c r="M61" s="72"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="55" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="56"/>
-      <c r="D62" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="E62" s="58" t="n">
-        <v>135.36</v>
-      </c>
-      <c r="F62" s="58"/>
-      <c r="G62" s="59"/>
-      <c r="H62" s="59"/>
-      <c r="I62" s="60"/>
-      <c r="J62" s="60"/>
-      <c r="K62" s="60"/>
-      <c r="L62" s="60"/>
-      <c r="M62" s="60"/>
-      <c r="N62" s="60"/>
-      <c r="O62" s="60"/>
-      <c r="P62" s="60"/>
-      <c r="Q62" s="61"/>
+      <c r="B62" s="69" t="n">
+        <v>44259</v>
+      </c>
+      <c r="C62" s="70" t="n">
+        <v>44257.8319444444</v>
+      </c>
+      <c r="D62" s="70"/>
+      <c r="E62" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F62" s="71"/>
+      <c r="G62" s="71"/>
+      <c r="H62" s="71"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="21" t="n">
+        <v>-382.44</v>
+      </c>
+      <c r="L62" s="21"/>
+      <c r="M62" s="72" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="62"/>
-      <c r="C63" s="63"/>
-      <c r="D63" s="63"/>
-      <c r="E63" s="63"/>
-      <c r="F63" s="64"/>
-      <c r="G63" s="64"/>
-      <c r="H63" s="64"/>
-      <c r="I63" s="64"/>
-      <c r="J63" s="64"/>
-      <c r="K63" s="65"/>
-      <c r="L63" s="66"/>
-      <c r="M63" s="66"/>
-      <c r="N63" s="67"/>
-      <c r="O63" s="64"/>
-      <c r="P63" s="64"/>
-      <c r="Q63" s="64"/>
-      <c r="R63" s="68"/>
-      <c r="S63" s="68"/>
-      <c r="T63" s="68"/>
-      <c r="U63" s="68"/>
-      <c r="V63" s="68"/>
+      <c r="B63" s="69" t="n">
+        <v>44259</v>
+      </c>
+      <c r="C63" s="70" t="n">
+        <v>44257.3449884259</v>
+      </c>
+      <c r="D63" s="70"/>
+      <c r="E63" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F63" s="71"/>
+      <c r="G63" s="71"/>
+      <c r="H63" s="71"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21" t="n">
+        <v>-13257</v>
+      </c>
+      <c r="L63" s="21"/>
+      <c r="M63" s="72" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-      <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
-      <c r="Q64" s="4"/>
-      <c r="R64" s="4"/>
-    </row>
-    <row r="65" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B65" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F65" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="J65" s="12"/>
-      <c r="K65" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L65" s="12"/>
-      <c r="M65" s="12" t="s">
+      <c r="B64" s="69" t="n">
+        <v>44260</v>
+      </c>
+      <c r="C64" s="70" t="n">
+        <v>44258.4781365741</v>
+      </c>
+      <c r="D64" s="70"/>
+      <c r="E64" s="18" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F64" s="71"/>
+      <c r="G64" s="71"/>
+      <c r="H64" s="71"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="21"/>
+      <c r="K64" s="21" t="n">
+        <v>14149</v>
+      </c>
+      <c r="L64" s="21"/>
+      <c r="M64" s="72" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B65" s="69" t="n">
+        <v>44260</v>
+      </c>
+      <c r="C65" s="70" t="n">
+        <v>44258.4974421296</v>
+      </c>
+      <c r="D65" s="70"/>
+      <c r="E65" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="G65" s="71"/>
+      <c r="H65" s="71"/>
+      <c r="I65" s="21" t="n">
+        <v>-50</v>
+      </c>
+      <c r="J65" s="21"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="21"/>
+      <c r="M65" s="72"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="69" t="n">
-        <v>44258</v>
+        <v>44260</v>
       </c>
       <c r="C66" s="70" t="n">
-        <v>44256.6360300926</v>
+        <v>44258.4974421296</v>
       </c>
       <c r="D66" s="70"/>
       <c r="E66" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="F66" s="71" t="s">
-        <v>43</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F66" s="71"/>
       <c r="G66" s="71"/>
       <c r="H66" s="71"/>
-      <c r="I66" s="21" t="n">
-        <v>-1</v>
-      </c>
+      <c r="I66" s="21"/>
       <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
+      <c r="K66" s="21" t="n">
+        <v>2034</v>
+      </c>
       <c r="L66" s="21"/>
-      <c r="M66" s="72"/>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="69" t="n">
-        <v>44258</v>
-      </c>
-      <c r="C67" s="70" t="n">
-        <v>44256.6360300926</v>
-      </c>
-      <c r="D67" s="70"/>
-      <c r="E67" s="18" t="s">
+      <c r="M66" s="72" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="9"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F67" s="71"/>
-      <c r="G67" s="71"/>
-      <c r="H67" s="71"/>
-      <c r="I67" s="21"/>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21" t="n">
-        <v>390.39</v>
-      </c>
-      <c r="L67" s="21"/>
-      <c r="M67" s="72" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B68" s="69" t="n">
-        <v>44258</v>
-      </c>
-      <c r="C68" s="70" t="n">
-        <v>44256.7498148148</v>
-      </c>
-      <c r="D68" s="70"/>
-      <c r="E68" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="F68" s="71" t="s">
-        <v>43</v>
-      </c>
-      <c r="G68" s="71"/>
-      <c r="H68" s="71"/>
-      <c r="I68" s="21" t="n">
-        <v>-1</v>
-      </c>
-      <c r="J68" s="21"/>
-      <c r="K68" s="21"/>
-      <c r="L68" s="21"/>
-      <c r="M68" s="72"/>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="69" t="n">
-        <v>44258</v>
-      </c>
-      <c r="C69" s="70" t="n">
-        <v>44256.7498148148</v>
-      </c>
-      <c r="D69" s="70"/>
-      <c r="E69" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="F69" s="71"/>
-      <c r="G69" s="71"/>
-      <c r="H69" s="71"/>
-      <c r="I69" s="21"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="21" t="n">
-        <v>403.39</v>
-      </c>
-      <c r="L69" s="21"/>
-      <c r="M69" s="72" t="s">
-        <v>11</v>
-      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="4"/>
+      <c r="Q68" s="4"/>
+      <c r="R68" s="4"/>
+    </row>
+    <row r="69" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B69" s="73" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="12"/>
+      <c r="E69" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="12"/>
+      <c r="M69" s="12"/>
+      <c r="N69" s="12"/>
+      <c r="O69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="69" t="n">
-        <v>44259</v>
-      </c>
-      <c r="C70" s="70" t="n">
-        <v>44257.8319444444</v>
-      </c>
-      <c r="D70" s="70"/>
-      <c r="E70" s="18" t="s">
+        <v>44257.9967824074</v>
+      </c>
+      <c r="C70" s="21" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="D70" s="21"/>
+      <c r="E70" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="G70" s="47"/>
+      <c r="H70" s="47"/>
+      <c r="I70" s="47"/>
+      <c r="J70" s="47"/>
+      <c r="K70" s="47"/>
+      <c r="L70" s="47"/>
+      <c r="M70" s="47"/>
+      <c r="N70" s="47"/>
+      <c r="O70" s="47"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B71" s="69" t="n">
+        <v>44257.9999884259</v>
+      </c>
+      <c r="C71" s="21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D71" s="21"/>
+      <c r="E71" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="F70" s="71" t="s">
+      <c r="G71" s="47"/>
+      <c r="H71" s="47"/>
+      <c r="I71" s="47"/>
+      <c r="J71" s="47"/>
+      <c r="K71" s="47"/>
+      <c r="L71" s="47"/>
+      <c r="M71" s="47"/>
+      <c r="N71" s="47"/>
+      <c r="O71" s="47"/>
+    </row>
+    <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B72" s="69" t="n">
+        <v>44258</v>
+      </c>
+      <c r="C72" s="21" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="D72" s="21"/>
+      <c r="E72" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="G72" s="47"/>
+      <c r="H72" s="47"/>
+      <c r="I72" s="47"/>
+      <c r="J72" s="47"/>
+      <c r="K72" s="47"/>
+      <c r="L72" s="47"/>
+      <c r="M72" s="47"/>
+      <c r="N72" s="47"/>
+      <c r="O72" s="47"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B73" s="76" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="31" t="n">
+        <v>69.62</v>
+      </c>
+      <c r="D73" s="31"/>
+      <c r="E73" s="77"/>
+      <c r="F73" s="78"/>
+      <c r="G73" s="78"/>
+      <c r="H73" s="78"/>
+      <c r="I73" s="78"/>
+      <c r="J73" s="78"/>
+      <c r="K73" s="78"/>
+      <c r="L73" s="78"/>
+      <c r="M73" s="78"/>
+      <c r="N73" s="78"/>
+      <c r="O73" s="79"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="2"/>
+      <c r="H74" s="80"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="4"/>
+    </row>
+    <row r="76" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B76" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H76" s="12"/>
+      <c r="I76" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="J76" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K76" s="82" t="s">
+        <v>32</v>
+      </c>
+      <c r="L76" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="M76" s="12"/>
+      <c r="N76" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O76" s="12"/>
+    </row>
+    <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B77" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="C77" s="83"/>
+      <c r="D77" s="83"/>
+      <c r="E77" s="83"/>
+      <c r="F77" s="83"/>
+      <c r="G77" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H77" s="18"/>
+      <c r="I77" s="84" t="s">
+        <v>115</v>
+      </c>
+      <c r="J77" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="K77" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="L77" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="M77" s="15"/>
+      <c r="N77" s="85" t="n">
+        <v>6</v>
+      </c>
+      <c r="O77" s="85"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B78" s="83" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" s="83"/>
+      <c r="D78" s="83"/>
+      <c r="E78" s="83"/>
+      <c r="F78" s="83"/>
+      <c r="G78" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="H78" s="18"/>
+      <c r="I78" s="84"/>
+      <c r="J78" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="K78" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L78" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="M78" s="15"/>
+      <c r="N78" s="85" t="n">
+        <v>400</v>
+      </c>
+      <c r="O78" s="85"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B79" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="C79" s="83"/>
+      <c r="D79" s="83"/>
+      <c r="E79" s="83"/>
+      <c r="F79" s="83"/>
+      <c r="G79" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H79" s="18"/>
+      <c r="I79" s="84"/>
+      <c r="J79" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K79" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L79" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="M79" s="15"/>
+      <c r="N79" s="85" t="n">
+        <v>200</v>
+      </c>
+      <c r="O79" s="85"/>
+    </row>
+    <row r="80" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B80" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="G70" s="71"/>
-      <c r="H70" s="71"/>
-      <c r="I70" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="J70" s="21"/>
-      <c r="K70" s="21"/>
-      <c r="L70" s="21"/>
-      <c r="M70" s="72"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="69" t="n">
-        <v>44259</v>
-      </c>
-      <c r="C71" s="70" t="n">
-        <v>44257.8319444444</v>
-      </c>
-      <c r="D71" s="70"/>
-      <c r="E71" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="F71" s="71"/>
-      <c r="G71" s="71"/>
-      <c r="H71" s="71"/>
-      <c r="I71" s="21"/>
-      <c r="J71" s="21"/>
-      <c r="K71" s="21" t="n">
-        <v>-382.44</v>
-      </c>
-      <c r="L71" s="21"/>
-      <c r="M71" s="72" t="s">
+      <c r="C80" s="83"/>
+      <c r="D80" s="83"/>
+      <c r="E80" s="83"/>
+      <c r="F80" s="83"/>
+      <c r="G80" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H80" s="18"/>
+      <c r="I80" s="84" t="s">
+        <v>45</v>
+      </c>
+      <c r="J80" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K80" s="15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="69" t="n">
-        <v>44259</v>
-      </c>
-      <c r="C72" s="70" t="n">
-        <v>44257.3449884259</v>
-      </c>
-      <c r="D72" s="70"/>
-      <c r="E72" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="F72" s="71"/>
-      <c r="G72" s="71"/>
-      <c r="H72" s="71"/>
-      <c r="I72" s="21"/>
-      <c r="J72" s="21"/>
-      <c r="K72" s="21" t="n">
-        <v>-13257</v>
-      </c>
-      <c r="L72" s="21"/>
-      <c r="M72" s="72" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="69" t="n">
-        <v>44260</v>
-      </c>
-      <c r="C73" s="70" t="n">
-        <v>44258.4781365741</v>
-      </c>
-      <c r="D73" s="70"/>
-      <c r="E73" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="F73" s="71"/>
-      <c r="G73" s="71"/>
-      <c r="H73" s="71"/>
-      <c r="I73" s="21"/>
-      <c r="J73" s="21"/>
-      <c r="K73" s="21" t="n">
-        <v>14149</v>
-      </c>
-      <c r="L73" s="21"/>
-      <c r="M73" s="72" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B74" s="69" t="n">
-        <v>44260</v>
-      </c>
-      <c r="C74" s="70" t="n">
-        <v>44258.4974421296</v>
-      </c>
-      <c r="D74" s="70"/>
-      <c r="E74" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F74" s="71" t="s">
-        <v>36</v>
-      </c>
-      <c r="G74" s="71"/>
-      <c r="H74" s="71"/>
-      <c r="I74" s="21" t="n">
-        <v>-50</v>
-      </c>
-      <c r="J74" s="21"/>
-      <c r="K74" s="21"/>
-      <c r="L74" s="21"/>
-      <c r="M74" s="72"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="69" t="n">
-        <v>44260</v>
-      </c>
-      <c r="C75" s="70" t="n">
-        <v>44258.4974421296</v>
-      </c>
-      <c r="D75" s="70"/>
-      <c r="E75" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F75" s="71"/>
-      <c r="G75" s="71"/>
-      <c r="H75" s="71"/>
-      <c r="I75" s="21"/>
-      <c r="J75" s="21"/>
-      <c r="K75" s="21" t="n">
-        <v>2034</v>
-      </c>
-      <c r="L75" s="21"/>
-      <c r="M75" s="72" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="9"/>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4"/>
-      <c r="K77" s="4"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
-      <c r="Q77" s="4"/>
-      <c r="R77" s="4"/>
-    </row>
-    <row r="78" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B78" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="C78" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" s="12"/>
-      <c r="E78" s="74" t="s">
-        <v>10</v>
-      </c>
-      <c r="F78" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
-      <c r="K78" s="12"/>
-      <c r="L78" s="12"/>
-      <c r="M78" s="12"/>
-      <c r="N78" s="12"/>
-      <c r="O78" s="12"/>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B79" s="69" t="n">
-        <v>44257.9967824074</v>
-      </c>
-      <c r="C79" s="21" t="n">
-        <v>0.26</v>
-      </c>
-      <c r="D79" s="21"/>
-      <c r="E79" s="75" t="s">
+      <c r="L80" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="M80" s="15"/>
+      <c r="N80" s="85" t="n">
+        <v>9</v>
+      </c>
+      <c r="O80" s="85"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B81" s="83" t="s">
+        <v>75</v>
+      </c>
+      <c r="C81" s="83"/>
+      <c r="D81" s="83"/>
+      <c r="E81" s="83"/>
+      <c r="F81" s="83"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="84"/>
+      <c r="J81" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="K81" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F79" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="G79" s="47"/>
-      <c r="H79" s="47"/>
-      <c r="I79" s="47"/>
-      <c r="J79" s="47"/>
-      <c r="K79" s="47"/>
-      <c r="L79" s="47"/>
-      <c r="M79" s="47"/>
-      <c r="N79" s="47"/>
-      <c r="O79" s="47"/>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B80" s="69" t="n">
-        <v>44257.9999884259</v>
-      </c>
-      <c r="C80" s="21" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D80" s="21"/>
-      <c r="E80" s="75" t="s">
+      <c r="L81" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="M81" s="15"/>
+      <c r="N81" s="85" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="O81" s="85"/>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B82" s="86" t="s">
+        <v>122</v>
+      </c>
+      <c r="C82" s="86"/>
+      <c r="D82" s="86"/>
+      <c r="E82" s="86"/>
+      <c r="F82" s="86"/>
+      <c r="G82" s="87" t="s">
+        <v>123</v>
+      </c>
+      <c r="H82" s="87"/>
+      <c r="I82" s="84" t="s">
+        <v>124</v>
+      </c>
+      <c r="J82" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="K82" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F80" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="G80" s="47"/>
-      <c r="H80" s="47"/>
-      <c r="I80" s="47"/>
-      <c r="J80" s="47"/>
-      <c r="K80" s="47"/>
-      <c r="L80" s="47"/>
-      <c r="M80" s="47"/>
-      <c r="N80" s="47"/>
-      <c r="O80" s="47"/>
-    </row>
-    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B81" s="69" t="n">
-        <v>44258</v>
-      </c>
-      <c r="C81" s="21" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="D81" s="21"/>
-      <c r="E81" s="75" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="G81" s="47"/>
-      <c r="H81" s="47"/>
-      <c r="I81" s="47"/>
-      <c r="J81" s="47"/>
-      <c r="K81" s="47"/>
-      <c r="L81" s="47"/>
-      <c r="M81" s="47"/>
-      <c r="N81" s="47"/>
-      <c r="O81" s="47"/>
-    </row>
-    <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="76" t="s">
-        <v>99</v>
-      </c>
-      <c r="C82" s="31" t="n">
-        <v>69.62</v>
-      </c>
-      <c r="D82" s="31"/>
-      <c r="E82" s="77"/>
-      <c r="F82" s="78"/>
-      <c r="G82" s="78"/>
-      <c r="H82" s="78"/>
-      <c r="I82" s="78"/>
-      <c r="J82" s="78"/>
-      <c r="K82" s="78"/>
-      <c r="L82" s="78"/>
-      <c r="M82" s="78"/>
-      <c r="N82" s="78"/>
-      <c r="O82" s="79"/>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="2"/>
-      <c r="H83" s="80"/>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="4"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
-      <c r="P84" s="4"/>
-      <c r="Q84" s="4"/>
-      <c r="R84" s="4"/>
-    </row>
-    <row r="85" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B85" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
-      <c r="G85" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H85" s="12"/>
-      <c r="I85" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="J85" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K85" s="82" t="s">
-        <v>32</v>
-      </c>
-      <c r="L85" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="M85" s="12"/>
-      <c r="N85" s="12" t="s">
+      <c r="L82" s="88" t="s">
         <v>117</v>
       </c>
-      <c r="O85" s="12"/>
-    </row>
-    <row r="86" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B86" s="83" t="s">
-        <v>118</v>
-      </c>
-      <c r="C86" s="83"/>
-      <c r="D86" s="83"/>
-      <c r="E86" s="83"/>
-      <c r="F86" s="83"/>
-      <c r="G86" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="H86" s="18"/>
-      <c r="I86" s="84" t="s">
-        <v>120</v>
-      </c>
-      <c r="J86" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="K86" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L86" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="M86" s="15"/>
-      <c r="N86" s="85" t="n">
-        <v>6</v>
-      </c>
-      <c r="O86" s="85"/>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B87" s="83" t="s">
-        <v>123</v>
-      </c>
-      <c r="C87" s="83"/>
-      <c r="D87" s="83"/>
-      <c r="E87" s="83"/>
-      <c r="F87" s="83"/>
-      <c r="G87" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="H87" s="18"/>
-      <c r="I87" s="84"/>
-      <c r="J87" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="K87" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L87" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="M87" s="15"/>
-      <c r="N87" s="85" t="n">
-        <v>400</v>
-      </c>
-      <c r="O87" s="85"/>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B88" s="83" t="s">
-        <v>36</v>
-      </c>
-      <c r="C88" s="83"/>
-      <c r="D88" s="83"/>
-      <c r="E88" s="83"/>
-      <c r="F88" s="83"/>
-      <c r="G88" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="H88" s="18"/>
-      <c r="I88" s="84"/>
-      <c r="J88" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K88" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L88" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="M88" s="15"/>
-      <c r="N88" s="85" t="n">
-        <v>200</v>
-      </c>
-      <c r="O88" s="85"/>
-    </row>
-    <row r="89" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B89" s="83" t="s">
-        <v>43</v>
-      </c>
-      <c r="C89" s="83"/>
-      <c r="D89" s="83"/>
-      <c r="E89" s="83"/>
-      <c r="F89" s="83"/>
-      <c r="G89" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H89" s="18"/>
-      <c r="I89" s="84" t="s">
-        <v>45</v>
-      </c>
-      <c r="J89" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="K89" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L89" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="M89" s="15"/>
-      <c r="N89" s="85" t="n">
-        <v>9</v>
-      </c>
-      <c r="O89" s="85"/>
-    </row>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B90" s="83" t="s">
-        <v>75</v>
-      </c>
-      <c r="C90" s="83"/>
-      <c r="D90" s="83"/>
-      <c r="E90" s="83"/>
-      <c r="F90" s="83"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="18"/>
-      <c r="I90" s="84"/>
-      <c r="J90" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="K90" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="L90" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="M90" s="15"/>
-      <c r="N90" s="85" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="O90" s="85"/>
-    </row>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="86"/>
-    </row>
+      <c r="M82" s="88"/>
+      <c r="N82" s="85" t="n">
+        <v>35</v>
+      </c>
+      <c r="O82" s="85"/>
+    </row>
+    <row r="1048254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3781,7 +3564,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="216">
+  <mergeCells count="184">
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
@@ -3884,43 +3667,43 @@
     <mergeCell ref="I51:L51"/>
     <mergeCell ref="M51:Q51"/>
     <mergeCell ref="E52:F52"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I52:L52"/>
-    <mergeCell ref="M52:Q52"/>
     <mergeCell ref="E53:F53"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="I53:L53"/>
-    <mergeCell ref="M53:Q53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="M54:Q54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="I55:L55"/>
-    <mergeCell ref="M55:Q55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="I56:L56"/>
-    <mergeCell ref="M56:Q56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="I57:L57"/>
-    <mergeCell ref="M57:Q57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="I58:L58"/>
-    <mergeCell ref="M58:Q58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="I59:L59"/>
-    <mergeCell ref="M59:Q59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="I60:L60"/>
-    <mergeCell ref="M60:Q60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="F57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="F58:H58"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="F60:H60"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="F61:H61"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="F62:H62"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="K64:L64"/>
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="F65:H65"/>
     <mergeCell ref="I65:J65"/>
@@ -3929,75 +3712,43 @@
     <mergeCell ref="F66:H66"/>
     <mergeCell ref="I66:J66"/>
     <mergeCell ref="K66:L66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="K68:L68"/>
     <mergeCell ref="C69:D69"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="K69:L69"/>
+    <mergeCell ref="F69:O69"/>
     <mergeCell ref="C70:D70"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="K70:L70"/>
+    <mergeCell ref="F70:O70"/>
     <mergeCell ref="C71:D71"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="K71:L71"/>
+    <mergeCell ref="F71:O71"/>
     <mergeCell ref="C72:D72"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="F72:O72"/>
     <mergeCell ref="C73:D73"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="K73:L73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="K74:L74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="F78:O78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="F79:O79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="F80:O80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="F81:O81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="L85:M85"/>
-    <mergeCell ref="N85:O85"/>
-    <mergeCell ref="B86:F86"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="L86:M86"/>
-    <mergeCell ref="N86:O86"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="L87:M87"/>
-    <mergeCell ref="N87:O87"/>
-    <mergeCell ref="B88:F88"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="L88:M88"/>
-    <mergeCell ref="N88:O88"/>
-    <mergeCell ref="B89:F89"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="L89:M89"/>
-    <mergeCell ref="N89:O89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="L90:M90"/>
-    <mergeCell ref="N90:O90"/>
+    <mergeCell ref="B76:F76"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="L76:M76"/>
+    <mergeCell ref="N76:O76"/>
+    <mergeCell ref="B77:F77"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="L77:M77"/>
+    <mergeCell ref="N77:O77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="L78:M78"/>
+    <mergeCell ref="N78:O78"/>
+    <mergeCell ref="B79:F79"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="L79:M79"/>
+    <mergeCell ref="N79:O79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="L80:M80"/>
+    <mergeCell ref="N80:O80"/>
+    <mergeCell ref="B81:F81"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="L81:M81"/>
+    <mergeCell ref="N81:O81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="L82:M82"/>
+    <mergeCell ref="N82:O82"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4020,7 +3771,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4043,7 +3794,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Just2Trade statement: import dividends and corresponding taxes - regex updated to handle more cases.
</commit_message>
<xml_diff>
--- a/tests/test_data/j2t.xlsx
+++ b/tests/test_data/j2t.xlsx
@@ -322,10 +322,10 @@
     <t xml:space="preserve">Дивиденды; Инструмент PFIZER Inc; Дата отсечки 29/01/2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Налог на дивиденды; Инструмент JOHNSON &amp; JOHNSON; Дата отсечки 23/02/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дивиденды; Инструмент JOHNSON &amp; JOHNSON; Дата отсечки 23/02/2021</t>
+    <t xml:space="preserve">Налог на дивиденды; Начисление дивидендов полученных по счету "JT222222"". Инструмент JOHNSON &amp; JOHNSON; Дата отсечки 23/02/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дивиденды; Начисление дивидендов полученных по счету "JT222222"". Инструмент JOHNSON &amp; JOHNSON; Дата отсечки 23/02/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Итого:</t>
@@ -740,7 +740,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="86">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1083,18 +1083,6 @@
     </xf>
     <xf numFmtId="174" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1120,14 +1108,14 @@
   </sheetPr>
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M47" activeCellId="0" sqref="M47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>
@@ -3211,17 +3199,17 @@
       <c r="O81" s="85"/>
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B82" s="86" t="s">
+      <c r="B82" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="C82" s="86"/>
-      <c r="D82" s="86"/>
-      <c r="E82" s="86"/>
-      <c r="F82" s="86"/>
-      <c r="G82" s="87" t="s">
+      <c r="C82" s="83"/>
+      <c r="D82" s="83"/>
+      <c r="E82" s="83"/>
+      <c r="F82" s="83"/>
+      <c r="G82" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="H82" s="87"/>
+      <c r="H82" s="18"/>
       <c r="I82" s="84" t="s">
         <v>124</v>
       </c>
@@ -3231,10 +3219,10 @@
       <c r="K82" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L82" s="88" t="s">
+      <c r="L82" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="M82" s="88"/>
+      <c r="M82" s="15"/>
       <c r="N82" s="85" t="n">
         <v>35</v>
       </c>
@@ -3771,7 +3759,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3794,7 +3782,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Just2Trade statement: Fee load from cash transaction table. Refactoring of cash transaction table loading.
</commit_message>
<xml_diff>
--- a/tests/test_data/j2t.xlsx
+++ b/tests/test_data/j2t.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="128">
   <si>
     <t xml:space="preserve">Отчет по счету клиента за период с 03.03.2021 по 10.03.2021</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t xml:space="preserve">Дивиденды; Инструмент PFIZER Inc; Дата отсечки 29/01/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Внешние затраты::Комиссия внешнего депозитария</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Депозитарная комиссия за выплату дивидендов; Начисление дивидендов полученных по счету "JT222222"". Инструмент Sony Group Corp; Дата отсечки 29/09/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Налог на дивиденды; Начисление дивидендов полученных по счету "JT222222"". Инструмент JOHNSON &amp; JOHNSON; Дата отсечки 23/02/2021</t>
@@ -1109,10 +1115,10 @@
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M47" activeCellId="0" sqref="M47"/>
+      <selection pane="topLeft" activeCell="M45" activeCellId="0" sqref="M45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.94"/>
@@ -2307,26 +2313,26 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="41" t="n">
-        <v>44264</v>
+        <v>44543</v>
       </c>
       <c r="C45" s="42"/>
       <c r="D45" s="43" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E45" s="44" t="n">
-        <v>9.22</v>
+        <v>0.24</v>
       </c>
       <c r="F45" s="44"/>
       <c r="G45" s="45"/>
       <c r="H45" s="45"/>
       <c r="I45" s="46" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="J45" s="46"/>
       <c r="K45" s="46"/>
       <c r="L45" s="46"/>
       <c r="M45" s="47" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="N45" s="47"/>
       <c r="O45" s="47"/>
@@ -2382,7 +2388,7 @@
       <c r="K47" s="46"/>
       <c r="L47" s="46"/>
       <c r="M47" s="47" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="N47" s="47"/>
       <c r="O47" s="47"/>
@@ -2410,7 +2416,7 @@
       <c r="K48" s="46"/>
       <c r="L48" s="46"/>
       <c r="M48" s="47" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="N48" s="47"/>
       <c r="O48" s="47"/>
@@ -2503,7 +2509,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="48" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C52" s="49"/>
       <c r="D52" s="50" t="s">
@@ -2527,7 +2533,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="55" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C53" s="56"/>
       <c r="D53" s="57" t="s">
@@ -2574,7 +2580,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -2605,20 +2611,20 @@
         <v>15</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="L56" s="12"/>
       <c r="M56" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2630,7 +2636,7 @@
       </c>
       <c r="D57" s="70"/>
       <c r="E57" s="18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F57" s="71" t="s">
         <v>43</v>
@@ -2654,7 +2660,7 @@
       </c>
       <c r="D58" s="70"/>
       <c r="E58" s="18" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F58" s="71"/>
       <c r="G58" s="71"/>
@@ -2678,7 +2684,7 @@
       </c>
       <c r="D59" s="70"/>
       <c r="E59" s="18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F59" s="71" t="s">
         <v>43</v>
@@ -2702,7 +2708,7 @@
       </c>
       <c r="D60" s="70"/>
       <c r="E60" s="18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F60" s="71"/>
       <c r="G60" s="71"/>
@@ -2726,7 +2732,7 @@
       </c>
       <c r="D61" s="70"/>
       <c r="E61" s="18" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F61" s="71" t="s">
         <v>43</v>
@@ -2750,7 +2756,7 @@
       </c>
       <c r="D62" s="70"/>
       <c r="E62" s="18" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F62" s="71"/>
       <c r="G62" s="71"/>
@@ -2774,7 +2780,7 @@
       </c>
       <c r="D63" s="70"/>
       <c r="E63" s="18" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F63" s="71"/>
       <c r="G63" s="71"/>
@@ -2798,7 +2804,7 @@
       </c>
       <c r="D64" s="70"/>
       <c r="E64" s="18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F64" s="71"/>
       <c r="G64" s="71"/>
@@ -2866,7 +2872,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -2921,7 +2927,7 @@
         <v>11</v>
       </c>
       <c r="F70" s="47" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G70" s="47"/>
       <c r="H70" s="47"/>
@@ -2945,7 +2951,7 @@
         <v>11</v>
       </c>
       <c r="F71" s="47" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G71" s="47"/>
       <c r="H71" s="47"/>
@@ -2969,7 +2975,7 @@
         <v>11</v>
       </c>
       <c r="F72" s="47" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G72" s="47"/>
       <c r="H72" s="47"/>
@@ -2983,7 +2989,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="76" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C73" s="31" t="n">
         <v>69.62</v>
@@ -3007,7 +3013,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -3028,7 +3034,7 @@
     </row>
     <row r="76" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
@@ -3048,37 +3054,37 @@
         <v>32</v>
       </c>
       <c r="L76" s="12" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="M76" s="12"/>
       <c r="N76" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="O76" s="12"/>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="83" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C77" s="83"/>
       <c r="D77" s="83"/>
       <c r="E77" s="83"/>
       <c r="F77" s="83"/>
       <c r="G77" s="18" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="84" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J77" s="15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="K77" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L77" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M77" s="15"/>
       <c r="N77" s="85" t="n">
@@ -3088,25 +3094,25 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="83" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C78" s="83"/>
       <c r="D78" s="83"/>
       <c r="E78" s="83"/>
       <c r="F78" s="83"/>
       <c r="G78" s="18" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H78" s="18"/>
       <c r="I78" s="84"/>
       <c r="J78" s="15" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="K78" s="15" t="s">
         <v>39</v>
       </c>
       <c r="L78" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M78" s="15"/>
       <c r="N78" s="85" t="n">
@@ -3134,7 +3140,7 @@
         <v>39</v>
       </c>
       <c r="L79" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M79" s="15"/>
       <c r="N79" s="85" t="n">
@@ -3164,7 +3170,7 @@
         <v>11</v>
       </c>
       <c r="L80" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M80" s="15"/>
       <c r="N80" s="85" t="n">
@@ -3184,13 +3190,13 @@
       <c r="H81" s="18"/>
       <c r="I81" s="84"/>
       <c r="J81" s="15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K81" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L81" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M81" s="15"/>
       <c r="N81" s="85" t="n">
@@ -3200,27 +3206,27 @@
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="83" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C82" s="83"/>
       <c r="D82" s="83"/>
       <c r="E82" s="83"/>
       <c r="F82" s="83"/>
       <c r="G82" s="18" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H82" s="18"/>
       <c r="I82" s="84" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J82" s="15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K82" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L82" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="M82" s="15"/>
       <c r="N82" s="85" t="n">
@@ -3759,7 +3765,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3782,7 +3788,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Just2Trade statement: Import of in/out money transfers
</commit_message>
<xml_diff>
--- a/tests/test_data/j2t.xlsx
+++ b/tests/test_data/j2t.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="130">
   <si>
     <t xml:space="preserve">Отчет по счету клиента за период с 03.03.2021 по 10.03.2021</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t xml:space="preserve">Дивиденды; Начисление дивидендов полученных по счету "JT222222"". Инструмент JOHNSON &amp; JOHNSON; Дата отсечки 23/02/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Перевод на ТП</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Списание c ТП</t>
   </si>
   <si>
     <t xml:space="preserve">Итого:</t>
@@ -1114,8 +1120,8 @@
   </sheetPr>
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M45" activeCellId="0" sqref="M45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G46" activeCellId="0" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2453,27 +2459,25 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="41" t="n">
-        <v>44265</v>
+        <v>44154</v>
       </c>
       <c r="C50" s="42"/>
       <c r="D50" s="43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E50" s="44" t="n">
-        <v>3.5</v>
+        <v>100</v>
       </c>
       <c r="F50" s="44"/>
       <c r="G50" s="45"/>
       <c r="H50" s="45"/>
       <c r="I50" s="46" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="J50" s="46"/>
       <c r="K50" s="46"/>
       <c r="L50" s="46"/>
-      <c r="M50" s="47" t="s">
-        <v>85</v>
-      </c>
+      <c r="M50" s="47"/>
       <c r="N50" s="47"/>
       <c r="O50" s="47"/>
       <c r="P50" s="47"/>
@@ -2481,20 +2485,20 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="41" t="n">
-        <v>44265</v>
+        <v>44349</v>
       </c>
       <c r="C51" s="42"/>
       <c r="D51" s="43" t="s">
         <v>86</v>
       </c>
       <c r="E51" s="44" t="n">
-        <v>1.35</v>
+        <v>200</v>
       </c>
       <c r="F51" s="44"/>
       <c r="G51" s="45"/>
       <c r="H51" s="45"/>
       <c r="I51" s="46" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="J51" s="46"/>
       <c r="K51" s="46"/>
@@ -2509,7 +2513,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="48" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C52" s="49"/>
       <c r="D52" s="50" t="s">
@@ -2533,7 +2537,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="55" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C53" s="56"/>
       <c r="D53" s="57" t="s">
@@ -2580,7 +2584,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -2611,20 +2615,20 @@
         <v>15</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J56" s="12"/>
       <c r="K56" s="12" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="L56" s="12"/>
       <c r="M56" s="12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2636,7 +2640,7 @@
       </c>
       <c r="D57" s="70"/>
       <c r="E57" s="18" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F57" s="71" t="s">
         <v>43</v>
@@ -2660,7 +2664,7 @@
       </c>
       <c r="D58" s="70"/>
       <c r="E58" s="18" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F58" s="71"/>
       <c r="G58" s="71"/>
@@ -2684,7 +2688,7 @@
       </c>
       <c r="D59" s="70"/>
       <c r="E59" s="18" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F59" s="71" t="s">
         <v>43</v>
@@ -2708,7 +2712,7 @@
       </c>
       <c r="D60" s="70"/>
       <c r="E60" s="18" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F60" s="71"/>
       <c r="G60" s="71"/>
@@ -2732,7 +2736,7 @@
       </c>
       <c r="D61" s="70"/>
       <c r="E61" s="18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F61" s="71" t="s">
         <v>43</v>
@@ -2756,7 +2760,7 @@
       </c>
       <c r="D62" s="70"/>
       <c r="E62" s="18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F62" s="71"/>
       <c r="G62" s="71"/>
@@ -2780,7 +2784,7 @@
       </c>
       <c r="D63" s="70"/>
       <c r="E63" s="18" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F63" s="71"/>
       <c r="G63" s="71"/>
@@ -2804,7 +2808,7 @@
       </c>
       <c r="D64" s="70"/>
       <c r="E64" s="18" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="F64" s="71"/>
       <c r="G64" s="71"/>
@@ -2872,7 +2876,7 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -2927,7 +2931,7 @@
         <v>11</v>
       </c>
       <c r="F70" s="47" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G70" s="47"/>
       <c r="H70" s="47"/>
@@ -2951,7 +2955,7 @@
         <v>11</v>
       </c>
       <c r="F71" s="47" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G71" s="47"/>
       <c r="H71" s="47"/>
@@ -2975,7 +2979,7 @@
         <v>11</v>
       </c>
       <c r="F72" s="47" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G72" s="47"/>
       <c r="H72" s="47"/>
@@ -2989,7 +2993,7 @@
     </row>
     <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="76" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C73" s="31" t="n">
         <v>69.62</v>
@@ -3013,7 +3017,7 @@
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -3034,7 +3038,7 @@
     </row>
     <row r="76" customFormat="false" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
@@ -3054,37 +3058,37 @@
         <v>32</v>
       </c>
       <c r="L76" s="12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="M76" s="12"/>
       <c r="N76" s="12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="O76" s="12"/>
     </row>
     <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="83" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C77" s="83"/>
       <c r="D77" s="83"/>
       <c r="E77" s="83"/>
       <c r="F77" s="83"/>
       <c r="G77" s="18" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H77" s="18"/>
       <c r="I77" s="84" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J77" s="15" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K77" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L77" s="15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="M77" s="15"/>
       <c r="N77" s="85" t="n">
@@ -3094,25 +3098,25 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="83" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C78" s="83"/>
       <c r="D78" s="83"/>
       <c r="E78" s="83"/>
       <c r="F78" s="83"/>
       <c r="G78" s="18" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H78" s="18"/>
       <c r="I78" s="84"/>
       <c r="J78" s="15" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K78" s="15" t="s">
         <v>39</v>
       </c>
       <c r="L78" s="15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="M78" s="15"/>
       <c r="N78" s="85" t="n">
@@ -3140,7 +3144,7 @@
         <v>39</v>
       </c>
       <c r="L79" s="15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="M79" s="15"/>
       <c r="N79" s="85" t="n">
@@ -3170,7 +3174,7 @@
         <v>11</v>
       </c>
       <c r="L80" s="15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="M80" s="15"/>
       <c r="N80" s="85" t="n">
@@ -3190,13 +3194,13 @@
       <c r="H81" s="18"/>
       <c r="I81" s="84"/>
       <c r="J81" s="15" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K81" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L81" s="15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="M81" s="15"/>
       <c r="N81" s="85" t="n">
@@ -3206,27 +3210,27 @@
     </row>
     <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="83" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C82" s="83"/>
       <c r="D82" s="83"/>
       <c r="E82" s="83"/>
       <c r="F82" s="83"/>
       <c r="G82" s="18" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H82" s="18"/>
       <c r="I82" s="84" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J82" s="15" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K82" s="15" t="s">
         <v>11</v>
       </c>
       <c r="L82" s="15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="M82" s="15"/>
       <c r="N82" s="85" t="n">

</xml_diff>